<commit_message>
Added elements from today's mi_warrant slack discussion.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26960" yWindow="6880" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="40660" yWindow="420" windowWidth="33280" windowHeight="16980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="253">
   <si>
     <t>CLASS</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Additional information about a person</t>
   </si>
   <si>
-    <t>A miscellaneous unique identification assigned to a person record.</t>
-  </si>
-  <si>
     <t>Additional information about a vehicle.</t>
   </si>
   <si>
@@ -353,9 +350,6 @@
     <t>Gang member</t>
   </si>
   <si>
-    <t>MR456782</t>
-  </si>
-  <si>
     <t>R69458998</t>
   </si>
   <si>
@@ -512,9 +506,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonSSNIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonMiscellaneousRecordIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonAdditionalInformationText</t>
   </si>
   <si>
@@ -756,6 +747,39 @@
   </si>
   <si>
     <t>war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderRequestEntity/nc:EntityPerson/wir-ext:PersonEmployeeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Miscellanous ID of a person, Examples: A selective service number: SS-12345678 or Port Security Number PS-123456</t>
+  </si>
+  <si>
+    <t>PS-123456</t>
+  </si>
+  <si>
+    <t>Person Entry Number</t>
+  </si>
+  <si>
+    <t>A miscellaneous unique identification assigned to a person record</t>
+  </si>
+  <si>
+    <t>PE45678</t>
+  </si>
+  <si>
+    <t>US Citizen Indicator</t>
+  </si>
+  <si>
+    <t>True if a person query should include the DHS ICE Database; false otherwise</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/wir-ext:PersonEntryNumber/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonUSCitizenIndicator</t>
+  </si>
+  <si>
+    <t>PersonImmigationAlienQueryIndicator</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonImmigrationAlienQueryIndicator</t>
   </si>
 </sst>
 </file>
@@ -884,7 +908,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="906">
+  <cellStyleXfs count="914">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1791,8 +1815,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1860,11 +1892,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="906">
+  <cellStyles count="914">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2317,6 +2352,10 @@
     <cellStyle name="Followed Hyperlink" xfId="901" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="903" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="905" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="907" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="909" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="911" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="913" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2769,6 +2808,10 @@
     <cellStyle name="Hyperlink" xfId="900" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="902" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="904" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="906" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="908" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="910" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="912" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3104,11 +3147,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F294"/>
+  <dimension ref="A1:G296"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C70" sqref="C70:F70"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3124,17 +3167,17 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="10"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="24"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -3154,7 +3197,7 @@
     </row>
     <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -3166,10 +3209,10 @@
         <v>41</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="19" customFormat="1">
@@ -3180,10 +3223,10 @@
         <v>44</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="19" customFormat="1">
@@ -3194,13 +3237,13 @@
         <v>47</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="19" customFormat="1">
@@ -3211,13 +3254,13 @@
         <v>50</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="19" customFormat="1">
@@ -3228,13 +3271,13 @@
         <v>49</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="19" customFormat="1">
@@ -3255,10 +3298,10 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="19" customFormat="1">
@@ -3268,10 +3311,10 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="19" customFormat="1">
@@ -3281,10 +3324,10 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="19" customFormat="1">
@@ -3294,10 +3337,10 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="19" customFormat="1">
@@ -3307,10 +3350,10 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3322,10 +3365,10 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3335,854 +3378,882 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" s="19" customFormat="1" ht="45">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B17" s="6"/>
       <c r="C17" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" s="19" customFormat="1" ht="45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" s="19" customFormat="1" ht="45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" s="19" customFormat="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="19" customFormat="1">
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" s="19" customFormat="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18">
-        <v>23235</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" s="19" customFormat="1">
+        <v>247</v>
+      </c>
+      <c r="E21" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" s="20" customFormat="1" ht="25" customHeight="1">
+      <c r="A22" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" s="19" customFormat="1">
+        <v>251</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="E22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" s="19" customFormat="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>103</v>
+        <v>4</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18">
+        <v>23235</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" s="19" customFormat="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="19" customFormat="1">
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>138</v>
+        <v>206</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" s="19" customFormat="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="19" customFormat="1">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" s="19" customFormat="1">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="19" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7">
-        <v>354786908</v>
+        <v>136</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" s="19" customFormat="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="D27" s="7"/>
+        <v>209</v>
+      </c>
       <c r="E27" s="7" t="s">
-        <v>214</v>
+        <v>103</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" s="19" customFormat="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>105</v>
+        <v>16</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7">
+        <v>354786908</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" s="19" customFormat="1">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>140</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="D29" s="7"/>
       <c r="E29" s="7" t="s">
-        <v>99</v>
+        <v>211</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" s="19" customFormat="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" s="19" customFormat="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="19" customFormat="1">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="7"/>
+        <v>138</v>
+      </c>
       <c r="E31" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" s="19" customFormat="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7">
-        <v>165</v>
+        <v>71</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="19" customFormat="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="19" customFormat="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>102</v>
+        <v>23</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7">
+        <v>165</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="19" customFormat="1">
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
-        <v>142</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D35" s="7"/>
       <c r="E35" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="19" customFormat="1">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7">
-        <v>98213455</v>
+        <v>139</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="19" customFormat="1" ht="30">
-      <c r="A37" s="19" t="s">
-        <v>37</v>
-      </c>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="19" customFormat="1">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="19" customFormat="1">
-      <c r="A38" s="19" t="s">
-        <v>37</v>
-      </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7">
+        <v>98213455</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="A39" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="F39" s="23"/>
+    </row>
+    <row r="40" spans="1:6" s="19" customFormat="1">
+      <c r="A40" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D40" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F38" s="7" t="s">
+      <c r="E40" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="19" customFormat="1">
+      <c r="A41" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="B42" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="19" customFormat="1">
-      <c r="A39" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="B40" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="B41" s="6"/>
-      <c r="C41" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="19" customFormat="1">
-      <c r="B42" s="14" t="s">
+    <row r="44" spans="1:6" s="19" customFormat="1">
+      <c r="B44" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-    </row>
-    <row r="43" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C43" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C44" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>169</v>
-      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
     </row>
     <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C45" s="7" t="s">
-        <v>133</v>
+        <v>27</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C46" s="7" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>217</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C47" s="7" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>144</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C48" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>204</v>
+        <v>132</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C49" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>204</v>
+        <v>28</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>219</v>
+        <v>114</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>220</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C50" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E50" s="19" t="s">
         <v>115</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C51" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C52" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C53" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="19">
+      <c r="E53" s="19">
         <v>2012</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="F53" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A54" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A52" s="19" t="s">
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="B55" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+    </row>
+    <row r="56" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="A56" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="19" customFormat="1" ht="30">
-      <c r="B53" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-    </row>
-    <row r="54" spans="1:6" s="9" customFormat="1" ht="45">
-      <c r="A54" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="9" customFormat="1" ht="45">
-      <c r="B55" s="16"/>
-      <c r="C55" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7">
-        <v>6407</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="9" customFormat="1">
       <c r="B56" s="16"/>
       <c r="C56" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F56" s="7"/>
-    </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="45">
+        <v>121</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="B57" s="16"/>
       <c r="C57" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>121</v>
+        <v>34</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7">
+        <v>6407</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="45">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="9" customFormat="1">
+      <c r="B58" s="16"/>
       <c r="C58" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>183</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C59" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C60" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C61" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E59" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C60" s="19" t="s">
+      <c r="E61" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C62" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="19">
+      <c r="E62" s="19">
         <v>63412</v>
       </c>
-      <c r="F60" s="19" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="19" customFormat="1">
-      <c r="B61" s="14" t="s">
+      <c r="F62" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="19" customFormat="1">
+      <c r="B63" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
-    </row>
-    <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C62" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D62" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E62" s="13">
-        <v>41133</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
-      <c r="C63" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E63" s="19">
-        <v>5000</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>188</v>
-      </c>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
     </row>
     <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C64" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="E64" s="13">
-        <v>40767</v>
+        <v>41133</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="19" customFormat="1" ht="45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
       <c r="C65" s="7" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="E65" s="19">
-        <v>659056746</v>
+        <v>5000</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C66" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E66" s="13">
+        <v>40767</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C67" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E67" s="19">
+        <v>659056746</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C68" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E66" s="19" t="s">
+      <c r="E68" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A69" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E69" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="19" customFormat="1" ht="60">
+      <c r="A70" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E70" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="F66" s="6" t="s">
+      <c r="F70" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C71" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E71" s="19">
+        <v>758075800</v>
+      </c>
+      <c r="F71" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A67" s="19" t="s">
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A72" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C67" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E67" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="6" t="s">
+      <c r="B72" s="20"/>
+      <c r="C72" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C73" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F73" s="19" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="19" customFormat="1" ht="60">
-      <c r="A68" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E68" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C69" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E69" s="19">
-        <v>758075800</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A70" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B70" s="20"/>
-      <c r="C70" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C71" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D71" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E71" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="F71" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A72" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B72" s="21"/>
-      <c r="C72" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="F72" s="19" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A73" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="F73" s="19" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="A74" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B74" s="9"/>
+      <c r="B74" s="21"/>
       <c r="C74" s="9" t="s">
-        <v>72</v>
+        <v>196</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E74" s="9">
-        <v>500</v>
+        <v>48</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="A75" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C75" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D75" s="19" t="s">
+      <c r="B75" s="9"/>
+      <c r="C75" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A76" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E76" s="9">
+        <v>500</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A77" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E75" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F75" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C76" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="E76" s="19" t="s">
+      <c r="E77" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C78" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="F78" s="20" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="A79" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" s="21"/>
+      <c r="C79" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D79" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="F76" s="20" t="s">
+      <c r="E79" s="9" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" s="22" customFormat="1" ht="45">
-      <c r="A77" s="20" t="s">
+      <c r="F79" s="20" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="22" customFormat="1" ht="75">
+      <c r="A80" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B77" s="21"/>
-      <c r="C77" s="9" t="s">
+      <c r="C80" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="D80" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E80" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="F77" s="20" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="22" customFormat="1" ht="75">
-      <c r="A78" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C78" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="D78" s="20" t="s">
+      <c r="F80" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="E78" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="F78" s="20" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="19" customFormat="1">
-      <c r="B79" s="22"/>
-    </row>
-    <row r="80" spans="1:6" s="19" customFormat="1"/>
-    <row r="81" s="19" customFormat="1"/>
-    <row r="281" hidden="1"/>
-    <row r="282" hidden="1"/>
+    </row>
+    <row r="81" spans="2:2" s="19" customFormat="1">
+      <c r="B81" s="22"/>
+    </row>
+    <row r="82" spans="2:2" s="19" customFormat="1"/>
+    <row r="83" spans="2:2" s="19" customFormat="1"/>
     <row r="283" hidden="1"/>
     <row r="284" hidden="1"/>
     <row r="285" hidden="1"/>
@@ -4195,6 +4266,8 @@
     <row r="292" hidden="1"/>
     <row r="293" hidden="1"/>
     <row r="294" hidden="1"/>
+    <row r="295" hidden="1"/>
+    <row r="296" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4212,10 +4285,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4232,10 +4305,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="24"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -4243,7 +4316,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -4284,10 +4357,10 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4297,10 +4370,10 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4310,10 +4383,10 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4323,10 +4396,10 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4339,102 +4412,118 @@
         <v>23235</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F10" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" s="20" customFormat="1" ht="53" customHeight="1">
+      <c r="A11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="19"/>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="45">
+      <c r="C13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="19">
+        <v>758075800</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
+      <c r="C14" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
+      <c r="A15" s="19"/>
+      <c r="C15" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="19"/>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" s="19" customFormat="1" ht="45">
-      <c r="C12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="19">
-        <v>758075800</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="22" customFormat="1" ht="30">
-      <c r="C13" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="30">
-      <c r="A14" s="19"/>
-      <c r="C14" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="19" customFormat="1"/>
+    </row>
     <row r="16" spans="1:7" s="19" customFormat="1"/>
     <row r="17" spans="1:1" s="19" customFormat="1"/>
     <row r="18" spans="1:1" s="19" customFormat="1"/>
     <row r="19" spans="1:1" s="19" customFormat="1"/>
     <row r="20" spans="1:1" s="19" customFormat="1"/>
     <row r="21" spans="1:1" s="19" customFormat="1"/>
-    <row r="22" spans="1:1">
-      <c r="A22" s="19"/>
-    </row>
+    <row r="22" spans="1:1" s="19" customFormat="1"/>
     <row r="23" spans="1:1">
       <c r="A23" s="19"/>
     </row>
@@ -4472,9 +4561,7 @@
       <c r="A34" s="19"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="A35" s="19"/>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="19" t="s">
@@ -4492,7 +4579,9 @@
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="19"/>
+      <c r="A39" s="19" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="19"/>
@@ -4528,9 +4617,7 @@
       <c r="A50" s="19"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="A51" s="19"/>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="19" t="s">
@@ -4543,21 +4630,23 @@
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="19"/>
+      <c r="A54" s="19" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="19"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="9"/>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="9"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="19"/>
+      <c r="A58" s="9"/>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="19"/>
@@ -4593,9 +4682,7 @@
       <c r="A69" s="19"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="A70" s="19"/>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="19" t="s">
@@ -4603,7 +4690,9 @@
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="19"/>
+      <c r="A72" s="19" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="19"/>
@@ -4612,9 +4701,7 @@
       <c r="A74" s="19"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="A75" s="19"/>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="19" t="s">
@@ -4632,7 +4719,9 @@
       </c>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="19"/>
+      <c r="A79" s="19" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="19"/>
@@ -4651,6 +4740,9 @@
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="19"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated PersonMiscellaneousRecordIdentificatin name in mapping spreadsheet.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40660" yWindow="420" windowWidth="33280" windowHeight="16980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="40660" yWindow="420" windowWidth="33280" windowHeight="16980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="254">
   <si>
     <t>CLASS</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Charge Code Text</t>
   </si>
   <si>
-    <t>Miscellaneous Person Record Number</t>
-  </si>
-  <si>
     <t>CONTACT LOCATION (Subject)</t>
   </si>
   <si>
@@ -780,6 +777,12 @@
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonImmigrationAlienQueryIndicator</t>
+  </si>
+  <si>
+    <t>Person Miscellaneous Record ID</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonMiscellaneousRecordIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1827,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1890,9 +1893,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3149,9 +3149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G296"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3167,17 +3167,17 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="10"/>
-      <c r="B1" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="24"/>
+      <c r="B1" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="23"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -3197,7 +3197,7 @@
     </row>
     <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -3209,10 +3209,10 @@
         <v>41</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="19" customFormat="1">
@@ -3223,10 +3223,10 @@
         <v>44</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="19" customFormat="1">
@@ -3237,13 +3237,13 @@
         <v>47</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="19" customFormat="1">
@@ -3254,13 +3254,13 @@
         <v>50</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="19" customFormat="1">
@@ -3271,13 +3271,13 @@
         <v>49</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="19" customFormat="1">
@@ -3298,10 +3298,10 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="19" customFormat="1">
@@ -3311,10 +3311,10 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="19" customFormat="1">
@@ -3324,10 +3324,10 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="19" customFormat="1">
@@ -3337,10 +3337,10 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="19" customFormat="1">
@@ -3350,10 +3350,10 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3365,10 +3365,10 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3378,10 +3378,10 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="19" customFormat="1" ht="45">
@@ -3391,10 +3391,10 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="19" customFormat="1" ht="45">
@@ -3404,10 +3404,10 @@
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="19" customFormat="1" ht="45">
@@ -3417,10 +3417,10 @@
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="19" customFormat="1">
@@ -3428,28 +3428,28 @@
         <v>5</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E21" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G21" s="9"/>
     </row>
@@ -3459,16 +3459,16 @@
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E22" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G22" s="9"/>
     </row>
@@ -3482,55 +3482,55 @@
         <v>23235</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="19" customFormat="1">
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="19" customFormat="1">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="19" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="19" customFormat="1">
@@ -3543,44 +3543,44 @@
         <v>354786908</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="19" customFormat="1">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="19" customFormat="1">
@@ -3593,7 +3593,7 @@
         <v>71</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="19" customFormat="1">
@@ -3603,10 +3603,10 @@
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="19" customFormat="1">
@@ -3619,7 +3619,7 @@
         <v>165</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="19" customFormat="1">
@@ -3629,34 +3629,34 @@
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="19" customFormat="1">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="19" customFormat="1">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="19" customFormat="1">
@@ -3669,24 +3669,26 @@
         <v>98213455</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="22" customFormat="1" ht="45">
-      <c r="A39" s="22" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="20" customFormat="1" ht="45">
+      <c r="A39" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="23" t="s">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="E39" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="F39" s="23"/>
+      <c r="F39" s="7" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="40" spans="1:6" s="19" customFormat="1">
       <c r="A40" s="19" t="s">
@@ -3694,16 +3696,16 @@
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="19" customFormat="1">
@@ -3712,16 +3714,16 @@
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3733,10 +3735,10 @@
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3748,10 +3750,10 @@
         <v>20</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="19" customFormat="1">
@@ -3768,43 +3770,43 @@
         <v>27</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C46" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C47" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C48" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3812,52 +3814,52 @@
         <v>28</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C50" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C51" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E51" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C52" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3868,7 +3870,7 @@
         <v>2012</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3877,21 +3879,21 @@
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="19" customFormat="1" ht="30">
       <c r="B55" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
@@ -3908,10 +3910,10 @@
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="9" customFormat="1" ht="45">
@@ -3924,7 +3926,7 @@
         <v>6407</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="9" customFormat="1">
@@ -3934,7 +3936,7 @@
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F58" s="7"/>
     </row>
@@ -3943,10 +3945,10 @@
         <v>30</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3954,10 +3956,10 @@
         <v>32</v>
       </c>
       <c r="E60" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3965,10 +3967,10 @@
         <v>31</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3979,7 +3981,7 @@
         <v>63412</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="19" customFormat="1">
@@ -4002,18 +4004,18 @@
         <v>41133</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
       <c r="C65" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E65" s="19">
         <v>5000</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4024,7 +4026,7 @@
         <v>40767</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4035,18 +4037,18 @@
         <v>659056746</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C68" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E68" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4054,16 +4056,16 @@
         <v>37</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E69" s="19" t="b">
         <v>1</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="19" customFormat="1" ht="60">
@@ -4071,16 +4073,16 @@
         <v>37</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D70" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4088,13 +4090,13 @@
         <v>46</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E71" s="19">
         <v>758075800</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4103,30 +4105,30 @@
       </c>
       <c r="B72" s="20"/>
       <c r="C72" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D72" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E72" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="E72" s="19" t="s">
+      <c r="F72" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C73" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D73" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4135,16 +4137,16 @@
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4153,16 +4155,16 @@
       </c>
       <c r="B75" s="9"/>
       <c r="C75" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4171,16 +4173,16 @@
       </c>
       <c r="B76" s="9"/>
       <c r="C76" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E76" s="9">
         <v>500</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4188,30 +4190,30 @@
         <v>37</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D77" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C78" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="D78" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="D78" s="20" t="s">
-        <v>200</v>
-      </c>
       <c r="E78" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="F78" s="20" t="s">
         <v>223</v>
-      </c>
-      <c r="F78" s="20" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="22" customFormat="1" ht="45">
@@ -4220,16 +4222,16 @@
       </c>
       <c r="B79" s="21"/>
       <c r="C79" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D79" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="E79" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="E79" s="9" t="s">
-        <v>227</v>
-      </c>
       <c r="F79" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="22" customFormat="1" ht="75">
@@ -4237,16 +4239,16 @@
         <v>37</v>
       </c>
       <c r="C80" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="D80" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="D80" s="20" t="s">
+      <c r="E80" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="E80" s="20" t="s">
-        <v>230</v>
-      </c>
       <c r="F80" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="81" spans="2:2" s="19" customFormat="1">
@@ -4287,7 +4289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
@@ -4305,10 +4307,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
-      <c r="B1" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="24"/>
+      <c r="B1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="23"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -4316,7 +4318,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -4357,10 +4359,10 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4370,10 +4372,10 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4383,10 +4385,10 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4396,10 +4398,10 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4412,35 +4414,35 @@
         <v>23235</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G10" s="9"/>
     </row>
@@ -4450,16 +4452,16 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="E11" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>246</v>
-      </c>
       <c r="F11" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G11" s="9"/>
     </row>
@@ -4479,42 +4481,42 @@
         <v>46</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="19">
         <v>758075800</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
       <c r="C14" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D14" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="E14" s="20" t="s">
-        <v>221</v>
-      </c>
       <c r="F14" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="19" customFormat="1"/>

</xml_diff>

<commit_message>
Added new elements to IEPDs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40660" yWindow="420" windowWidth="33280" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="39760" yWindow="1640" windowWidth="33280" windowHeight="16860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="258">
   <si>
     <t>CLASS</t>
   </si>
@@ -164,12 +164,6 @@
     <t>Law Enforcement ORI</t>
   </si>
   <si>
-    <t>Offense Code Text</t>
-  </si>
-  <si>
-    <t>A code assigned to a warrant record by prosecution</t>
-  </si>
-  <si>
     <t>Original Offense Code Text</t>
   </si>
   <si>
@@ -542,9 +536,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Case/nc:ActivityIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Case/j:CaseAugmentation/j:CaseCharge/wir-ext:OffenseCodeText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Case/j:CaseAugmentation/j:CaseCharge/wir-ext:ChargeCodeText</t>
   </si>
   <si>
@@ -677,9 +668,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/j:VehicleStyleCode</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:CriminalTrackingNumber</t>
-  </si>
-  <si>
     <t>OCA</t>
   </si>
   <si>
@@ -783,6 +771,30 @@
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonMiscellaneousRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>GeneralOffense Code Text</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Case/j:CaseAugmentation/j:CaseCharge/wir-ext:GeneralOffenseCodeText</t>
+  </si>
+  <si>
+    <t>Prosecution Charge  Code Text</t>
+  </si>
+  <si>
+    <t>A charge code assigned by the prosecutuion</t>
+  </si>
+  <si>
+    <t>PCC45678</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Case/j:CaseAugmentation/j:CaseCharge/wir-ext:ProsecutionChargeCodeText</t>
+  </si>
+  <si>
+    <t>A case number assigned by the prosecution</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Case/wir-ext:CriminalTrackingNumber</t>
   </si>
 </sst>
 </file>
@@ -911,9 +923,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="914">
+  <cellStyleXfs count="916">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1899,7 +1913,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="914">
+  <cellStyles count="916">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2356,6 +2370,7 @@
     <cellStyle name="Followed Hyperlink" xfId="909" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="911" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="913" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="915" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2812,6 +2827,7 @@
     <cellStyle name="Hyperlink" xfId="908" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="910" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="912" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="914" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3147,11 +3163,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G296"/>
+  <dimension ref="A1:G297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3168,7 +3184,7 @@
     <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="10"/>
@@ -3177,7 +3193,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -3197,7 +3213,7 @@
     </row>
     <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -3209,10 +3225,10 @@
         <v>41</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="19" customFormat="1">
@@ -3223,10 +3239,10 @@
         <v>44</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="19" customFormat="1">
@@ -3234,16 +3250,16 @@
         <v>37</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>47</v>
+        <v>250</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>173</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="19" customFormat="1">
@@ -3251,16 +3267,16 @@
         <v>37</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="19" customFormat="1">
@@ -3268,903 +3284,899 @@
         <v>37</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="19" customFormat="1">
-      <c r="B9" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="20" customFormat="1">
+      <c r="C9" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="19" customFormat="1">
+      <c r="A10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="19" customFormat="1">
+      <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" spans="1:6" s="19" customFormat="1">
-      <c r="B10" s="6" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" s="19" customFormat="1">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C12" s="19" t="s">
         <v>9</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="19" customFormat="1">
-      <c r="B11" s="6"/>
-      <c r="C11" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="19" customFormat="1">
-      <c r="B12" s="6"/>
-      <c r="C12" s="19" t="s">
-        <v>11</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="19" customFormat="1">
       <c r="B13" s="6"/>
       <c r="C13" s="19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="19" customFormat="1">
       <c r="B14" s="6"/>
       <c r="C14" s="19" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="B15" s="6" t="s">
-        <v>14</v>
-      </c>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="19" customFormat="1">
+      <c r="B15" s="6"/>
       <c r="C15" s="19" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="19" customFormat="1" ht="45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="19" customFormat="1">
       <c r="B16" s="6"/>
       <c r="C16" s="19" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="19" customFormat="1" ht="45">
-      <c r="B17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="C17" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>168</v>
+        <v>88</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>169</v>
+        <v>89</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="19" customFormat="1">
-      <c r="B20" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="19" customFormat="1" ht="45">
+      <c r="B20" s="6"/>
+      <c r="C20" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="19" customFormat="1" ht="45">
+      <c r="B21" s="6"/>
+      <c r="C21" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="19" customFormat="1">
+      <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="20" customFormat="1" ht="25" customHeight="1">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="E21" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="1:7" s="20" customFormat="1" ht="25" customHeight="1">
-      <c r="A22" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>247</v>
-      </c>
-      <c r="E22" s="7" t="b">
-        <v>0</v>
+      <c r="C22" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:7" s="19" customFormat="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="18">
-        <v>23235</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="19" customFormat="1">
+        <v>242</v>
+      </c>
+      <c r="E23" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" s="20" customFormat="1" ht="25" customHeight="1">
+      <c r="A24" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>203</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="E24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" s="19" customFormat="1">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>101</v>
+        <v>4</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18">
+        <v>23235</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>207</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="19" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>135</v>
+        <v>202</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>149</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7">
-        <v>354786908</v>
+        <v>133</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D29" s="7"/>
+        <v>205</v>
+      </c>
       <c r="E29" s="7" t="s">
-        <v>210</v>
+        <v>100</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>103</v>
+        <v>16</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7">
+        <v>354786908</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="19" customFormat="1">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
-        <v>137</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="D31" s="7"/>
       <c r="E31" s="7" t="s">
-        <v>97</v>
+        <v>207</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>152</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7">
-        <v>71</v>
+        <v>134</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="19" customFormat="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="7"/>
+        <v>135</v>
+      </c>
       <c r="E33" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="19" customFormat="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7">
-        <v>165</v>
+        <v>71</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="19" customFormat="1">
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="19" customFormat="1">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>100</v>
+        <v>23</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7">
+        <v>165</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="19" customFormat="1">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
-        <v>139</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D37" s="7"/>
       <c r="E37" s="7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="19" customFormat="1">
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7">
-        <v>98213455</v>
+        <v>136</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="A39" s="20" t="s">
-        <v>37</v>
-      </c>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="19" customFormat="1">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>241</v>
+        <v>137</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>242</v>
+        <v>102</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>253</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="19" customFormat="1">
-      <c r="A40" s="19" t="s">
-        <v>37</v>
-      </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>107</v>
+        <v>6</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7">
+        <v>98213455</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="19" customFormat="1">
-      <c r="A41" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="20" customFormat="1" ht="45">
+      <c r="A41" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
-        <v>58</v>
+        <v>248</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>63</v>
+        <v>237</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>109</v>
+        <v>238</v>
       </c>
       <c r="F41" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="19" customFormat="1">
+      <c r="A42" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="19" customFormat="1">
+      <c r="A43" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="B44" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="B42" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="B43" s="6"/>
-      <c r="C43" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="19" customFormat="1">
-      <c r="B44" s="14" t="s">
+    <row r="46" spans="1:6" s="19" customFormat="1">
+      <c r="B46" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-    </row>
-    <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C45" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C46" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>165</v>
-      </c>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
     </row>
     <row r="47" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C47" s="7" t="s">
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C48" s="7" t="s">
-        <v>131</v>
+        <v>75</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>213</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C49" s="7" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>141</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C50" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C51" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>200</v>
+        <v>28</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>215</v>
+        <v>111</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>216</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C52" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E52" s="19" t="s">
         <v>112</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C53" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C54" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C55" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E53" s="19">
+      <c r="E55" s="19">
         <v>2012</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F55" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A56" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F56" s="6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A54" s="19" t="s">
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="B57" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+    </row>
+    <row r="58" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="A58" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="30">
-      <c r="B55" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-    </row>
-    <row r="56" spans="1:6" s="9" customFormat="1" ht="45">
-      <c r="A56" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="9" customFormat="1" ht="45">
-      <c r="B57" s="16"/>
-      <c r="C57" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7">
-        <v>6407</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="9" customFormat="1">
       <c r="B58" s="16"/>
       <c r="C58" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F58" s="7"/>
-    </row>
-    <row r="59" spans="1:6" s="19" customFormat="1" ht="45">
+        <v>118</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="B59" s="16"/>
       <c r="C59" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>118</v>
+        <v>34</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7">
+        <v>6407</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="19" customFormat="1" ht="45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="9" customFormat="1">
+      <c r="B60" s="16"/>
       <c r="C60" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>179</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C61" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C62" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C63" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E61" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C62" s="19" t="s">
+      <c r="E63" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C64" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E62" s="19">
+      <c r="E64" s="19">
         <v>63412</v>
       </c>
-      <c r="F62" s="19" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="19" customFormat="1">
-      <c r="B63" s="14" t="s">
+      <c r="F64" s="19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="19" customFormat="1">
+      <c r="B65" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-    </row>
-    <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C64" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E64" s="13">
-        <v>41133</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
-      <c r="C65" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E65" s="19">
-        <v>5000</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>184</v>
-      </c>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
     </row>
     <row r="66" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C66" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="E66" s="13">
-        <v>40767</v>
+        <v>41133</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="19" customFormat="1" ht="45">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
       <c r="C67" s="7" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E67" s="19">
-        <v>659056746</v>
+        <v>5000</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C68" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E68" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E68" s="13">
+        <v>40767</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C69" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" s="19">
+        <v>659056746</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C70" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A71" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E71" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="60">
+      <c r="A72" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E72" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F68" s="6" t="s">
+      <c r="F72" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C73" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E73" s="19">
+        <v>758075800</v>
+      </c>
+      <c r="F73" s="6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A69" s="19" t="s">
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A74" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E69" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="6" t="s">
+      <c r="B74" s="20"/>
+      <c r="C74" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C75" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F75" s="19" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="19" customFormat="1" ht="60">
-      <c r="A70" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D70" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C71" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D71" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E71" s="19">
-        <v>758075800</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A72" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B72" s="20"/>
-      <c r="C72" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D72" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="E72" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C73" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D73" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E73" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="F73" s="19" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A74" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B74" s="21"/>
-      <c r="C74" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="F74" s="19" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A75" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F75" s="19" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4173,90 +4185,107 @@
       </c>
       <c r="B76" s="9"/>
       <c r="C76" s="9" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E76" s="9">
-        <v>500</v>
+        <v>127</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="A77" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C77" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E77" s="19" t="s">
-        <v>127</v>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E77" s="9">
+        <v>500</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C78" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>199</v>
+      <c r="A78" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="F78" s="20" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="22" customFormat="1" ht="45">
-      <c r="A79" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B79" s="21"/>
-      <c r="C79" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>226</v>
+        <v>125</v>
+      </c>
+      <c r="F78" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C79" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>218</v>
       </c>
       <c r="F79" s="20" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" s="22" customFormat="1" ht="75">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="22" customFormat="1" ht="45">
       <c r="A80" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C80" s="20" t="s">
+      <c r="B80" s="21"/>
+      <c r="C80" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="22" customFormat="1" ht="75">
+      <c r="A81" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="E81" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="F81" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="D80" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="E80" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="F80" s="20" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" s="19" customFormat="1">
-      <c r="B81" s="22"/>
-    </row>
-    <row r="82" spans="2:2" s="19" customFormat="1"/>
-    <row r="83" spans="2:2" s="19" customFormat="1"/>
-    <row r="283" hidden="1"/>
+    </row>
+    <row r="82" spans="1:6" s="19" customFormat="1">
+      <c r="B82" s="22"/>
+    </row>
+    <row r="83" spans="1:6" s="19" customFormat="1"/>
+    <row r="84" spans="1:6" s="19" customFormat="1"/>
     <row r="284" hidden="1"/>
     <row r="285" hidden="1"/>
     <row r="286" hidden="1"/>
@@ -4270,6 +4299,7 @@
     <row r="294" hidden="1"/>
     <row r="295" hidden="1"/>
     <row r="296" hidden="1"/>
+    <row r="297" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4308,7 +4338,7 @@
     <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="10"/>
@@ -4318,7 +4348,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -4359,10 +4389,10 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4372,10 +4402,10 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4385,10 +4415,10 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4398,10 +4428,10 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4414,35 +4444,35 @@
         <v>23235</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G10" s="9"/>
     </row>
@@ -4452,16 +4482,16 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>244</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>248</v>
       </c>
       <c r="G11" s="9"/>
     </row>
@@ -4481,42 +4511,42 @@
         <v>46</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E13" s="19">
         <v>758075800</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
       <c r="C14" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="19" customFormat="1"/>

</xml_diff>

<commit_message>
Changed physical feature code to j:PhysicalFeatureCategoryCode.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -488,9 +488,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonWeightMeasure/nc:MeasureUnitText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonPhysicalFeature/intel:PhysicalFeatureCategoryCodeText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonBirthLocation/nc:LocationCategoryText</t>
   </si>
   <si>
@@ -795,6 +792,9 @@
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/nc:Case/wir-ext:CriminalTrackingNumber</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonPhysicalFeature/j:PhysicalFeatureCategoryCode</t>
   </si>
 </sst>
 </file>
@@ -3166,8 +3166,8 @@
   <dimension ref="A1:G297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3228,7 +3228,7 @@
         <v>78</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="19" customFormat="1">
@@ -3242,7 +3242,7 @@
         <v>79</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="19" customFormat="1">
@@ -3250,7 +3250,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>70</v>
@@ -3259,7 +3259,7 @@
         <v>80</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="19" customFormat="1">
@@ -3276,7 +3276,7 @@
         <v>81</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="19" customFormat="1">
@@ -3293,21 +3293,21 @@
         <v>82</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="20" customFormat="1">
       <c r="C9" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="E9" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="F9" s="20" t="s">
         <v>254</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="19" customFormat="1">
@@ -3316,16 +3316,16 @@
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>124</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="19" customFormat="1">
@@ -3416,7 +3416,7 @@
         <v>88</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="19" customFormat="1" ht="45">
@@ -3429,7 +3429,7 @@
         <v>89</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="19" customFormat="1" ht="45">
@@ -3442,7 +3442,7 @@
         <v>90</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="19" customFormat="1" ht="45">
@@ -3455,7 +3455,7 @@
         <v>86</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="19" customFormat="1" ht="45">
@@ -3468,7 +3468,7 @@
         <v>91</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="19" customFormat="1">
@@ -3476,28 +3476,28 @@
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>92</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E23" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G23" s="9"/>
     </row>
@@ -3507,16 +3507,16 @@
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E24" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G24" s="9"/>
     </row>
@@ -3536,25 +3536,25 @@
     <row r="26" spans="1:7" s="19" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>93</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="19" customFormat="1">
@@ -3572,13 +3572,13 @@
     <row r="29" spans="1:7" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>100</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="19" customFormat="1">
@@ -3597,14 +3597,14 @@
     <row r="31" spans="1:7" s="19" customFormat="1">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="19" customFormat="1">
@@ -3692,7 +3692,7 @@
         <v>98</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="19" customFormat="1">
@@ -3704,7 +3704,7 @@
         <v>102</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>155</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="19" customFormat="1">
@@ -3717,7 +3717,7 @@
         <v>98213455</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="20" customFormat="1" ht="45">
@@ -3726,16 +3726,16 @@
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F41" s="7" t="s">
         <v>248</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="19" customFormat="1">
@@ -3753,7 +3753,7 @@
         <v>105</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="19" customFormat="1">
@@ -3771,7 +3771,7 @@
         <v>107</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3786,7 +3786,7 @@
         <v>103</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3801,7 +3801,7 @@
         <v>104</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="19" customFormat="1">
@@ -3821,7 +3821,7 @@
         <v>114</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3832,7 +3832,7 @@
         <v>115</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3843,7 +3843,7 @@
         <v>108</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3854,7 +3854,7 @@
         <v>109</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3873,13 +3873,13 @@
         <v>130</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E52" s="19" t="s">
         <v>112</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3887,13 +3887,13 @@
         <v>131</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E53" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3901,13 +3901,13 @@
         <v>132</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E54" s="19" t="s">
         <v>110</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3961,7 +3961,7 @@
         <v>118</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="9" customFormat="1" ht="45">
@@ -3974,7 +3974,7 @@
         <v>6407</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="9" customFormat="1">
@@ -3996,7 +3996,7 @@
         <v>116</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4007,7 +4007,7 @@
         <v>119</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4018,7 +4018,7 @@
         <v>120</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4029,7 +4029,7 @@
         <v>63412</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="19" customFormat="1">
@@ -4052,7 +4052,7 @@
         <v>41133</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
@@ -4063,7 +4063,7 @@
         <v>5000</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4074,7 +4074,7 @@
         <v>40767</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4085,7 +4085,7 @@
         <v>659056746</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4096,7 +4096,7 @@
         <v>121</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4113,7 +4113,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="19" customFormat="1" ht="60">
@@ -4130,7 +4130,7 @@
         <v>123</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4144,7 +4144,7 @@
         <v>758075800</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4153,16 +4153,16 @@
       </c>
       <c r="B74" s="20"/>
       <c r="C74" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D74" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="E74" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="E74" s="19" t="s">
+      <c r="F74" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4176,7 +4176,7 @@
         <v>122</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4194,7 +4194,7 @@
         <v>106</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4212,7 +4212,7 @@
         <v>500</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4229,21 +4229,21 @@
         <v>125</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C79" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="D79" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="D79" s="20" t="s">
-        <v>196</v>
-      </c>
       <c r="E79" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="F79" s="20" t="s">
         <v>218</v>
-      </c>
-      <c r="F79" s="20" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="22" customFormat="1" ht="45">
@@ -4252,16 +4252,16 @@
       </c>
       <c r="B80" s="21"/>
       <c r="C80" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D80" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D80" s="9" t="s">
+      <c r="E80" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="E80" s="9" t="s">
-        <v>222</v>
-      </c>
       <c r="F80" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="22" customFormat="1" ht="75">
@@ -4269,16 +4269,16 @@
         <v>37</v>
       </c>
       <c r="C81" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="D81" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="D81" s="20" t="s">
+      <c r="E81" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="E81" s="20" t="s">
-        <v>225</v>
-      </c>
       <c r="F81" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="19" customFormat="1">
@@ -4392,7 +4392,7 @@
         <v>83</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4405,7 +4405,7 @@
         <v>84</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4418,7 +4418,7 @@
         <v>85</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4431,7 +4431,7 @@
         <v>86</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4444,35 +4444,35 @@
         <v>23235</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
         <v>100</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G10" s="9"/>
     </row>
@@ -4482,16 +4482,16 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="E11" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>241</v>
-      </c>
       <c r="F11" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G11" s="9"/>
     </row>
@@ -4517,21 +4517,21 @@
         <v>758075800</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
       <c r="C14" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D14" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="E14" s="20" t="s">
-        <v>216</v>
-      </c>
       <c r="F14" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
@@ -4546,7 +4546,7 @@
         <v>122</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="19" customFormat="1"/>

</xml_diff>

<commit_message>
IEPD updates per Diane's email on 3/30/16.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="39760" yWindow="1640" windowWidth="33280" windowHeight="16860" tabRatio="500"/>
+    <workbookView xWindow="3660" yWindow="3140" windowWidth="31340" windowHeight="15080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="274">
   <si>
     <t>CLASS</t>
   </si>
@@ -191,9 +191,6 @@
     <t>ORI of the warrant issuing agency</t>
   </si>
   <si>
-    <t>Caution Code Text</t>
-  </si>
-  <si>
     <t>ID of the person who entered the warrant</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>Person Additional Information Text</t>
   </si>
   <si>
-    <t>A cautionary code for a person</t>
-  </si>
-  <si>
     <t>Additional information about a person</t>
   </si>
   <si>
@@ -233,9 +227,6 @@
     <t>Warrant Broadcast Code Text</t>
   </si>
   <si>
-    <t>A code representing an offense</t>
-  </si>
-  <si>
     <t>A code representing an original offense.</t>
   </si>
   <si>
@@ -413,15 +404,6 @@
     <t>Vehicle Secondary Color Code Text</t>
   </si>
   <si>
-    <t>Vehicle Make Code Text</t>
-  </si>
-  <si>
-    <t>Vehicle Model Code Text</t>
-  </si>
-  <si>
-    <t>Vehicle Style Code Text</t>
-  </si>
-  <si>
     <t>Eye Color Code Text</t>
   </si>
   <si>
@@ -434,9 +416,6 @@
     <t>Place Of Birth Code Text</t>
   </si>
   <si>
-    <t>Physical Feature Category Code Text</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemModelYearDate</t>
   </si>
   <si>
@@ -497,9 +476,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonAdditionalInformationText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonCautionCodeText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -617,30 +593,12 @@
     <t>AgencyRecordIdentification</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonCitizenshipISO3166Alpha2Code</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonEthnicityCode</t>
-  </si>
-  <si>
-    <t>Citizenship Code</t>
-  </si>
-  <si>
-    <t>Ethnicity Code</t>
-  </si>
-  <si>
     <t>Race Code</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonRaceCode</t>
-  </si>
-  <si>
     <t>Sex Code</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonSexCode</t>
-  </si>
-  <si>
     <t>SID56567</t>
   </si>
   <si>
@@ -653,18 +611,9 @@
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorSecondaryCode</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/j:VehicleMakeCode</t>
-  </si>
-  <si>
     <t>DIA</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/j:VehicleModelCode</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/j:VehicleStyleCode</t>
-  </si>
-  <si>
     <t>OCA</t>
   </si>
   <si>
@@ -770,12 +719,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonMiscellaneousRecordIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>GeneralOffense Code Text</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Case/j:CaseAugmentation/j:CaseCharge/wir-ext:GeneralOffenseCodeText</t>
-  </si>
-  <si>
     <t>Prosecution Charge  Code Text</t>
   </si>
   <si>
@@ -794,9 +737,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Case/wir-ext:CriminalTrackingNumber</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonPhysicalFeature/j:PhysicalFeatureCategoryCode</t>
-  </si>
-  <si>
     <t>Person Age Description</t>
   </si>
   <si>
@@ -804,6 +744,105 @@
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonAgeDescriptionText</t>
+  </si>
+  <si>
+    <t>Vehicle Registration Expiration Date</t>
+  </si>
+  <si>
+    <t>Citizenship Text</t>
+  </si>
+  <si>
+    <t>Ethnicity Text</t>
+  </si>
+  <si>
+    <t>Race Text</t>
+  </si>
+  <si>
+    <t>Sex Text</t>
+  </si>
+  <si>
+    <t>Physical Feature Description Text</t>
+  </si>
+  <si>
+    <t>Person Additional Information CategoryText</t>
+  </si>
+  <si>
+    <t>Person Caution Text</t>
+  </si>
+  <si>
+    <t>Cautionary information about a person</t>
+  </si>
+  <si>
+    <t>Vehicle Make Name</t>
+  </si>
+  <si>
+    <t>Vehicle Model Name</t>
+  </si>
+  <si>
+    <t>Vehicle Style Text</t>
+  </si>
+  <si>
+    <t>Additional Vehicle Information Category Text</t>
+  </si>
+  <si>
+    <t>Additional Warrant Information Category Text</t>
+  </si>
+  <si>
+    <t>Further description regarding the circumstances of a charge</t>
+  </si>
+  <si>
+    <t>Warrant Information Category</t>
+  </si>
+  <si>
+    <t>Vehicle Information Category</t>
+  </si>
+  <si>
+    <t>General Offense Character Description Text</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Case/j:CaseAugmentation/j:CaseCharge/wir-ext:GeneralOffenseCharacterDescriptionText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonCitizenshipText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonEthnicityText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureDescriptionText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonAdditionalInformationCategoryText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonCautionText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemMakeName</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemModelName</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemStyleText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wir-ext:VehicleAdditionalInformationCategoryText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformationCategoryText</t>
+  </si>
+  <si>
+    <t>2016-11</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:ConveyanceRegistration[@structures:id=/wir-doc:WarrantIssuedReport/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:RegistrationExpirationDate/nc:YearMonthDate</t>
   </si>
 </sst>
 </file>
@@ -932,9 +971,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="916">
+  <cellStyleXfs count="936">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1922,7 +1981,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="916">
+  <cellStyles count="936">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2380,6 +2439,16 @@
     <cellStyle name="Followed Hyperlink" xfId="911" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="913" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="915" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="917" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="919" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="921" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="923" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="925" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="927" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="929" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="931" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="933" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="935" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2837,6 +2906,16 @@
     <cellStyle name="Hyperlink" xfId="910" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="912" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="914" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="916" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="918" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="920" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="922" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="924" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="926" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="928" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="930" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="932" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="934" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3172,18 +3251,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G298"/>
+  <dimension ref="A1:F302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
@@ -3202,7 +3281,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -3222,7 +3301,7 @@
     </row>
     <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -3234,10 +3313,10 @@
         <v>41</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="19" customFormat="1">
@@ -3248,27 +3327,27 @@
         <v>44</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="19" customFormat="1">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="19" customFormat="1" ht="30">
       <c r="A6" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>70</v>
+        <v>255</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="19" customFormat="1">
@@ -3279,13 +3358,13 @@
         <v>48</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="19" customFormat="1">
@@ -3296,27 +3375,27 @@
         <v>47</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="20" customFormat="1">
       <c r="C9" s="20" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="19" customFormat="1">
@@ -3325,16 +3404,16 @@
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="9" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="19" customFormat="1">
@@ -3355,10 +3434,10 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="19" customFormat="1">
@@ -3368,10 +3447,10 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="19" customFormat="1">
@@ -3381,10 +3460,10 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="19" customFormat="1">
@@ -3394,10 +3473,10 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="19" customFormat="1">
@@ -3407,13 +3486,13 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="19" customFormat="1" ht="45">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -3422,114 +3501,112 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="19" customFormat="1" ht="45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="19" customFormat="1" ht="45">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="19" customFormat="1" ht="45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B20" s="6"/>
       <c r="C20" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="19" customFormat="1" ht="45">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B21" s="6"/>
       <c r="C21" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="19" customFormat="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="19" customFormat="1">
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>200</v>
+        <v>242</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="20" customFormat="1" ht="25" customHeight="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="E23" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="1:7" s="20" customFormat="1" ht="25" customHeight="1">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
       <c r="A24" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="E24" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:7" s="19" customFormat="1">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
         <v>4</v>
@@ -3539,71 +3616,71 @@
         <v>23235</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="20" customFormat="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="20" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="19" customFormat="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>201</v>
+        <v>243</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="19" customFormat="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="19" customFormat="1">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="19" customFormat="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>204</v>
+        <v>245</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="19" customFormat="1">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="19" customFormat="1">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
@@ -3613,44 +3690,44 @@
         <v>354786908</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="19" customFormat="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="19" customFormat="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="19" customFormat="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="19" customFormat="1">
@@ -3663,7 +3740,7 @@
         <v>71</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="19" customFormat="1">
@@ -3673,10 +3750,10 @@
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="19" customFormat="1">
@@ -3689,7 +3766,7 @@
         <v>165</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="19" customFormat="1">
@@ -3699,34 +3776,34 @@
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="19" customFormat="1">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="19" customFormat="1">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>137</v>
+        <v>246</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="19" customFormat="1">
@@ -3739,7 +3816,7 @@
         <v>98213455</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="20" customFormat="1" ht="45">
@@ -3748,34 +3825,32 @@
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="19" customFormat="1">
-      <c r="A43" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="20" customFormat="1">
+      <c r="A43" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
-        <v>105</v>
+        <v>256</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>157</v>
+        <v>265</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="19" customFormat="1">
@@ -3784,534 +3859,584 @@
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="B45" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="19" customFormat="1">
+      <c r="A45" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="B46" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C46" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="B46" s="6"/>
-      <c r="C46" s="6" t="s">
+      <c r="D46" s="6"/>
+      <c r="E46" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="B47" s="6"/>
+      <c r="C47" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="19" customFormat="1">
-      <c r="B47" s="14" t="s">
+      <c r="E47" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="19" customFormat="1">
+      <c r="B48" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-    </row>
-    <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C48" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>161</v>
-      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
     </row>
     <row r="49" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C49" s="7" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C50" s="7" t="s">
-        <v>128</v>
+        <v>72</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="19" customFormat="1" ht="45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C51" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>109</v>
+        <v>241</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>272</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>209</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C52" s="7" t="s">
-        <v>28</v>
+        <v>125</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>139</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C53" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C54" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>196</v>
+        <v>28</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>212</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C55" s="7" t="s">
-        <v>132</v>
+        <v>250</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>213</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C56" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D56" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="C57" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C58" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E56" s="19">
+      <c r="E58" s="19">
         <v>2012</v>
       </c>
-      <c r="F56" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A57" s="19" t="s">
+      <c r="F58" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="20" customFormat="1" ht="45">
+      <c r="A59" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9" t="s">
+      <c r="C59" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A60" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D57" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E57" s="9" t="s">
+      <c r="D60" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="B61" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+    </row>
+    <row r="62" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="A62" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B62" s="16"/>
+      <c r="C62" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="B63" s="16"/>
+      <c r="C63" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7">
+        <v>6407</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="9" customFormat="1">
+      <c r="B64" s="16"/>
+      <c r="C64" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C65" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E65" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F57" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="30">
-      <c r="B58" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-    </row>
-    <row r="59" spans="1:6" s="9" customFormat="1" ht="45">
-      <c r="A59" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="9" customFormat="1" ht="45">
-      <c r="B60" s="16"/>
-      <c r="C60" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7">
-        <v>6407</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="9" customFormat="1">
-      <c r="B61" s="16"/>
-      <c r="C61" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F61" s="7"/>
-    </row>
-    <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C62" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E62" s="19" t="s">
+      <c r="F65" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C66" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E66" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="F62" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C63" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C64" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C65" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E65" s="19">
-        <v>63412</v>
-      </c>
-      <c r="F65" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="19" customFormat="1">
-      <c r="B66" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
+      <c r="F66" s="6" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="67" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C67" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D67" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E67" s="13">
-        <v>41133</v>
+        <v>31</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>117</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
-      <c r="C68" s="7" t="s">
-        <v>58</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C68" s="19" t="s">
+        <v>36</v>
       </c>
       <c r="E68" s="19">
-        <v>5000</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C69" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E69" s="13">
-        <v>40767</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>179</v>
-      </c>
+        <v>63412</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="19" customFormat="1">
+      <c r="B69" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
     </row>
     <row r="70" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C70" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E70" s="13">
+        <v>41133</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
+      <c r="C71" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E71" s="19">
+        <v>5000</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C72" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E72" s="13">
+        <v>40767</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C73" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E70" s="19">
+      <c r="E73" s="19">
         <v>659056746</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="F73" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C74" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A75" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="60">
+      <c r="A76" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C77" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E77" s="19">
+        <v>758075800</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A78" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78" s="20"/>
+      <c r="C78" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C79" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A80" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A81" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E81" s="9">
+        <v>500</v>
+      </c>
+      <c r="F81" s="19" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A82" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F82" s="19" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C71" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E71" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A72" s="19" t="s">
+    <row r="83" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C83" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D83" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="F83" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="20" customFormat="1" ht="45">
+      <c r="A84" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C72" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D72" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E72" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="60">
-      <c r="A73" s="19" t="s">
+      <c r="C84" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="F84" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="A85" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C73" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D73" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E73" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C74" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D74" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E74" s="19">
-        <v>758075800</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A75" s="20" t="s">
+      <c r="B85" s="21"/>
+      <c r="C85" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="F85" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="22" customFormat="1" ht="75">
+      <c r="A86" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B75" s="20"/>
-      <c r="C75" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="E75" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C76" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E76" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="F76" s="19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A77" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F77" s="19" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A78" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E78" s="9">
-        <v>500</v>
-      </c>
-      <c r="F78" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A79" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C79" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D79" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E79" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="F79" s="19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C80" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="D80" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="E80" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="F80" s="20" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="22" customFormat="1" ht="45">
-      <c r="A81" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B81" s="21"/>
-      <c r="C81" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="F81" s="20" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="22" customFormat="1" ht="75">
-      <c r="A82" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C82" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="D82" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="E82" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="F82" s="20" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="19" customFormat="1">
-      <c r="B83" s="22"/>
-    </row>
-    <row r="84" spans="1:6" s="19" customFormat="1"/>
-    <row r="85" spans="1:6" s="19" customFormat="1"/>
-    <row r="285" hidden="1"/>
-    <row r="286" hidden="1"/>
-    <row r="287" hidden="1"/>
-    <row r="288" hidden="1"/>
+      <c r="C86" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D86" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="E86" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="F86" s="20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" s="19" customFormat="1">
+      <c r="B87" s="22"/>
+    </row>
+    <row r="88" spans="1:6" s="19" customFormat="1"/>
+    <row r="89" spans="1:6" s="19" customFormat="1"/>
     <row r="289" hidden="1"/>
     <row r="290" hidden="1"/>
     <row r="291" hidden="1"/>
@@ -4322,6 +4447,10 @@
     <row r="296" hidden="1"/>
     <row r="297" hidden="1"/>
     <row r="298" hidden="1"/>
+    <row r="299" hidden="1"/>
+    <row r="300" hidden="1"/>
+    <row r="301" hidden="1"/>
+    <row r="302" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4370,7 +4499,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -4411,10 +4540,10 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4424,10 +4553,10 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4437,10 +4566,10 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4450,10 +4579,10 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4466,35 +4595,35 @@
         <v>23235</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="G10" s="9"/>
     </row>
@@ -4504,16 +4633,16 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="G11" s="9"/>
     </row>
@@ -4539,36 +4668,36 @@
         <v>758075800</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
       <c r="C14" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>214</v>
-      </c>
       <c r="E14" s="20" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="19" customFormat="1"/>

</xml_diff>

<commit_message>
Created "AdditionalInformation" objects in schema. Changed Vehicle Primary/Scecondary Color from "code" to "text".
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="3140" windowWidth="31340" windowHeight="15080" tabRatio="500"/>
+    <workbookView xWindow="4300" yWindow="3300" windowWidth="31340" windowHeight="15080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -422,9 +422,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wir-ext:VehicleAdditionalInformationText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonName/nc:PersonGivenName</t>
   </si>
   <si>
@@ -473,9 +470,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonSSNIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonAdditionalInformationText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -605,12 +599,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonStateIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorPrimaryCode</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorSecondaryCode</t>
-  </si>
-  <si>
     <t>DIA</t>
   </si>
   <si>
@@ -647,9 +635,6 @@
     <t>Entry</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformationText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformationText</t>
   </si>
   <si>
@@ -818,9 +803,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureDescriptionText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonAdditionalInformationCategoryText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonCautionText</t>
   </si>
   <si>
@@ -833,16 +815,34 @@
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemStyleText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wir-ext:VehicleAdditionalInformationCategoryText</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformationCategoryText</t>
-  </si>
-  <si>
     <t>2016-11</t>
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/j:ConveyanceRegistration[@structures:id=/wir-doc:WarrantIssuedReport/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:RegistrationExpirationDate/nc:YearMonthDate</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorPrimaryText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorSecondaryText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonAdditionalInformation/wir-ext:PersonAdditionalInformationCategoryText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonAdditionalInformation/wir-ext:PersonAdditionalInformationText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wir-ext:VehicleAdditionalInformation/wir-ext:VehicleAdditionalInformationCategoryText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wir-ext:VehicleAdditionalInformation/wir-ext:VehicleAdditionalInformationText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformation/wir-ext:WarrantAdditionalInformationCategoryText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformation/wir-ext:WarrantAdditionalInformationText</t>
   </si>
 </sst>
 </file>
@@ -3254,8 +3254,8 @@
   <dimension ref="A1:F302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
+      <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3316,7 +3316,7 @@
         <v>75</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="19" customFormat="1">
@@ -3330,7 +3330,7 @@
         <v>76</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="19" customFormat="1" ht="30">
@@ -3338,16 +3338,16 @@
         <v>37</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="19" customFormat="1">
@@ -3364,7 +3364,7 @@
         <v>78</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="19" customFormat="1">
@@ -3381,21 +3381,21 @@
         <v>79</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="20" customFormat="1">
       <c r="C9" s="20" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="19" customFormat="1">
@@ -3404,16 +3404,16 @@
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>121</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="19" customFormat="1">
@@ -3437,7 +3437,7 @@
         <v>80</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="19" customFormat="1">
@@ -3450,7 +3450,7 @@
         <v>81</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="19" customFormat="1">
@@ -3463,7 +3463,7 @@
         <v>82</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="19" customFormat="1">
@@ -3476,7 +3476,7 @@
         <v>83</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="19" customFormat="1">
@@ -3489,7 +3489,7 @@
         <v>84</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3504,7 +3504,7 @@
         <v>85</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3517,7 +3517,7 @@
         <v>86</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3530,7 +3530,7 @@
         <v>87</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3543,7 +3543,7 @@
         <v>83</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3556,7 +3556,7 @@
         <v>88</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="19" customFormat="1">
@@ -3564,28 +3564,28 @@
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>89</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E23" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
@@ -3594,16 +3594,16 @@
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E24" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
@@ -3616,44 +3616,44 @@
         <v>23235</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="20" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>90</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>96</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="19" customFormat="1">
@@ -3665,19 +3665,19 @@
         <v>91</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>97</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="19" customFormat="1">
@@ -3690,20 +3690,20 @@
         <v>354786908</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="19" customFormat="1">
@@ -3715,7 +3715,7 @@
         <v>98</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="19" customFormat="1">
@@ -3727,7 +3727,7 @@
         <v>92</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="19" customFormat="1">
@@ -3740,7 +3740,7 @@
         <v>71</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="19" customFormat="1">
@@ -3753,7 +3753,7 @@
         <v>93</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="19" customFormat="1">
@@ -3766,7 +3766,7 @@
         <v>165</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="19" customFormat="1">
@@ -3779,7 +3779,7 @@
         <v>94</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="19" customFormat="1">
@@ -3791,19 +3791,19 @@
         <v>95</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="19" customFormat="1">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="19" customFormat="1">
@@ -3816,7 +3816,7 @@
         <v>98213455</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="20" customFormat="1" ht="45">
@@ -3825,35 +3825,35 @@
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="20" customFormat="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="20" customFormat="1" ht="30">
       <c r="A43" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="19" customFormat="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="30">
       <c r="A44" s="19" t="s">
         <v>37</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>102</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>150</v>
+        <v>269</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="19" customFormat="1">
@@ -3877,16 +3877,16 @@
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>104</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3901,7 +3901,7 @@
         <v>100</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3916,7 +3916,7 @@
         <v>101</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="19" customFormat="1">
@@ -3936,7 +3936,7 @@
         <v>111</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3947,18 +3947,18 @@
         <v>112</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C51" s="7" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3969,7 +3969,7 @@
         <v>105</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>194</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3980,7 +3980,7 @@
         <v>106</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>195</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3996,44 +3996,44 @@
     </row>
     <row r="55" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C55" s="7" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>109</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C56" s="7" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="19" customFormat="1" ht="30">
       <c r="C57" s="7" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E57" s="19" t="s">
         <v>107</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4052,10 +4052,10 @@
         <v>37</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>270</v>
@@ -4076,7 +4076,7 @@
         <v>110</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>133</v>
+        <v>271</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="19" customFormat="1" ht="30">
@@ -4101,7 +4101,7 @@
         <v>115</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="9" customFormat="1" ht="45">
@@ -4114,7 +4114,7 @@
         <v>6407</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="9" customFormat="1">
@@ -4136,7 +4136,7 @@
         <v>113</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4147,7 +4147,7 @@
         <v>116</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4158,7 +4158,7 @@
         <v>117</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4169,7 +4169,7 @@
         <v>63412</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="19" customFormat="1">
@@ -4192,7 +4192,7 @@
         <v>41133</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
@@ -4203,7 +4203,7 @@
         <v>5000</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4214,7 +4214,7 @@
         <v>40767</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4225,7 +4225,7 @@
         <v>659056746</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4236,7 +4236,7 @@
         <v>118</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4253,7 +4253,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="19" customFormat="1" ht="60">
@@ -4270,7 +4270,7 @@
         <v>120</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4284,7 +4284,7 @@
         <v>758075800</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4293,16 +4293,16 @@
       </c>
       <c r="B78" s="20"/>
       <c r="C78" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4316,7 +4316,7 @@
         <v>119</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4334,7 +4334,7 @@
         <v>103</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4352,7 +4352,7 @@
         <v>500</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4369,32 +4369,32 @@
         <v>122</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C83" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D83" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="20" customFormat="1" ht="45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="20" customFormat="1" ht="60">
       <c r="A84" s="20" t="s">
         <v>37</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="22" customFormat="1" ht="45">
@@ -4403,16 +4403,16 @@
       </c>
       <c r="B85" s="21"/>
       <c r="C85" s="9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>208</v>
+        <v>273</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="22" customFormat="1" ht="75">
@@ -4420,16 +4420,16 @@
         <v>37</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D86" s="20" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E86" s="20" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F86" s="20" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="19" customFormat="1">
@@ -4543,7 +4543,7 @@
         <v>80</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4556,7 +4556,7 @@
         <v>81</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4569,7 +4569,7 @@
         <v>82</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4582,7 +4582,7 @@
         <v>83</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4595,35 +4595,35 @@
         <v>23235</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
         <v>96</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
         <v>97</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G10" s="9"/>
     </row>
@@ -4633,16 +4633,16 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>221</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>226</v>
       </c>
       <c r="G11" s="9"/>
     </row>
@@ -4668,21 +4668,21 @@
         <v>758075800</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
       <c r="C14" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
@@ -4697,7 +4697,7 @@
         <v>119</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="19" customFormat="1"/>

</xml_diff>

<commit_message>
Updated XPATH in mapping spreadsheets for streetname & charge severity
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="275">
   <si>
     <t>CLASS</t>
   </si>
@@ -843,6 +843,9 @@
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformation/wir-ext:WarrantAdditionalInformationText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStreet/nc:StreetName</t>
   </si>
 </sst>
 </file>
@@ -3254,8 +3257,8 @@
   <dimension ref="A1:F302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
+      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4117,7 +4120,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B64" s="16"/>
       <c r="C64" s="7" t="s">
         <v>35</v>
@@ -4126,7 +4129,9 @@
       <c r="E64" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="F64" s="7"/>
+      <c r="F64" s="6" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="65" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C65" s="7" t="s">

</xml_diff>

<commit_message>
Changed Warrant Accepted Report...'code' to 'text'.  Added WarrantEntryCategoryCodeText.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="3300" windowWidth="31335" windowHeight="15075" tabRatio="500"/>
+    <workbookView xWindow="3600" yWindow="1300" windowWidth="31340" windowHeight="15080" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="274">
   <si>
     <t>CLASS</t>
   </si>
@@ -587,12 +587,6 @@
     <t>AgencyRecordIdentification</t>
   </si>
   <si>
-    <t>Race Code</t>
-  </si>
-  <si>
-    <t>Sex Code</t>
-  </si>
-  <si>
     <t>SID56567</t>
   </si>
   <si>
@@ -635,9 +629,6 @@
     <t>Entry</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformationText</t>
-  </si>
-  <si>
     <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
   </si>
   <si>
@@ -650,12 +641,6 @@
     <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
   </si>
   <si>
-    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/j:PersonRaceCode</t>
-  </si>
-  <si>
-    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/j:PersonSexCode</t>
-  </si>
-  <si>
     <t>war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderEnforcementAgency/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -846,6 +831,18 @@
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStreet/nc:StreetName</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantEntryCategoryCodeText</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/j:Warrant/wir-ext:WarrantAugmentation</t>
   </si>
 </sst>
 </file>
@@ -974,9 +971,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="936">
+  <cellStyleXfs count="946">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1984,7 +1991,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="936">
+  <cellStyles count="946">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2452,6 +2459,11 @@
     <cellStyle name="Followed Hyperlink" xfId="931" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="933" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="935" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="937" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="939" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="941" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="943" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="945" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2919,6 +2931,11 @@
     <cellStyle name="Hyperlink" xfId="930" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="932" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="934" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="936" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="938" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="940" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="942" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="944" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3256,23 +3273,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F302"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="28.375" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="2"/>
+    <col min="5" max="5" width="28.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="23" t="s">
         <v>54</v>
@@ -3282,7 +3299,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>123</v>
       </c>
@@ -3302,7 +3319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
         <v>70</v>
       </c>
@@ -3311,7 +3328,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="19" customFormat="1">
       <c r="C4" s="7" t="s">
         <v>41</v>
       </c>
@@ -3322,7 +3339,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="19" customFormat="1">
       <c r="C5" s="7" t="s">
         <v>43</v>
       </c>
@@ -3336,24 +3353,24 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.5">
       <c r="A6" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="19" customFormat="1">
       <c r="A7" s="19" t="s">
         <v>37</v>
       </c>
@@ -3370,7 +3387,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="19" customFormat="1">
       <c r="A8" s="19" t="s">
         <v>37</v>
       </c>
@@ -3387,21 +3404,21 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="20" customFormat="1" ht="31.5">
       <c r="C9" s="20" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="19" customFormat="1">
       <c r="A10" s="19" t="s">
         <v>37</v>
       </c>
@@ -3410,16 +3427,16 @@
         <v>181</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>121</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="19" customFormat="1">
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
@@ -3428,7 +3445,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="19" customFormat="1">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -3443,7 +3460,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="19" customFormat="1">
       <c r="B13" s="6"/>
       <c r="C13" s="19" t="s">
         <v>10</v>
@@ -3456,7 +3473,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="19" customFormat="1">
       <c r="B14" s="6"/>
       <c r="C14" s="19" t="s">
         <v>11</v>
@@ -3469,7 +3486,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="19" customFormat="1">
       <c r="B15" s="6"/>
       <c r="C15" s="19" t="s">
         <v>12</v>
@@ -3482,7 +3499,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="19" customFormat="1">
       <c r="B16" s="6"/>
       <c r="C16" s="19" t="s">
         <v>25</v>
@@ -3495,7 +3512,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -3510,7 +3527,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>10</v>
@@ -3523,7 +3540,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>11</v>
@@ -3536,7 +3553,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19" t="s">
         <v>12</v>
@@ -3549,7 +3566,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B21" s="6"/>
       <c r="C21" s="19" t="s">
         <v>25</v>
@@ -3562,12 +3579,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="19" customFormat="1">
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>182</v>
@@ -3576,40 +3593,40 @@
         <v>89</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="20" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E23" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
       <c r="A24" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E24" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="19" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
         <v>4</v>
@@ -3622,44 +3639,44 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="20" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>90</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>96</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
         <v>127</v>
@@ -3671,19 +3688,19 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>97</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="19" customFormat="1">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
@@ -3696,20 +3713,20 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>183</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="19" customFormat="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>128</v>
@@ -3721,7 +3738,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="19" customFormat="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
         <v>129</v>
@@ -3733,7 +3750,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="19" customFormat="1">
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
         <v>21</v>
@@ -3746,7 +3763,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="19" customFormat="1">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
         <v>22</v>
@@ -3759,7 +3776,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="19" customFormat="1">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
         <v>23</v>
@@ -3772,7 +3789,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="19" customFormat="1">
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
         <v>24</v>
@@ -3785,7 +3802,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="19" customFormat="1">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
         <v>130</v>
@@ -3797,19 +3814,19 @@
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="19" customFormat="1">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="19" customFormat="1">
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
         <v>6</v>
@@ -3822,41 +3839,41 @@
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="47.25">
       <c r="A42" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="20" customFormat="1" ht="31.5">
       <c r="A43" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="31.5">
       <c r="A44" s="19" t="s">
         <v>37</v>
       </c>
@@ -3871,28 +3888,28 @@
         <v>102</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="19" customFormat="1">
       <c r="A45" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>104</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B46" s="6" t="s">
         <v>17</v>
       </c>
@@ -3907,7 +3924,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B47" s="6"/>
       <c r="C47" s="6" t="s">
         <v>19</v>
@@ -3922,7 +3939,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="19" customFormat="1">
       <c r="B48" s="14" t="s">
         <v>26</v>
       </c>
@@ -3931,7 +3948,7 @@
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
     </row>
-    <row r="49" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C49" s="7" t="s">
         <v>27</v>
       </c>
@@ -3942,7 +3959,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C50" s="7" t="s">
         <v>72</v>
       </c>
@@ -3953,18 +3970,18 @@
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C51" s="7" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C52" s="7" t="s">
         <v>125</v>
       </c>
@@ -3972,10 +3989,10 @@
         <v>105</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C53" s="7" t="s">
         <v>126</v>
       </c>
@@ -3983,10 +4000,10 @@
         <v>106</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C54" s="7" t="s">
         <v>28</v>
       </c>
@@ -3997,9 +4014,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C55" s="7" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>186</v>
@@ -4008,26 +4025,26 @@
         <v>109</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C56" s="7" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>186</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C57" s="7" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D57" s="19" t="s">
         <v>186</v>
@@ -4036,10 +4053,10 @@
         <v>107</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C58" s="7" t="s">
         <v>29</v>
       </c>
@@ -4050,21 +4067,21 @@
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" s="20" customFormat="1" ht="47.25">
       <c r="A59" s="20" t="s">
         <v>37</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A60" s="19" t="s">
         <v>37</v>
       </c>
@@ -4079,10 +4096,10 @@
         <v>110</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="19" customFormat="1" ht="31.5">
       <c r="B61" s="14" t="s">
         <v>49</v>
       </c>
@@ -4091,7 +4108,7 @@
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
     </row>
-    <row r="62" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" s="9" customFormat="1" ht="47.25">
       <c r="A62" s="9" t="s">
         <v>37</v>
       </c>
@@ -4107,7 +4124,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" s="9" customFormat="1" ht="47.25">
       <c r="B63" s="16"/>
       <c r="C63" s="7" t="s">
         <v>34</v>
@@ -4120,7 +4137,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" s="9" customFormat="1" ht="47.25">
       <c r="B64" s="16"/>
       <c r="C64" s="7" t="s">
         <v>35</v>
@@ -4130,10 +4147,10 @@
         <v>114</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C65" s="7" t="s">
         <v>30</v>
       </c>
@@ -4144,7 +4161,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C66" s="7" t="s">
         <v>32</v>
       </c>
@@ -4155,7 +4172,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C67" s="7" t="s">
         <v>31</v>
       </c>
@@ -4166,7 +4183,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C68" s="19" t="s">
         <v>36</v>
       </c>
@@ -4177,7 +4194,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="19" customFormat="1">
       <c r="B69" s="14" t="s">
         <v>38</v>
       </c>
@@ -4186,7 +4203,7 @@
       <c r="E69" s="15"/>
       <c r="F69" s="15"/>
     </row>
-    <row r="70" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C70" s="7" t="s">
         <v>39</v>
       </c>
@@ -4200,7 +4217,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
       <c r="C71" s="7" t="s">
         <v>57</v>
       </c>
@@ -4211,7 +4228,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C72" s="7" t="s">
         <v>45</v>
       </c>
@@ -4222,7 +4239,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C73" s="7" t="s">
         <v>42</v>
       </c>
@@ -4233,7 +4250,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C74" s="7" t="s">
         <v>58</v>
       </c>
@@ -4244,7 +4261,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A75" s="19" t="s">
         <v>37</v>
       </c>
@@ -4261,7 +4278,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="63">
       <c r="A76" s="19" t="s">
         <v>37</v>
       </c>
@@ -4278,7 +4295,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C77" s="6" t="s">
         <v>46</v>
       </c>
@@ -4292,7 +4309,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A78" s="20" t="s">
         <v>37</v>
       </c>
@@ -4301,16 +4318,16 @@
         <v>187</v>
       </c>
       <c r="D78" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F78" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E78" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C79" s="19" t="s">
         <v>74</v>
       </c>
@@ -4324,7 +4341,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A80" s="19" t="s">
         <v>37</v>
       </c>
@@ -4342,7 +4359,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A81" s="19" t="s">
         <v>37</v>
       </c>
@@ -4360,7 +4377,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A82" s="19" t="s">
         <v>37</v>
       </c>
@@ -4377,7 +4394,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C83" s="20" t="s">
         <v>184</v>
       </c>
@@ -4385,77 +4402,77 @@
         <v>185</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="20" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="20" customFormat="1" ht="60">
       <c r="A84" s="20" t="s">
         <v>37</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="22" customFormat="1" ht="47.25">
       <c r="A85" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B85" s="21"/>
       <c r="C85" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E85" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="D85" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>200</v>
-      </c>
       <c r="F85" s="20" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" s="22" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="22" customFormat="1" ht="45">
       <c r="A86" s="20" t="s">
         <v>37</v>
       </c>
       <c r="C86" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="D86" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="E86" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="D86" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="E86" s="20" t="s">
-        <v>203</v>
-      </c>
       <c r="F86" s="20" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" s="19" customFormat="1">
       <c r="B87" s="22"/>
     </row>
-    <row r="88" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="292" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="293" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="294" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="295" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="296" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="297" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="298" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="299" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="300" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="301" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="302" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:6" s="19" customFormat="1"/>
+    <row r="89" spans="1:6" s="19" customFormat="1"/>
+    <row r="289" ht="15.75" hidden="1"/>
+    <row r="290" ht="15.75" hidden="1"/>
+    <row r="291" ht="15.75" hidden="1"/>
+    <row r="292" ht="15.75" hidden="1"/>
+    <row r="293" ht="15.75" hidden="1"/>
+    <row r="294" ht="15.75" hidden="1"/>
+    <row r="295" ht="15.75" hidden="1"/>
+    <row r="296" ht="15.75" hidden="1"/>
+    <row r="297" ht="15.75" hidden="1"/>
+    <row r="298" ht="15.75" hidden="1"/>
+    <row r="299" ht="15.75" hidden="1"/>
+    <row r="300" ht="15.75" hidden="1"/>
+    <row r="301" ht="15.75" hidden="1"/>
+    <row r="302" ht="15.75" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4475,23 +4492,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="2"/>
+    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="23" t="s">
         <v>53</v>
@@ -4502,7 +4519,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>123</v>
       </c>
@@ -4525,7 +4542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -4536,7 +4553,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4551,7 +4568,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B5" s="6"/>
       <c r="C5" s="19" t="s">
         <v>10</v>
@@ -4561,10 +4578,10 @@
         <v>81</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B6" s="6"/>
       <c r="C6" s="19" t="s">
         <v>11</v>
@@ -4574,10 +4591,10 @@
         <v>82</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B7" s="6"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
@@ -4587,10 +4604,10 @@
         <v>83</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4600,58 +4617,58 @@
         <v>23235</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
         <v>96</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>209</v>
+        <v>270</v>
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
         <v>97</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>210</v>
+        <v>271</v>
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" s="20" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="20" customFormat="1" ht="53" customHeight="1">
       <c r="A11" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>221</v>
-      </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>38</v>
@@ -4662,7 +4679,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
@@ -4673,24 +4690,24 @@
         <v>758075800</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.5">
       <c r="C14" s="6" t="s">
         <v>187</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
         <v>74</v>
@@ -4702,234 +4719,241 @@
         <v>119</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="19" customFormat="1">
+      <c r="C16" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="19" customFormat="1"/>
+    <row r="18" spans="1:1" s="19" customFormat="1"/>
+    <row r="19" spans="1:1" s="19" customFormat="1"/>
+    <row r="20" spans="1:1" s="19" customFormat="1"/>
+    <row r="21" spans="1:1" s="19" customFormat="1"/>
+    <row r="22" spans="1:1" s="19" customFormat="1"/>
+    <row r="23" spans="1:1">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="19"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="19"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="19"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="19"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="19"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="19"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="19"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="19"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="19"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="19"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="19"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="19"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="19"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="19"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="19"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="19"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="19"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="19"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="19"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="19"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="19"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" s="19"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" s="9"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" s="9"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1">
       <c r="A59" s="19"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1">
       <c r="A60" s="19"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1">
       <c r="A61" s="19"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1">
       <c r="A62" s="19"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1">
       <c r="A63" s="19"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1">
       <c r="A64" s="19"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1">
       <c r="A65" s="19"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1">
       <c r="A66" s="19"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1">
       <c r="A67" s="19"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1">
       <c r="A68" s="19"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1">
       <c r="A69" s="19"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1">
       <c r="A70" s="19"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1">
       <c r="A71" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1">
       <c r="A72" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1">
       <c r="A73" s="19"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1">
       <c r="A74" s="19"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1">
       <c r="A75" s="19"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1">
       <c r="A76" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1">
       <c r="A77" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1">
       <c r="A78" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1">
       <c r="A79" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1">
       <c r="A80" s="19"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1">
       <c r="A81" s="19"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1">
       <c r="A82" s="19"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1">
       <c r="A83" s="19"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1">
       <c r="A84" s="19"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1">
       <c r="A85" s="19"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1">
       <c r="A86" s="19"/>
     </row>
   </sheetData>
@@ -4954,7 +4978,7 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Removed "Additional Elements" for Warrant, Vehicle and Person.  Added WarrantCommentText.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="1300" windowWidth="31340" windowHeight="15080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3600" yWindow="1300" windowWidth="31340" windowHeight="15080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="258">
   <si>
     <t>CLASS</t>
   </si>
@@ -173,9 +173,6 @@
     <t>CONTACT LOCATION (Subject)</t>
   </si>
   <si>
-    <t>Additional Vehicle Information Text</t>
-  </si>
-  <si>
     <t>Person Record Number</t>
   </si>
   <si>
@@ -200,15 +197,6 @@
     <t>Subject Corrections ID</t>
   </si>
   <si>
-    <t>Person Additional Information Text</t>
-  </si>
-  <si>
-    <t>Additional information about a person</t>
-  </si>
-  <si>
-    <t>Additional information about a vehicle.</t>
-  </si>
-  <si>
     <t>Extradition Indicator</t>
   </si>
   <si>
@@ -329,9 +317,6 @@
     <t>MI</t>
   </si>
   <si>
-    <t>Gang member</t>
-  </si>
-  <si>
     <t>R69458998</t>
   </si>
   <si>
@@ -353,9 +338,6 @@
     <t>AAA</t>
   </si>
   <si>
-    <t>Excessive Rust</t>
-  </si>
-  <si>
     <t>LP4365-0234</t>
   </si>
   <si>
@@ -611,9 +593,6 @@
     <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/scr:TransactionControlNumberIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>Additional Warrant Information Text</t>
-  </si>
-  <si>
     <t>Additional information about a warrant.</t>
   </si>
   <si>
@@ -734,9 +713,6 @@
     <t>Physical Feature Description Text</t>
   </si>
   <si>
-    <t>Person Additional Information CategoryText</t>
-  </si>
-  <si>
     <t>Person Caution Text</t>
   </si>
   <si>
@@ -752,21 +728,9 @@
     <t>Vehicle Style Text</t>
   </si>
   <si>
-    <t>Additional Vehicle Information Category Text</t>
-  </si>
-  <si>
-    <t>Additional Warrant Information Category Text</t>
-  </si>
-  <si>
     <t>Further description regarding the circumstances of a charge</t>
   </si>
   <si>
-    <t>Warrant Information Category</t>
-  </si>
-  <si>
-    <t>Vehicle Information Category</t>
-  </si>
-  <si>
     <t>General Offense Character Description Text</t>
   </si>
   <si>
@@ -812,24 +776,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorSecondaryText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonAdditionalInformation/wir-ext:PersonAdditionalInformationCategoryText</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonAdditionalInformation/wir-ext:PersonAdditionalInformationText</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wir-ext:VehicleAdditionalInformation/wir-ext:VehicleAdditionalInformationCategoryText</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wir-ext:VehicleAdditionalInformation/wir-ext:VehicleAdditionalInformationText</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformation/wir-ext:WarrantAdditionalInformationCategoryText</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformation/wir-ext:WarrantAdditionalInformationText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStreet/nc:StreetName</t>
   </si>
   <si>
@@ -843,6 +789,12 @@
   </si>
   <si>
     <t>war-doc:WarrantAcceptedReport/j:Warrant/wir-ext:WarrantAugmentation</t>
+  </si>
+  <si>
+    <t>Warrant Comment Text</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantCommentText</t>
   </si>
 </sst>
 </file>
@@ -3271,11 +3223,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F302"/>
+  <dimension ref="A1:F297"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3292,7 +3244,7 @@
     <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="10"/>
@@ -3301,7 +3253,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -3321,7 +3273,7 @@
     </row>
     <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -3333,10 +3285,10 @@
         <v>41</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="19" customFormat="1">
@@ -3347,27 +3299,27 @@
         <v>44</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="19" customFormat="1" ht="30">
       <c r="A6" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="19" customFormat="1">
@@ -3378,13 +3330,13 @@
         <v>48</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="19" customFormat="1">
@@ -3395,27 +3347,27 @@
         <v>47</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="20" customFormat="1" ht="31.5">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="20" customFormat="1">
       <c r="C9" s="20" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="19" customFormat="1">
@@ -3424,16 +3376,16 @@
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="19" customFormat="1">
@@ -3454,10 +3406,10 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="19" customFormat="1">
@@ -3467,10 +3419,10 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="19" customFormat="1">
@@ -3480,10 +3432,10 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="19" customFormat="1">
@@ -3493,10 +3445,10 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="19" customFormat="1">
@@ -3506,13 +3458,13 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="19" customFormat="1" ht="47.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -3521,62 +3473,62 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="19" customFormat="1" ht="47.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" ht="47.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="19" customFormat="1" ht="47.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B20" s="6"/>
       <c r="C20" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="19" customFormat="1" ht="47.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B21" s="6"/>
       <c r="C21" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="19" customFormat="1">
@@ -3584,28 +3536,28 @@
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E23" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
@@ -3614,16 +3566,16 @@
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E24" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
@@ -3636,68 +3588,68 @@
         <v>23235</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="20" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="19" customFormat="1">
@@ -3710,44 +3662,44 @@
         <v>354786908</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="19" customFormat="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="19" customFormat="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="19" customFormat="1">
@@ -3760,7 +3712,7 @@
         <v>71</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="19" customFormat="1">
@@ -3770,10 +3722,10 @@
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="19" customFormat="1">
@@ -3786,7 +3738,7 @@
         <v>165</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="19" customFormat="1">
@@ -3796,34 +3748,34 @@
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="19" customFormat="1">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="19" customFormat="1">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="19" customFormat="1">
@@ -3836,643 +3788,566 @@
         <v>98213455</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="47.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="45">
       <c r="A42" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="20" customFormat="1" ht="31.5">
-      <c r="A43" s="20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="19" customFormat="1">
+      <c r="A43" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="D43" s="7"/>
+        <v>230</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="E43" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="B44" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="19" customFormat="1">
+      <c r="B46" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+    </row>
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C47" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C48" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+      <c r="C49" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C50" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C51" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C52" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C53" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C54" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="C55" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="F43" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="31.5">
-      <c r="A44" s="19" t="s">
+    </row>
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C56" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E56" s="19">
+        <v>2012</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="B57" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+    </row>
+    <row r="58" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="A58" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7" t="s">
+      <c r="B58" s="16"/>
+      <c r="C58" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="B59" s="16"/>
+      <c r="C59" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7">
+        <v>6407</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="B60" s="16"/>
+      <c r="C60" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C61" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C62" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C63" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C64" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="19">
+        <v>63412</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="19" customFormat="1">
+      <c r="B65" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+    </row>
+    <row r="66" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C66" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E66" s="13">
+        <v>41133</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
+      <c r="C67" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E67" s="19">
+        <v>5000</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C68" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E68" s="13">
+        <v>40767</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C69" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" s="19">
+        <v>659056746</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C70" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A71" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E71" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="60">
+      <c r="A72" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C72" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="19" customFormat="1">
-      <c r="A45" s="19" t="s">
+      <c r="D72" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C73" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E73" s="19">
+        <v>758075800</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A74" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="B46" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="B47" s="6"/>
-      <c r="C47" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="19" customFormat="1">
-      <c r="B48" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-    </row>
-    <row r="49" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C49" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C50" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E50" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
-      <c r="C51" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="E51" s="20" t="s">
-        <v>259</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C52" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C53" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C54" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C55" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D55" s="19" t="s">
+      <c r="B74" s="20"/>
+      <c r="C74" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E74" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="E55" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C56" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C57" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="D57" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C58" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E58" s="19">
-        <v>2012</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="20" customFormat="1" ht="47.25">
-      <c r="A59" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>247</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="A60" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="19" customFormat="1" ht="31.5">
-      <c r="B61" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
-    </row>
-    <row r="62" spans="1:6" s="9" customFormat="1" ht="47.25">
-      <c r="A62" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="9" customFormat="1" ht="47.25">
-      <c r="B63" s="16"/>
-      <c r="C63" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7">
-        <v>6407</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="9" customFormat="1" ht="47.25">
-      <c r="B64" s="16"/>
-      <c r="C64" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C65" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E65" s="19" t="s">
+      <c r="F74" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C75" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E75" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F65" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C66" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C67" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C68" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E68" s="19">
-        <v>63412</v>
-      </c>
-      <c r="F68" s="19" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="19" customFormat="1">
-      <c r="B69" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-    </row>
-    <row r="70" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C70" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D70" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E70" s="13">
-        <v>41133</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
-      <c r="C71" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E71" s="19">
-        <v>5000</v>
-      </c>
-      <c r="F71" s="6" t="s">
+      <c r="F75" s="19" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C72" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E72" s="13">
-        <v>40767</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C73" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E73" s="19">
-        <v>659056746</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C74" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E74" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="A75" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D75" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E75" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="63">
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="A76" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="B76" s="9"/>
+      <c r="C76" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A77" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E77" s="9">
+        <v>500</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A78" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C78" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D76" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E76" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C77" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E77" s="19">
-        <v>758075800</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="A78" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B78" s="20"/>
-      <c r="C78" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>191</v>
+      <c r="D78" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C79" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D79" s="19" t="s">
-        <v>56</v>
+        <v>116</v>
+      </c>
+      <c r="F78" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C79" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>179</v>
       </c>
       <c r="E79" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="F79" s="19" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="A80" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="F79" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="20" customFormat="1" ht="45">
+      <c r="A80" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B80" s="9"/>
       <c r="C80" s="9" t="s">
-        <v>51</v>
+        <v>256</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="F80" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="A81" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="A81" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E81" s="9">
-        <v>500</v>
-      </c>
-      <c r="F81" s="19" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="A82" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C82" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D82" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="19" customFormat="1" ht="47.25">
-      <c r="C83" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="D83" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="E83" s="19" t="s">
+      <c r="C81" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E81" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="F83" s="20" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="20" customFormat="1" ht="60">
-      <c r="A84" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="F84" s="20" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="22" customFormat="1" ht="47.25">
-      <c r="A85" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B85" s="21"/>
-      <c r="C85" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="F85" s="20" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" s="22" customFormat="1" ht="45">
-      <c r="A86" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C86" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="D86" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="E86" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="F86" s="20" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" s="19" customFormat="1">
-      <c r="B87" s="22"/>
-    </row>
-    <row r="88" spans="1:6" s="19" customFormat="1"/>
-    <row r="89" spans="1:6" s="19" customFormat="1"/>
-    <row r="289" ht="15.75" hidden="1"/>
-    <row r="290" ht="15.75" hidden="1"/>
-    <row r="291" ht="15.75" hidden="1"/>
-    <row r="292" ht="15.75" hidden="1"/>
-    <row r="293" ht="15.75" hidden="1"/>
-    <row r="294" ht="15.75" hidden="1"/>
-    <row r="295" ht="15.75" hidden="1"/>
-    <row r="296" ht="15.75" hidden="1"/>
-    <row r="297" ht="15.75" hidden="1"/>
-    <row r="298" ht="15.75" hidden="1"/>
-    <row r="299" ht="15.75" hidden="1"/>
-    <row r="300" ht="15.75" hidden="1"/>
-    <row r="301" ht="15.75" hidden="1"/>
-    <row r="302" ht="15.75" hidden="1"/>
+      <c r="F81" s="20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="19" customFormat="1">
+      <c r="B82" s="22"/>
+    </row>
+    <row r="83" spans="1:6" s="19" customFormat="1"/>
+    <row r="84" spans="1:6" s="19" customFormat="1"/>
+    <row r="284" hidden="1"/>
+    <row r="285" hidden="1"/>
+    <row r="286" hidden="1"/>
+    <row r="287" hidden="1"/>
+    <row r="288" hidden="1"/>
+    <row r="289" hidden="1"/>
+    <row r="290" hidden="1"/>
+    <row r="291" hidden="1"/>
+    <row r="292" hidden="1"/>
+    <row r="293" hidden="1"/>
+    <row r="294" hidden="1"/>
+    <row r="295" hidden="1"/>
+    <row r="296" hidden="1"/>
+    <row r="297" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4492,8 +4367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4511,7 +4386,7 @@
     <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="10"/>
@@ -4521,7 +4396,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -4553,7 +4428,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4562,52 +4437,52 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" ht="47.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B5" s="6"/>
       <c r="C5" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="19" customFormat="1" ht="47.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B6" s="6"/>
       <c r="C6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" ht="47.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B7" s="6"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="19" customFormat="1" ht="47.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4617,35 +4492,35 @@
         <v>23235</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="G10" s="9"/>
     </row>
@@ -4655,16 +4530,16 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G11" s="9"/>
     </row>
@@ -4679,55 +4554,55 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="19">
         <v>758075800</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.5">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
       <c r="C14" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="19" customFormat="1">
       <c r="C16" s="20" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:1" s="19" customFormat="1"/>

</xml_diff>

<commit_message>
Added remaining elements from Warrant Issued Reporting SSP.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="258">
   <si>
     <t>CLASS</t>
   </si>
@@ -1871,7 +1871,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1940,6 +1940,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3226,8 +3235,8 @@
   <dimension ref="A1:F297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A80:XFD80"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3356,35 +3365,38 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="20" customFormat="1">
-      <c r="C9" s="20" t="s">
+    <row r="9" spans="1:6" s="22" customFormat="1">
+      <c r="A9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="22" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="19" customFormat="1">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:6" s="22" customFormat="1">
+      <c r="A10" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="22" t="s">
         <v>220</v>
       </c>
     </row>
@@ -4089,17 +4101,17 @@
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
     </row>
-    <row r="66" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C66" s="7" t="s">
+    <row r="66" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="C66" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D66" s="19" t="s">
+      <c r="D66" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E66" s="13">
+      <c r="E66" s="25">
         <v>41133</v>
       </c>
-      <c r="F66" s="6" t="s">
+      <c r="F66" s="26" t="s">
         <v>162</v>
       </c>
     </row>
@@ -4136,14 +4148,14 @@
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C70" s="7" t="s">
+    <row r="70" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="C70" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E70" s="19" t="s">
+      <c r="E70" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="F70" s="26" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Vehicle Registartion State Code to 'issued' and 'modification' SSPs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="1300" windowWidth="31340" windowHeight="15080" tabRatio="500"/>
+    <workbookView xWindow="6000" yWindow="1280" windowWidth="31340" windowHeight="15080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="260">
   <si>
     <t>CLASS</t>
   </si>
@@ -795,6 +795,12 @@
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantCommentText</t>
+  </si>
+  <si>
+    <t>Vehicle RegistrationState</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:ConveyanceRegistration[@structures:id=/wir-doc:WarrantIssuedReport/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:JurisdictionNCICLISCode</t>
   </si>
 </sst>
 </file>
@@ -923,9 +929,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="946">
+  <cellStyleXfs count="948">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1939,9 +1947,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1951,8 +1956,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="946">
+  <cellStyles count="948">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2425,6 +2433,7 @@
     <cellStyle name="Followed Hyperlink" xfId="941" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="943" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="945" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="947" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2897,6 +2906,7 @@
     <cellStyle name="Hyperlink" xfId="940" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="942" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="944" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="946" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3232,11 +3242,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F297"/>
+  <dimension ref="A1:F298"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3244,18 +3254,18 @@
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="40.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="40.5" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="10"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -3911,350 +3921,343 @@
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="50" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C50" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E50" s="19" t="s">
-        <v>100</v>
+        <v>258</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C51" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C52" s="7" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C53" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>180</v>
+        <v>28</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>244</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C54" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D54" s="19" t="s">
         <v>180</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>184</v>
+        <v>104</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="30">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C55" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>180</v>
       </c>
       <c r="E55" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="C56" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D56" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E56" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F56" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C56" s="7" t="s">
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C57" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E56" s="19">
+      <c r="E57" s="19">
         <v>2012</v>
       </c>
-      <c r="F56" s="6" t="s">
+      <c r="F57" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="30">
-      <c r="B57" s="14" t="s">
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="B58" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-    </row>
-    <row r="58" spans="1:6" s="9" customFormat="1" ht="45">
-      <c r="A58" s="9" t="s">
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+    </row>
+    <row r="59" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="A59" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B58" s="16"/>
-      <c r="C58" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="9" customFormat="1" ht="45">
       <c r="B59" s="16"/>
       <c r="C59" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D59" s="7"/>
-      <c r="E59" s="7">
-        <v>6407</v>
+      <c r="E59" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="9" customFormat="1" ht="45">
       <c r="B60" s="16"/>
       <c r="C60" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7">
+        <v>6407</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="B61" s="16"/>
+      <c r="C61" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7" t="s">
+      <c r="D61" s="7"/>
+      <c r="E61" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F60" s="6" t="s">
+      <c r="F61" s="6" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C61" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C62" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C63" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C64" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E63" s="19" t="s">
+      <c r="E64" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="F64" s="6" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C64" s="19" t="s">
+    <row r="65" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C65" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E64" s="19">
+      <c r="E65" s="19">
         <v>63412</v>
       </c>
-      <c r="F64" s="19" t="s">
+      <c r="F65" s="19" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="19" customFormat="1">
-      <c r="B65" s="14" t="s">
+    <row r="66" spans="1:6" s="19" customFormat="1">
+      <c r="B66" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="15"/>
-    </row>
-    <row r="66" spans="1:6" s="22" customFormat="1" ht="45">
-      <c r="C66" s="24" t="s">
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+    </row>
+    <row r="67" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="C67" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D66" s="22" t="s">
+      <c r="D67" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E66" s="25">
+      <c r="E67" s="24">
         <v>41133</v>
       </c>
-      <c r="F66" s="26" t="s">
+      <c r="F67" s="25" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
-      <c r="C67" s="7" t="s">
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
+      <c r="C68" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E67" s="19">
+      <c r="E68" s="19">
         <v>5000</v>
       </c>
-      <c r="F67" s="6" t="s">
+      <c r="F68" s="6" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C68" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E68" s="13">
-        <v>40767</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C69" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E69" s="13">
+        <v>40767</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C70" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E69" s="19">
+      <c r="E70" s="19">
         <v>659056746</v>
       </c>
-      <c r="F69" s="6" t="s">
+      <c r="F70" s="6" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="22" customFormat="1" ht="45">
-      <c r="C70" s="24" t="s">
+    <row r="71" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="C71" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E70" s="22" t="s">
+      <c r="E71" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="F70" s="26" t="s">
+      <c r="F71" s="25" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A71" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D71" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E71" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="60">
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="A72" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C72" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E72" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="60">
+      <c r="A73" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C73" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D72" s="19" t="s">
+      <c r="D73" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E72" s="19" t="s">
+      <c r="E73" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F72" s="6" t="s">
+      <c r="F73" s="6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C73" s="6" t="s">
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C74" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D73" s="19" t="s">
+      <c r="D74" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E73" s="19">
+      <c r="E74" s="19">
         <v>758075800</v>
       </c>
-      <c r="F73" s="6" t="s">
+      <c r="F74" s="6" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A74" s="20" t="s">
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A75" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B74" s="20"/>
-      <c r="C74" s="6" t="s">
+      <c r="B75" s="20"/>
+      <c r="C75" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D74" s="20" t="s">
+      <c r="D75" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="E74" s="19" t="s">
+      <c r="E75" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="F74" s="6" t="s">
+      <c r="F75" s="6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C75" s="19" t="s">
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C76" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D75" s="19" t="s">
+      <c r="D76" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E75" s="19" t="s">
+      <c r="E76" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F75" s="19" t="s">
+      <c r="F76" s="19" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A76" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F76" s="19" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4263,90 +4266,107 @@
       </c>
       <c r="B77" s="9"/>
       <c r="C77" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E77" s="9">
-        <v>500</v>
+        <v>118</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="A78" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="B78" s="9"/>
+      <c r="C78" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E78" s="9">
+        <v>500</v>
+      </c>
+      <c r="F78" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A79" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C79" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D78" s="19" t="s">
+      <c r="D79" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E78" s="19" t="s">
+      <c r="E79" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="F78" s="19" t="s">
+      <c r="F79" s="19" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C79" s="20" t="s">
+    <row r="80" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C80" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="D79" s="20" t="s">
+      <c r="D80" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="E79" s="19" t="s">
+      <c r="E80" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="F79" s="20" t="s">
+      <c r="F80" s="20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="A80" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="F80" s="20" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="22" customFormat="1" ht="45">
+    <row r="81" spans="1:6" s="20" customFormat="1" ht="45">
       <c r="A81" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C81" s="20" t="s">
+      <c r="B81" s="9"/>
+      <c r="C81" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="F81" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="A82" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C82" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="D81" s="20" t="s">
+      <c r="D82" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="E81" s="20" t="s">
+      <c r="E82" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="F81" s="20" t="s">
+      <c r="F82" s="20" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="19" customFormat="1">
-      <c r="B82" s="22"/>
-    </row>
-    <row r="83" spans="1:6" s="19" customFormat="1"/>
+    <row r="83" spans="1:6" s="19" customFormat="1">
+      <c r="B83" s="22"/>
+    </row>
     <row r="84" spans="1:6" s="19" customFormat="1"/>
-    <row r="284" hidden="1"/>
+    <row r="85" spans="1:6" s="19" customFormat="1"/>
     <row r="285" hidden="1"/>
     <row r="286" hidden="1"/>
     <row r="287" hidden="1"/>
@@ -4360,6 +4380,7 @@
     <row r="295" hidden="1"/>
     <row r="296" hidden="1"/>
     <row r="297" hidden="1"/>
+    <row r="298" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4397,10 +4418,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>

</xml_diff>

<commit_message>
Added Vehicle Registration Non-Expiring Indicator
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="1280" windowWidth="31340" windowHeight="15080" tabRatio="500"/>
+    <workbookView xWindow="6000" yWindow="1284" windowWidth="19416" windowHeight="11016" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="263">
   <si>
     <t>CLASS</t>
   </si>
@@ -801,6 +801,15 @@
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/j:ConveyanceRegistration[@structures:id=/wir-doc:WarrantIssuedReport/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:JurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>Vehicle Registration Non-Expiring Indicator</t>
+  </si>
+  <si>
+    <t>True if vehicle registration is non-expiring</t>
+  </si>
+  <si>
+    <t>/wir-doc:WarrantIssuedReport/j:ConveyanceRegistration[not(j:RegistrationExpirationDate)]/wir-ext:ConveyanceRegistrationNonExpiringIndicator</t>
   </si>
 </sst>
 </file>
@@ -3242,25 +3251,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F298"/>
+  <dimension ref="A1:F299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.19921875" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="28.296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.296875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23" customHeight="1">
+    <row r="1" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>53</v>
@@ -3270,7 +3279,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -3290,7 +3299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="19" customFormat="1">
+    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>66</v>
       </c>
@@ -3299,7 +3308,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" s="19" customFormat="1">
+    <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>41</v>
       </c>
@@ -3310,7 +3319,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="19" customFormat="1">
+    <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>43</v>
       </c>
@@ -3324,7 +3333,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="19" customFormat="1" ht="30">
+    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>37</v>
       </c>
@@ -3341,7 +3350,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="19" customFormat="1">
+    <row r="7" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>37</v>
       </c>
@@ -3358,7 +3367,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="19" customFormat="1">
+    <row r="8" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>37</v>
       </c>
@@ -3375,7 +3384,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="22" customFormat="1">
+    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>37</v>
       </c>
@@ -3392,7 +3401,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="22" customFormat="1">
+    <row r="10" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>37</v>
       </c>
@@ -3410,7 +3419,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="19" customFormat="1">
+    <row r="11" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
@@ -3419,7 +3428,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" s="19" customFormat="1">
+    <row r="12" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -3434,7 +3443,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="19" customFormat="1">
+    <row r="13" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="19" t="s">
         <v>10</v>
@@ -3447,7 +3456,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="19" customFormat="1">
+    <row r="14" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
       <c r="C14" s="19" t="s">
         <v>11</v>
@@ -3460,7 +3469,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="19" customFormat="1">
+    <row r="15" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="19" t="s">
         <v>12</v>
@@ -3473,7 +3482,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="19" customFormat="1">
+    <row r="16" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
       <c r="C16" s="19" t="s">
         <v>25</v>
@@ -3486,7 +3495,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="17" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -3501,7 +3510,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="18" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>10</v>
@@ -3514,7 +3523,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="19" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>11</v>
@@ -3527,7 +3536,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="20" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="19" t="s">
         <v>12</v>
@@ -3540,7 +3549,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B21" s="6"/>
       <c r="C21" s="19" t="s">
         <v>25</v>
@@ -3553,7 +3562,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="19" customFormat="1">
+    <row r="22" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
@@ -3570,7 +3579,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
         <v>207</v>
@@ -3582,7 +3591,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
+    <row r="24" spans="1:6" s="20" customFormat="1" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>37</v>
       </c>
@@ -3600,7 +3609,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
+    <row r="25" spans="1:6" s="19" customFormat="1" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
         <v>4</v>
@@ -3613,7 +3622,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="20" customFormat="1">
+    <row r="26" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
         <v>221</v>
@@ -3626,7 +3635,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="19" customFormat="1">
+    <row r="27" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
         <v>226</v>
@@ -3638,7 +3647,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="19" customFormat="1">
+    <row r="28" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
         <v>227</v>
@@ -3650,7 +3659,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="19" customFormat="1">
+    <row r="29" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
         <v>121</v>
@@ -3662,7 +3671,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="19" customFormat="1">
+    <row r="30" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
         <v>228</v>
@@ -3674,7 +3683,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="19" customFormat="1">
+    <row r="31" spans="1:6" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
@@ -3687,7 +3696,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="19" customFormat="1">
+    <row r="32" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>177</v>
@@ -3700,7 +3709,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="19" customFormat="1">
+    <row r="33" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>122</v>
@@ -3712,7 +3721,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="19" customFormat="1">
+    <row r="34" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
         <v>123</v>
@@ -3724,7 +3733,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="19" customFormat="1">
+    <row r="35" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
         <v>21</v>
@@ -3737,7 +3746,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="19" customFormat="1">
+    <row r="36" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
         <v>22</v>
@@ -3750,7 +3759,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="19" customFormat="1">
+    <row r="37" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
         <v>23</v>
@@ -3763,7 +3772,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="19" customFormat="1">
+    <row r="38" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
         <v>24</v>
@@ -3776,7 +3785,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="19" customFormat="1">
+    <row r="39" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
         <v>124</v>
@@ -3788,7 +3797,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="19" customFormat="1">
+    <row r="40" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
         <v>229</v>
@@ -3800,7 +3809,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="19" customFormat="1">
+    <row r="41" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
         <v>6</v>
@@ -3813,7 +3822,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="45">
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
         <v>37</v>
       </c>
@@ -3831,7 +3840,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="19" customFormat="1">
+    <row r="43" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="19" t="s">
         <v>37</v>
       </c>
@@ -3849,7 +3858,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B44" s="6" t="s">
         <v>17</v>
       </c>
@@ -3864,7 +3873,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="s">
         <v>19</v>
@@ -3879,7 +3888,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="19" customFormat="1">
+    <row r="46" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="14" t="s">
         <v>26</v>
       </c>
@@ -3888,7 +3897,7 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
     </row>
-    <row r="47" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C47" s="7" t="s">
         <v>27</v>
       </c>
@@ -3899,7 +3908,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="48" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C48" s="7" t="s">
         <v>68</v>
       </c>
@@ -3910,7 +3919,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="49" spans="1:6" s="20" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="7" t="s">
         <v>224</v>
       </c>
@@ -3921,473 +3930,487 @@
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="50" spans="1:6" s="20" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="E50" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="20" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E51" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F51" s="6" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C51" s="7" t="s">
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C52" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E51" s="19" t="s">
+      <c r="E52" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="F52" s="6" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C52" s="7" t="s">
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C53" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E52" s="19" t="s">
+      <c r="E53" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="F53" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C53" s="7" t="s">
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C54" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="19" t="s">
+      <c r="E54" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F54" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C54" s="7" t="s">
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C55" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C55" s="7" t="s">
-        <v>233</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>180</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>184</v>
+        <v>104</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="19" customFormat="1" ht="30">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C56" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>180</v>
       </c>
       <c r="E56" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C57" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F56" s="6" t="s">
+      <c r="F57" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C57" s="7" t="s">
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C58" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E57" s="19">
+      <c r="E58" s="19">
         <v>2012</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="F58" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="30">
-      <c r="B58" s="14" t="s">
+    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B59" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-    </row>
-    <row r="59" spans="1:6" s="9" customFormat="1" ht="45">
-      <c r="A59" s="9" t="s">
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+    </row>
+    <row r="60" spans="1:6" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="9" customFormat="1" ht="45">
       <c r="B60" s="16"/>
       <c r="C60" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D60" s="7"/>
-      <c r="E60" s="7">
-        <v>6407</v>
+      <c r="E60" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="9" customFormat="1" ht="45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B61" s="16"/>
       <c r="C61" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7">
+        <v>6407</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B62" s="16"/>
+      <c r="C62" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7" t="s">
+      <c r="D62" s="7"/>
+      <c r="E62" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F61" s="6" t="s">
+      <c r="F62" s="6" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C62" s="7" t="s">
+    <row r="63" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C63" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E62" s="19" t="s">
+      <c r="E63" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="F62" s="6" t="s">
+      <c r="F63" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C63" s="7" t="s">
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C64" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E63" s="19" t="s">
+      <c r="E64" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="F64" s="6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C64" s="7" t="s">
+    <row r="65" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C65" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E65" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F64" s="6" t="s">
+      <c r="F65" s="6" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C65" s="19" t="s">
+    <row r="66" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C66" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E65" s="19">
+      <c r="E66" s="19">
         <v>63412</v>
       </c>
-      <c r="F65" s="19" t="s">
+      <c r="F66" s="19" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="19" customFormat="1">
-      <c r="B66" s="14" t="s">
+    <row r="67" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-    </row>
-    <row r="67" spans="1:6" s="22" customFormat="1" ht="45">
-      <c r="C67" s="23" t="s">
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+    </row>
+    <row r="68" spans="1:6" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C68" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="22" t="s">
+      <c r="D68" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E67" s="24">
+      <c r="E68" s="24">
         <v>41133</v>
       </c>
-      <c r="F67" s="25" t="s">
+      <c r="F68" s="25" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
-      <c r="C68" s="7" t="s">
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E68" s="19">
+      <c r="E69" s="19">
         <v>5000</v>
       </c>
-      <c r="F68" s="6" t="s">
+      <c r="F69" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C69" s="7" t="s">
+    <row r="70" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C70" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E69" s="13">
+      <c r="E70" s="13">
         <v>40767</v>
       </c>
-      <c r="F69" s="6" t="s">
+      <c r="F70" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C70" s="7" t="s">
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C71" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E70" s="19">
+      <c r="E71" s="19">
         <v>659056746</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="F71" s="6" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="22" customFormat="1" ht="45">
-      <c r="C71" s="23" t="s">
+    <row r="72" spans="1:6" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C72" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E71" s="22" t="s">
+      <c r="E72" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="F71" s="25" t="s">
+      <c r="F72" s="25" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A72" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D72" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E72" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="60">
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A73" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C73" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E73" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A74" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C74" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D73" s="19" t="s">
+      <c r="D74" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E73" s="19" t="s">
+      <c r="E74" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F73" s="6" t="s">
+      <c r="F74" s="6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C74" s="6" t="s">
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C75" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D74" s="19" t="s">
+      <c r="D75" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E74" s="19">
+      <c r="E75" s="19">
         <v>758075800</v>
       </c>
-      <c r="F74" s="6" t="s">
+      <c r="F75" s="6" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A75" s="20" t="s">
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B75" s="20"/>
-      <c r="C75" s="6" t="s">
+      <c r="B76" s="20"/>
+      <c r="C76" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D75" s="20" t="s">
+      <c r="D76" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="E75" s="19" t="s">
+      <c r="E76" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="F75" s="6" t="s">
+      <c r="F76" s="6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C76" s="19" t="s">
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C77" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="D77" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E76" s="19" t="s">
+      <c r="E77" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F76" s="19" t="s">
+      <c r="F77" s="19" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="A77" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F77" s="19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A78" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B78" s="9"/>
       <c r="C78" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E78" s="9">
-        <v>500</v>
+        <v>118</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A79" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="B79" s="9"/>
+      <c r="C79" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E79" s="9">
+        <v>500</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A80" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C80" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D79" s="19" t="s">
+      <c r="D80" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E79" s="19" t="s">
+      <c r="E80" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="F79" s="19" t="s">
+      <c r="F80" s="19" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="19" customFormat="1" ht="45">
-      <c r="C80" s="20" t="s">
+    <row r="81" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C81" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="D80" s="20" t="s">
+      <c r="D81" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="E80" s="19" t="s">
+      <c r="E81" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="F80" s="20" t="s">
+      <c r="F81" s="20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="A81" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="F81" s="20" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="22" customFormat="1" ht="45">
+    <row r="82" spans="1:6" s="20" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A82" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C82" s="20" t="s">
+      <c r="B82" s="9"/>
+      <c r="C82" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="F82" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A83" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C83" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="D82" s="20" t="s">
+      <c r="D83" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="E82" s="20" t="s">
+      <c r="E83" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="F82" s="20" t="s">
+      <c r="F83" s="20" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="19" customFormat="1">
-      <c r="B83" s="22"/>
-    </row>
-    <row r="84" spans="1:6" s="19" customFormat="1"/>
-    <row r="85" spans="1:6" s="19" customFormat="1"/>
-    <row r="285" hidden="1"/>
-    <row r="286" hidden="1"/>
-    <row r="287" hidden="1"/>
-    <row r="288" hidden="1"/>
-    <row r="289" hidden="1"/>
-    <row r="290" hidden="1"/>
-    <row r="291" hidden="1"/>
-    <row r="292" hidden="1"/>
-    <row r="293" hidden="1"/>
-    <row r="294" hidden="1"/>
-    <row r="295" hidden="1"/>
-    <row r="296" hidden="1"/>
-    <row r="297" hidden="1"/>
-    <row r="298" hidden="1"/>
+    <row r="84" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="22"/>
+    </row>
+    <row r="85" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="1:6" s="19" customFormat="1" ht="409.6" x14ac:dyDescent="0"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="289" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="290" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="291" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="292" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="293" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="294" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="295" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="296" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="297" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="298" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="299" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4404,19 +4427,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="13.69921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.19921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.296875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.69921875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23" customHeight="1">
+    <row r="1" spans="1:7" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>52</v>
@@ -4427,7 +4450,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -4450,7 +4473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -4461,7 +4484,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4476,7 +4499,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="5" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
       <c r="C5" s="19" t="s">
         <v>10</v>
@@ -4489,7 +4512,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="6" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
       <c r="C6" s="19" t="s">
         <v>11</v>
@@ -4502,7 +4525,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="7" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
@@ -4515,7 +4538,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="8" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4529,7 +4552,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
         <v>227</v>
@@ -4543,7 +4566,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="10" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
         <v>228</v>
@@ -4557,7 +4580,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" s="20" customFormat="1" ht="53" customHeight="1">
+    <row r="11" spans="1:7" s="20" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>37</v>
       </c>
@@ -4576,7 +4599,7 @@
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>38</v>
@@ -4587,7 +4610,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
@@ -4601,7 +4624,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C14" s="6" t="s">
         <v>181</v>
       </c>
@@ -4615,7 +4638,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
         <v>70</v>
@@ -4630,7 +4653,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="19" customFormat="1">
+    <row r="16" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C16" s="20" t="s">
         <v>192</v>
       </c>
@@ -4638,230 +4661,230 @@
         <v>255</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="19" customFormat="1"/>
-    <row r="18" spans="1:1" s="19" customFormat="1"/>
-    <row r="19" spans="1:1" s="19" customFormat="1"/>
-    <row r="20" spans="1:1" s="19" customFormat="1"/>
-    <row r="21" spans="1:1" s="19" customFormat="1"/>
-    <row r="22" spans="1:1" s="19" customFormat="1"/>
-    <row r="23" spans="1:1">
+    <row r="17" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="19"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="19"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="19"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="19"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="19"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="19"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="19"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="19"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="19"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="19"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="19"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="19"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="19"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="19"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="19"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="19"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="19"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="19"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="19"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="19"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="19"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="19"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="19"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="19"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="19"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="19"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="19"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="19"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="19"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="19"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="19"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="19"/>
     </row>
   </sheetData>
@@ -4886,7 +4909,7 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Replaced “Person Entry Number" in the Warrant Accepted Report with "State Warrant Repository ID".
Replaced "Person Record Identification ID” in the Warrant Modification
Request” with "State Warrant Repository ID”.

See corresponding mapping spreadsheets.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="1284" windowWidth="19416" windowHeight="11016" tabRatio="500"/>
+    <workbookView xWindow="4660" yWindow="3540" windowWidth="28420" windowHeight="13760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -635,12 +635,6 @@
     <t>PS-123456</t>
   </si>
   <si>
-    <t>Person Entry Number</t>
-  </si>
-  <si>
-    <t>A miscellaneous unique identification assigned to a person record</t>
-  </si>
-  <si>
     <t>PE45678</t>
   </si>
   <si>
@@ -650,9 +644,6 @@
     <t>True if a person query should include the DHS ICE Database; false otherwise</t>
   </si>
   <si>
-    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/wir-ext:PersonEntryNumber/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonUSCitizenIndicator</t>
   </si>
   <si>
@@ -810,6 +801,15 @@
   </si>
   <si>
     <t>/wir-doc:WarrantIssuedReport/j:ConveyanceRegistration[not(j:RegistrationExpirationDate)]/wir-ext:ConveyanceRegistrationNonExpiringIndicator</t>
+  </si>
+  <si>
+    <t>A unique identification assigned to a warrant record.</t>
+  </si>
+  <si>
+    <t>StateWarrantRepositoryIdentification</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/j:Warrant/wir-ext:WarrantAugmentation/wir-ext:StateWarrantRepositoryIdentification/nc:IdentificationID/#text</t>
   </si>
 </sst>
 </file>
@@ -938,9 +938,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="948">
+  <cellStyleXfs count="950">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1969,7 +1971,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="948">
+  <cellStyles count="950">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2443,6 +2445,7 @@
     <cellStyle name="Followed Hyperlink" xfId="943" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="945" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="947" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="949" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2916,6 +2919,7 @@
     <cellStyle name="Hyperlink" xfId="942" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="944" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="946" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="948" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3253,23 +3257,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.19921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.296875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.796875" style="2"/>
+    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>53</v>
@@ -3279,7 +3283,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -3299,7 +3303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
         <v>66</v>
       </c>
@@ -3308,7 +3312,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="19" customFormat="1">
       <c r="C4" s="7" t="s">
         <v>41</v>
       </c>
@@ -3319,7 +3323,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="19" customFormat="1">
       <c r="C5" s="7" t="s">
         <v>43</v>
       </c>
@@ -3333,24 +3337,24 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.25">
       <c r="A6" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>73</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="19" customFormat="1">
       <c r="A7" s="19" t="s">
         <v>37</v>
       </c>
@@ -3367,7 +3371,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="19" customFormat="1">
       <c r="A8" s="19" t="s">
         <v>37</v>
       </c>
@@ -3384,24 +3388,24 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.25">
       <c r="A9" s="22" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="F9" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="D9" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" s="22" customFormat="1">
       <c r="A10" s="22" t="s">
         <v>37</v>
       </c>
@@ -3410,16 +3414,16 @@
         <v>175</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>115</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="19" customFormat="1">
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
@@ -3428,7 +3432,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="19" customFormat="1">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -3443,7 +3447,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="19" customFormat="1">
       <c r="B13" s="6"/>
       <c r="C13" s="19" t="s">
         <v>10</v>
@@ -3456,7 +3460,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="19" customFormat="1">
       <c r="B14" s="6"/>
       <c r="C14" s="19" t="s">
         <v>11</v>
@@ -3469,7 +3473,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="19" customFormat="1">
       <c r="B15" s="6"/>
       <c r="C15" s="19" t="s">
         <v>12</v>
@@ -3482,7 +3486,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="19" customFormat="1">
       <c r="B16" s="6"/>
       <c r="C16" s="19" t="s">
         <v>25</v>
@@ -3495,7 +3499,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -3510,7 +3514,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>10</v>
@@ -3523,7 +3527,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>11</v>
@@ -3536,7 +3540,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="B20" s="6"/>
       <c r="C20" s="19" t="s">
         <v>12</v>
@@ -3549,7 +3553,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="B21" s="6"/>
       <c r="C21" s="19" t="s">
         <v>25</v>
@@ -3562,12 +3566,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="19" customFormat="1">
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>176</v>
@@ -3576,40 +3580,40 @@
         <v>85</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="20" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E23" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="20" customFormat="1" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
       <c r="A24" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E24" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="19" customFormat="1" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
         <v>4</v>
@@ -3622,44 +3626,44 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="20" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>86</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>92</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
         <v>121</v>
@@ -3671,19 +3675,19 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>93</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="19" customFormat="1" ht="31.25">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
@@ -3696,7 +3700,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>177</v>
@@ -3709,7 +3713,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="19" customFormat="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>122</v>
@@ -3721,7 +3725,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="19" customFormat="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
         <v>123</v>
@@ -3733,7 +3737,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="19" customFormat="1">
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
         <v>21</v>
@@ -3746,7 +3750,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="19" customFormat="1">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
         <v>22</v>
@@ -3759,7 +3763,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="19" customFormat="1">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
         <v>23</v>
@@ -3772,7 +3776,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" s="19" customFormat="1">
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
         <v>24</v>
@@ -3785,7 +3789,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" s="19" customFormat="1">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
         <v>124</v>
@@ -3797,19 +3801,19 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" s="19" customFormat="1">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>95</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="19" customFormat="1">
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
         <v>6</v>
@@ -3822,13 +3826,13 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="46.75">
       <c r="A42" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>202</v>
@@ -3837,28 +3841,28 @@
         <v>203</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="19" customFormat="1">
       <c r="A43" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="B44" s="6" t="s">
         <v>17</v>
       </c>
@@ -3873,7 +3877,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="s">
         <v>19</v>
@@ -3888,7 +3892,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" s="19" customFormat="1">
       <c r="B46" s="14" t="s">
         <v>26</v>
       </c>
@@ -3897,7 +3901,7 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
     </row>
-    <row r="47" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C47" s="7" t="s">
         <v>27</v>
       </c>
@@ -3908,7 +3912,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C48" s="7" t="s">
         <v>68</v>
       </c>
@@ -3919,43 +3923,43 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="20" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C49" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="20" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C50" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E50" s="20" t="b">
         <v>1</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="20" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C51" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E51" s="20" t="s">
         <v>97</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C52" s="7" t="s">
         <v>119</v>
       </c>
@@ -3963,10 +3967,10 @@
         <v>100</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C53" s="7" t="s">
         <v>120</v>
       </c>
@@ -3974,10 +3978,10 @@
         <v>101</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C54" s="7" t="s">
         <v>28</v>
       </c>
@@ -3988,9 +3992,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C55" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>180</v>
@@ -3999,12 +4003,12 @@
         <v>104</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C56" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>180</v>
@@ -4013,12 +4017,12 @@
         <v>184</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C57" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D57" s="19" t="s">
         <v>180</v>
@@ -4027,10 +4031,10 @@
         <v>102</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C58" s="7" t="s">
         <v>29</v>
       </c>
@@ -4041,7 +4045,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.25">
       <c r="B59" s="14" t="s">
         <v>49</v>
       </c>
@@ -4050,7 +4054,7 @@
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
     </row>
-    <row r="60" spans="1:6" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" s="9" customFormat="1" ht="46.75">
       <c r="A60" s="9" t="s">
         <v>37</v>
       </c>
@@ -4066,7 +4070,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" s="9" customFormat="1" ht="46.75">
       <c r="B61" s="16"/>
       <c r="C61" s="7" t="s">
         <v>34</v>
@@ -4079,7 +4083,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" s="9" customFormat="1" ht="46.75">
       <c r="B62" s="16"/>
       <c r="C62" s="7" t="s">
         <v>35</v>
@@ -4089,10 +4093,10 @@
         <v>108</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C63" s="7" t="s">
         <v>30</v>
       </c>
@@ -4103,7 +4107,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C64" s="7" t="s">
         <v>32</v>
       </c>
@@ -4114,7 +4118,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C65" s="7" t="s">
         <v>31</v>
       </c>
@@ -4125,7 +4129,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C66" s="19" t="s">
         <v>36</v>
       </c>
@@ -4136,7 +4140,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" s="19" customFormat="1">
       <c r="B67" s="14" t="s">
         <v>38</v>
       </c>
@@ -4145,7 +4149,7 @@
       <c r="E67" s="15"/>
       <c r="F67" s="15"/>
     </row>
-    <row r="68" spans="1:6" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" s="22" customFormat="1" ht="46.75">
       <c r="C68" s="23" t="s">
         <v>39</v>
       </c>
@@ -4159,7 +4163,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
       <c r="C69" s="7" t="s">
         <v>56</v>
       </c>
@@ -4170,7 +4174,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C70" s="7" t="s">
         <v>45</v>
       </c>
@@ -4181,7 +4185,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C71" s="7" t="s">
         <v>42</v>
       </c>
@@ -4192,7 +4196,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" s="22" customFormat="1" ht="46.75">
       <c r="C72" s="23" t="s">
         <v>57</v>
       </c>
@@ -4203,7 +4207,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="A73" s="19" t="s">
         <v>37</v>
       </c>
@@ -4220,7 +4224,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="62.5">
       <c r="A74" s="19" t="s">
         <v>37</v>
       </c>
@@ -4237,7 +4241,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C75" s="6" t="s">
         <v>46</v>
       </c>
@@ -4251,7 +4255,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="A76" s="20" t="s">
         <v>37</v>
       </c>
@@ -4269,7 +4273,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C77" s="19" t="s">
         <v>70</v>
       </c>
@@ -4283,7 +4287,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="A78" s="19" t="s">
         <v>37</v>
       </c>
@@ -4301,7 +4305,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="A79" s="19" t="s">
         <v>37</v>
       </c>
@@ -4319,7 +4323,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="A80" s="19" t="s">
         <v>37</v>
       </c>
@@ -4336,7 +4340,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" s="19" customFormat="1" ht="46.75">
       <c r="C81" s="20" t="s">
         <v>178</v>
       </c>
@@ -4350,13 +4354,13 @@
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="20" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" s="20" customFormat="1" ht="46.75">
       <c r="A82" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>190</v>
@@ -4365,10 +4369,10 @@
         <v>191</v>
       </c>
       <c r="F82" s="20" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="22" customFormat="1" ht="46.75">
       <c r="A83" s="20" t="s">
         <v>37</v>
       </c>
@@ -4382,35 +4386,35 @@
         <v>194</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="19" customFormat="1">
       <c r="B84" s="22"/>
     </row>
-    <row r="85" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" spans="1:6" s="19" customFormat="1" ht="409.6" x14ac:dyDescent="0"/>
-    <row r="286" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="287" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="288" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="289" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="290" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="291" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="292" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="293" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="294" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="295" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="296" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="297" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="298" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="299" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:6" s="19" customFormat="1"/>
+    <row r="86" spans="1:6" s="19" customFormat="1" ht="409.5"/>
+    <row r="286" ht="15.5" hidden="1"/>
+    <row r="287" ht="15.5" hidden="1"/>
+    <row r="288" ht="15.5" hidden="1"/>
+    <row r="289" ht="15.5" hidden="1"/>
+    <row r="290" ht="15.5" hidden="1"/>
+    <row r="291" ht="15.5" hidden="1"/>
+    <row r="292" ht="15.5" hidden="1"/>
+    <row r="293" ht="15.5" hidden="1"/>
+    <row r="294" ht="15.5" hidden="1"/>
+    <row r="295" ht="15.5" hidden="1"/>
+    <row r="296" ht="15.5" hidden="1"/>
+    <row r="297" ht="15.5" hidden="1"/>
+    <row r="298" ht="15.5" hidden="1"/>
+    <row r="299" ht="15.5" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4423,23 +4427,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.69921875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.19921875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.296875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.69921875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.796875" style="2"/>
+    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>52</v>
@@ -4450,7 +4454,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -4473,7 +4477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -4484,7 +4488,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="46.75">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4499,7 +4503,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="19" customFormat="1" ht="46.75">
       <c r="B5" s="6"/>
       <c r="C5" s="19" t="s">
         <v>10</v>
@@ -4512,7 +4516,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="19" customFormat="1" ht="46.75">
       <c r="B6" s="6"/>
       <c r="C6" s="19" t="s">
         <v>11</v>
@@ -4525,7 +4529,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="19" customFormat="1" ht="46.75">
       <c r="B7" s="6"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
@@ -4538,7 +4542,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="19" customFormat="1" ht="46.75">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4552,54 +4556,35 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="46.75">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
         <v>92</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="19" customFormat="1" ht="46.75">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
         <v>93</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" s="20" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>38</v>
@@ -4610,7 +4595,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="46.75">
       <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
@@ -4624,7 +4609,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.25">
       <c r="C14" s="6" t="s">
         <v>181</v>
       </c>
@@ -4638,7 +4623,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.25">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
         <v>70</v>
@@ -4653,238 +4638,261 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="19" customFormat="1">
       <c r="C16" s="20" t="s">
         <v>192</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="20" customFormat="1" ht="34" customHeight="1">
+      <c r="A17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" s="19" customFormat="1">
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="1:7" s="19" customFormat="1"/>
+    <row r="20" spans="1:7" s="19" customFormat="1"/>
+    <row r="21" spans="1:7" s="19" customFormat="1"/>
+    <row r="22" spans="1:7" s="19" customFormat="1"/>
+    <row r="23" spans="1:7">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27" s="19"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" s="19"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29" s="19"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30" s="19"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31" s="19"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32" s="19"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1">
       <c r="A33" s="19"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1">
       <c r="A34" s="19"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1">
       <c r="A35" s="19"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1">
       <c r="A36" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1">
       <c r="A37" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1">
       <c r="A38" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1">
       <c r="A39" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1">
       <c r="A40" s="19"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1">
       <c r="A41" s="19"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1">
       <c r="A42" s="19"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1">
       <c r="A43" s="19"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1">
       <c r="A44" s="19"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1">
       <c r="A45" s="19"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1">
       <c r="A46" s="19"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1">
       <c r="A47" s="19"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1">
       <c r="A48" s="19"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1">
       <c r="A49" s="19"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1">
       <c r="A50" s="19"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1">
       <c r="A51" s="19"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1">
       <c r="A52" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1">
       <c r="A53" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1">
       <c r="A54" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1">
       <c r="A55" s="19"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1">
       <c r="A56" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1">
       <c r="A57" s="9"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1">
       <c r="A58" s="9"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1">
       <c r="A59" s="19"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1">
       <c r="A60" s="19"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1">
       <c r="A61" s="19"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1">
       <c r="A62" s="19"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1">
       <c r="A63" s="19"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1">
       <c r="A64" s="19"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1">
       <c r="A65" s="19"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1">
       <c r="A66" s="19"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1">
       <c r="A67" s="19"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1">
       <c r="A68" s="19"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1">
       <c r="A69" s="19"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1">
       <c r="A70" s="19"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1">
       <c r="A71" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1">
       <c r="A72" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1">
       <c r="A73" s="19"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1">
       <c r="A74" s="19"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1">
       <c r="A75" s="19"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1">
       <c r="A76" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1">
       <c r="A77" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1">
       <c r="A78" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1">
       <c r="A79" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1">
       <c r="A80" s="19"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1">
       <c r="A81" s="19"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1">
       <c r="A82" s="19"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1">
       <c r="A83" s="19"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1">
       <c r="A84" s="19"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1">
       <c r="A85" s="19"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1">
       <c r="A86" s="19"/>
     </row>
   </sheetData>
@@ -4909,7 +4917,7 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Removed nc:AddressFullText; nc:StreetNumberText and nc:StreetName
Added nc:StreetFullText
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="3540" windowWidth="28420" windowHeight="13760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4440" yWindow="2940" windowWidth="28420" windowHeight="13760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="258">
   <si>
     <t>CLASS</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Vehicle Year</t>
   </si>
   <si>
-    <t>Address Full Text</t>
-  </si>
-  <si>
     <t>Address State Name</t>
   </si>
   <si>
@@ -125,12 +122,6 @@
     <t>Address Category Text</t>
   </si>
   <si>
-    <t>Street Number Text</t>
-  </si>
-  <si>
-    <t>Street Name</t>
-  </si>
-  <si>
     <t>Zip Code</t>
   </si>
   <si>
@@ -344,12 +335,6 @@
     <t>LP-category</t>
   </si>
   <si>
-    <t>Full Address</t>
-  </si>
-  <si>
-    <t>Cedar Ave</t>
-  </si>
-  <si>
     <t>Mail</t>
   </si>
   <si>
@@ -491,15 +476,9 @@
     <t>wir-doc:WarrantIssuedReport/nc:Case/j:CaseAugmentation/j:CaseCharge/wir-ext:OriginalOffenseCodeText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:AddressFullText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/wir-ext:AddressCategoryText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStreet/nc:StreetNumberText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationCityName</t>
   </si>
   <si>
@@ -767,9 +746,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorSecondaryText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStreet/nc:StreetName</t>
-  </si>
-  <si>
     <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonRaceText</t>
   </si>
   <si>
@@ -810,6 +786,15 @@
   </si>
   <si>
     <t>war-doc:WarrantAcceptedReport/j:Warrant/wir-ext:WarrantAugmentation/wir-ext:StateWarrantRepositoryIdentification/nc:IdentificationID/#text</t>
+  </si>
+  <si>
+    <t>Street Full Text</t>
+  </si>
+  <si>
+    <t>6407 Cedar Ave</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStreet/nc:StreetFullText</t>
   </si>
 </sst>
 </file>
@@ -3255,11 +3240,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F299"/>
+  <dimension ref="A1:F297"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3276,7 +3261,7 @@
     <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="10"/>
@@ -3285,7 +3270,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -3305,7 +3290,7 @@
     </row>
     <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -3314,113 +3299,113 @@
     </row>
     <row r="4" spans="1:6" s="19" customFormat="1">
       <c r="C4" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="19" customFormat="1">
       <c r="C5" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="19" customFormat="1" ht="30">
       <c r="A6" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="19" customFormat="1">
       <c r="A7" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="19" customFormat="1">
       <c r="A8" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="22" customFormat="1">
       <c r="A9" s="22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="22" customFormat="1">
       <c r="A10" s="22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="21" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="19" customFormat="1">
@@ -3441,10 +3426,10 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="19" customFormat="1">
@@ -3454,10 +3439,10 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="19" customFormat="1">
@@ -3467,10 +3452,10 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="19" customFormat="1">
@@ -3480,10 +3465,10 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="19" customFormat="1">
@@ -3493,13 +3478,13 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -3508,62 +3493,62 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B20" s="6"/>
       <c r="C20" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B21" s="6"/>
       <c r="C21" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="19" customFormat="1">
@@ -3571,46 +3556,46 @@
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E23" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
       <c r="A24" s="20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E24" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
@@ -3623,71 +3608,71 @@
         <v>23235</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="20" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="19" customFormat="1" ht="31.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="19" customFormat="1">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
@@ -3697,44 +3682,44 @@
         <v>354786908</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="19" customFormat="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="19" customFormat="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="19" customFormat="1">
@@ -3747,7 +3732,7 @@
         <v>71</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="19" customFormat="1">
@@ -3757,10 +3742,10 @@
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="19" customFormat="1">
@@ -3773,7 +3758,7 @@
         <v>165</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="19" customFormat="1">
@@ -3783,34 +3768,34 @@
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="19" customFormat="1">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="19" customFormat="1">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="19" customFormat="1">
@@ -3823,46 +3808,46 @@
         <v>98213455</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="46.75">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="45">
       <c r="A42" s="20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="19" customFormat="1">
       <c r="A43" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B44" s="6" t="s">
         <v>17</v>
       </c>
@@ -3871,13 +3856,13 @@
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="s">
         <v>19</v>
@@ -3886,10 +3871,10 @@
         <v>20</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="19" customFormat="1">
@@ -3901,140 +3886,140 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
     </row>
-    <row r="47" spans="1:6" s="19" customFormat="1" ht="46.75">
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C47" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C48" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C49" s="7" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C50" s="7" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E50" s="20" t="b">
         <v>1</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C51" s="7" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="E51" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C52" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E52" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="C52" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>100</v>
-      </c>
       <c r="F52" s="6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C53" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C54" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C55" s="7" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C56" s="7" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="30">
       <c r="C57" s="7" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C58" s="7" t="s">
         <v>29</v>
       </c>
@@ -4042,372 +4027,348 @@
         <v>2012</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="19" customFormat="1" ht="30">
       <c r="B59" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
     </row>
-    <row r="60" spans="1:6" s="9" customFormat="1" ht="46.75">
+    <row r="60" spans="1:6" s="9" customFormat="1" ht="45">
       <c r="A60" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B60" s="16"/>
       <c r="C60" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="9" customFormat="1" ht="46.75">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="9" customFormat="1" ht="45">
       <c r="B61" s="16"/>
       <c r="C61" s="7" t="s">
-        <v>34</v>
+        <v>255</v>
       </c>
       <c r="D61" s="7"/>
-      <c r="E61" s="7">
-        <v>6407</v>
+      <c r="E61" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="9" customFormat="1" ht="46.75">
-      <c r="B62" s="16"/>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C62" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7" t="s">
-        <v>108</v>
+        <v>31</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="19" customFormat="1" ht="46.75">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C63" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E63" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C64" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" s="19">
+        <v>63412</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="19" customFormat="1">
+      <c r="B65" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+    </row>
+    <row r="66" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="C66" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E66" s="24">
+        <v>41133</v>
+      </c>
+      <c r="F66" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
+      <c r="C67" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E67" s="19">
+        <v>5000</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C68" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E68" s="13">
+        <v>40767</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C69" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E69" s="19">
+        <v>659056746</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="C70" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E70" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="F63" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="C64" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="F64" s="6" t="s">
+      <c r="F70" s="25" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="C65" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E65" s="19" t="s">
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A71" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E71" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="60">
+      <c r="A72" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C73" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E73" s="19">
+        <v>758075800</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A74" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="20"/>
+      <c r="C74" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C75" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A76" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A77" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E77" s="9">
+        <v>500</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A78" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E78" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F65" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="C66" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E66" s="19">
-        <v>63412</v>
-      </c>
-      <c r="F66" s="19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="19" customFormat="1">
-      <c r="B67" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-    </row>
-    <row r="68" spans="1:6" s="22" customFormat="1" ht="46.75">
-      <c r="C68" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D68" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E68" s="24">
-        <v>41133</v>
-      </c>
-      <c r="F68" s="25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
-      <c r="C69" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E69" s="19">
-        <v>5000</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="C70" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E70" s="13">
-        <v>40767</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="C71" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E71" s="19">
-        <v>659056746</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="22" customFormat="1" ht="46.75">
-      <c r="C72" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E72" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F72" s="25" t="s">
+      <c r="F78" s="19" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="A73" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D73" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E73" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="62.5">
-      <c r="A74" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D74" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E74" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="C75" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D75" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E75" s="19">
-        <v>758075800</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="A76" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B76" s="20"/>
-      <c r="C76" s="6" t="s">
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C79" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="E79" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="D76" s="20" t="s">
+      <c r="F79" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="20" customFormat="1" ht="45">
+      <c r="A80" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="22" customFormat="1" ht="45">
+      <c r="A81" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C81" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="E76" s="19" t="s">
+      <c r="D81" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="F76" s="6" t="s">
+      <c r="E81" s="20" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="C77" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E77" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="F77" s="19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="A78" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F78" s="19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="A79" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E79" s="9">
-        <v>500</v>
-      </c>
-      <c r="F79" s="19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="A80" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C80" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E80" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F80" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="19" customFormat="1" ht="46.75">
-      <c r="C81" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="D81" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="E81" s="19" t="s">
-        <v>188</v>
-      </c>
       <c r="F81" s="20" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="20" customFormat="1" ht="46.75">
-      <c r="A82" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="F82" s="20" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="22" customFormat="1" ht="46.75">
-      <c r="A83" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C83" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D83" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="E83" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="F83" s="20" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="19" customFormat="1">
-      <c r="B84" s="22"/>
-    </row>
-    <row r="85" spans="1:6" s="19" customFormat="1"/>
-    <row r="86" spans="1:6" s="19" customFormat="1" ht="409.5"/>
-    <row r="286" ht="15.5" hidden="1"/>
-    <row r="287" ht="15.5" hidden="1"/>
-    <row r="288" ht="15.5" hidden="1"/>
-    <row r="289" ht="15.5" hidden="1"/>
-    <row r="290" ht="15.5" hidden="1"/>
-    <row r="291" ht="15.5" hidden="1"/>
-    <row r="292" ht="15.5" hidden="1"/>
-    <row r="293" ht="15.5" hidden="1"/>
-    <row r="294" ht="15.5" hidden="1"/>
-    <row r="295" ht="15.5" hidden="1"/>
-    <row r="296" ht="15.5" hidden="1"/>
-    <row r="297" ht="15.5" hidden="1"/>
-    <row r="298" ht="15.5" hidden="1"/>
-    <row r="299" ht="15.5" hidden="1"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="19" customFormat="1">
+      <c r="B82" s="22"/>
+    </row>
+    <row r="83" spans="1:6" s="19" customFormat="1"/>
+    <row r="84" spans="1:6" s="19" customFormat="1"/>
+    <row r="284" hidden="1"/>
+    <row r="285" hidden="1"/>
+    <row r="286" hidden="1"/>
+    <row r="287" hidden="1"/>
+    <row r="288" hidden="1"/>
+    <row r="289" hidden="1"/>
+    <row r="290" hidden="1"/>
+    <row r="291" hidden="1"/>
+    <row r="292" hidden="1"/>
+    <row r="293" hidden="1"/>
+    <row r="294" hidden="1"/>
+    <row r="295" hidden="1"/>
+    <row r="296" hidden="1"/>
+    <row r="297" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4427,7 +4388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -4446,7 +4407,7 @@
     <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="10"/>
@@ -4456,7 +4417,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -4488,7 +4449,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="46.75">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4497,52 +4458,52 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" ht="46.75">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B5" s="6"/>
       <c r="C5" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="19" customFormat="1" ht="46.75">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B6" s="6"/>
       <c r="C6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" ht="46.75">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B7" s="6"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="19" customFormat="1" ht="46.75">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4552,42 +4513,42 @@
         <v>23235</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="19" customFormat="1" ht="46.75">
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="19" customFormat="1" ht="46.75">
+    <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G10" s="9"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -4595,73 +4556,73 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="19" customFormat="1" ht="46.75">
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="C13" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E13" s="19">
         <v>758075800</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
       <c r="C14" s="6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="19" customFormat="1">
       <c r="C16" s="20" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="20" customFormat="1" ht="34" customHeight="1">
       <c r="A17" s="20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="G17" s="9"/>
     </row>
@@ -4716,22 +4677,22 @@
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:1">
@@ -4772,17 +4733,17 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:1">
@@ -4790,7 +4751,7 @@
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:1">
@@ -4837,12 +4798,12 @@
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:1">
@@ -4856,22 +4817,22 @@
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="80" spans="1:1">

</xml_diff>

<commit_message>
Added a new action, "ReportWarrantModification" to the Warrant_Issued_Reporting SSP.  Also changed, "PersonCautionText" to "PersonCautionCodeText".
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -191,9 +191,6 @@
     <t>Extradition Indicator</t>
   </si>
   <si>
-    <t>Extradition Limits Code Text</t>
-  </si>
-  <si>
     <t>True if a subjectcan be extradited; false otherwise.</t>
   </si>
   <si>
@@ -683,9 +680,6 @@
     <t>Physical Feature Description Text</t>
   </si>
   <si>
-    <t>Person Caution Text</t>
-  </si>
-  <si>
     <t>Cautionary information about a person</t>
   </si>
   <si>
@@ -722,9 +716,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureDescriptionText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonCautionText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemMakeName</t>
   </si>
   <si>
@@ -795,6 +786,15 @@
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>Person Caution Code Text</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonCautionCodeText</t>
+  </si>
+  <si>
+    <t>Extradition Limit Code Text</t>
   </si>
 </sst>
 </file>
@@ -3243,8 +3243,8 @@
   <dimension ref="A1:F297"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
+      <pane ySplit="2" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3270,7 +3270,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -3302,10 +3302,10 @@
         <v>38</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="19" customFormat="1">
@@ -3316,10 +3316,10 @@
         <v>41</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="19" customFormat="1" ht="30">
@@ -3327,16 +3327,16 @@
         <v>34</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D6" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="19" customFormat="1">
@@ -3347,13 +3347,13 @@
         <v>45</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="19" customFormat="1">
@@ -3364,13 +3364,13 @@
         <v>44</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="22" customFormat="1">
@@ -3378,16 +3378,16 @@
         <v>34</v>
       </c>
       <c r="C9" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="E9" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="F9" s="22" t="s">
         <v>207</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="22" customFormat="1">
@@ -3396,16 +3396,16 @@
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="22" t="s">
         <v>209</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="19" customFormat="1">
@@ -3426,10 +3426,10 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="19" customFormat="1">
@@ -3439,10 +3439,10 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="19" customFormat="1">
@@ -3452,10 +3452,10 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="19" customFormat="1">
@@ -3465,10 +3465,10 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="19" customFormat="1">
@@ -3478,10 +3478,10 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3493,10 +3493,10 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3506,10 +3506,10 @@
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3519,10 +3519,10 @@
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3532,10 +3532,10 @@
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3545,10 +3545,10 @@
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="19" customFormat="1">
@@ -3556,28 +3556,28 @@
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E23" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
@@ -3586,16 +3586,16 @@
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E24" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
@@ -3608,68 +3608,68 @@
         <v>23235</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="20" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="19" customFormat="1">
@@ -3682,44 +3682,44 @@
         <v>354786908</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="19" customFormat="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="19" customFormat="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="19" customFormat="1">
@@ -3732,7 +3732,7 @@
         <v>71</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="19" customFormat="1">
@@ -3742,10 +3742,10 @@
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="19" customFormat="1">
@@ -3758,7 +3758,7 @@
         <v>165</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="19" customFormat="1">
@@ -3768,34 +3768,34 @@
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="19" customFormat="1">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="19" customFormat="1">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="19" customFormat="1">
@@ -3808,7 +3808,7 @@
         <v>98213455</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="20" customFormat="1" ht="45">
@@ -3817,16 +3817,16 @@
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F42" s="7" t="s">
         <v>203</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="19" customFormat="1">
@@ -3835,16 +3835,16 @@
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3856,10 +3856,10 @@
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3871,10 +3871,10 @@
         <v>20</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="19" customFormat="1">
@@ -3891,79 +3891,79 @@
         <v>27</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C48" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C49" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C50" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E50" s="20" t="b">
         <v>1</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C51" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C52" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C53" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
@@ -3971,52 +3971,52 @@
         <v>28</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C55" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C56" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="19" customFormat="1" ht="30">
       <c r="C57" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4027,7 +4027,7 @@
         <v>2012</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="19" customFormat="1" ht="30">
@@ -4049,23 +4049,23 @@
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="9" customFormat="1" ht="45">
       <c r="B61" s="16"/>
       <c r="C61" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4073,10 +4073,10 @@
         <v>31</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4084,10 +4084,10 @@
         <v>30</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4098,7 +4098,7 @@
         <v>63412</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="19" customFormat="1">
@@ -4121,7 +4121,7 @@
         <v>41133</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
@@ -4132,7 +4132,7 @@
         <v>5000</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4143,7 +4143,7 @@
         <v>40767</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4154,7 +4154,7 @@
         <v>659056746</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="22" customFormat="1" ht="45">
@@ -4162,10 +4162,10 @@
         <v>54</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4176,13 +4176,13 @@
         <v>55</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E71" s="19" t="b">
         <v>1</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="19" customFormat="1" ht="60">
@@ -4190,16 +4190,16 @@
         <v>34</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>56</v>
+        <v>257</v>
       </c>
       <c r="D72" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4207,13 +4207,13 @@
         <v>43</v>
       </c>
       <c r="D73" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E73" s="19">
         <v>758075800</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4222,30 +4222,30 @@
       </c>
       <c r="B74" s="20"/>
       <c r="C74" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D74" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E74" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="E74" s="19" t="s">
+      <c r="F74" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C75" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D75" s="19" t="s">
         <v>52</v>
       </c>
       <c r="E75" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4257,13 +4257,13 @@
         <v>47</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4272,16 +4272,16 @@
       </c>
       <c r="B77" s="9"/>
       <c r="C77" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E77" s="9">
         <v>500</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
@@ -4289,30 +4289,30 @@
         <v>34</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D78" s="19" t="s">
         <v>48</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C79" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D79" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="D79" s="20" t="s">
-        <v>172</v>
-      </c>
       <c r="E79" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="F79" s="20" t="s">
         <v>181</v>
-      </c>
-      <c r="F79" s="20" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="20" customFormat="1" ht="45">
@@ -4321,16 +4321,16 @@
       </c>
       <c r="B80" s="9"/>
       <c r="C80" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D80" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E80" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E80" s="9" t="s">
-        <v>184</v>
-      </c>
       <c r="F80" s="20" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="22" customFormat="1" ht="45">
@@ -4338,16 +4338,16 @@
         <v>34</v>
       </c>
       <c r="C81" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D81" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="D81" s="20" t="s">
+      <c r="E81" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="E81" s="20" t="s">
-        <v>187</v>
-      </c>
       <c r="F81" s="20" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="19" customFormat="1">
@@ -4417,7 +4417,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -4458,10 +4458,10 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4471,10 +4471,10 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4484,10 +4484,10 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4497,10 +4497,10 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
@@ -4513,35 +4513,35 @@
         <v>23235</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G10" s="9"/>
     </row>
@@ -4567,44 +4567,44 @@
         <v>758075800</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
       <c r="C14" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D14" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="E14" s="20" t="s">
-        <v>179</v>
-      </c>
       <c r="F14" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>52</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="19" customFormat="1">
       <c r="C16" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="20" customFormat="1" ht="34" customHeight="1">
@@ -4613,16 +4613,16 @@
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G17" s="9"/>
     </row>

</xml_diff>

<commit_message>
Added mapping for Warrant Cancelled Report
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="2940" windowWidth="28420" windowHeight="13760" tabRatio="500"/>
+    <workbookView xWindow="4440" yWindow="2940" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
     <sheet name="Warrant Accepted Report" sheetId="2" r:id="rId2"/>
-    <sheet name="Warrant Rejected Report" sheetId="3" r:id="rId3"/>
+    <sheet name="Warrant Cancelled Report" sheetId="5" r:id="rId3"/>
+    <sheet name="Warrant Rejected Report" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="269">
   <si>
     <t>CLASS</t>
   </si>
@@ -795,6 +796,39 @@
   </si>
   <si>
     <t>Extradition Limit Code Text</t>
+  </si>
+  <si>
+    <t>Warrant Cancelled Report</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonNameSuffixText</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderEnforcementAgency/wir-ext:AgencyRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderRequestEntity/nc:EntityPerson/wir-ext:PersonEmployeeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantAcceptedReport/j:Warrant/wir-ext:WarrantAugmentation/wir-ext:StateWarrantRepositoryIdentification/nc:IdentificationID/#text</t>
   </si>
 </sst>
 </file>
@@ -3242,23 +3276,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23" customHeight="1">
+    <row r="1" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>50</v>
@@ -3268,7 +3302,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -3288,7 +3322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="19" customFormat="1">
+    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>62</v>
       </c>
@@ -3297,7 +3331,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" s="19" customFormat="1">
+    <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>38</v>
       </c>
@@ -3308,7 +3342,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="19" customFormat="1">
+    <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3322,7 +3356,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="19" customFormat="1" ht="30">
+    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>34</v>
       </c>
@@ -3339,7 +3373,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="19" customFormat="1">
+    <row r="7" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>34</v>
       </c>
@@ -3356,7 +3390,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="19" customFormat="1">
+    <row r="8" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>34</v>
       </c>
@@ -3373,7 +3407,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="22" customFormat="1">
+    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>34</v>
       </c>
@@ -3390,7 +3424,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="22" customFormat="1">
+    <row r="10" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>34</v>
       </c>
@@ -3408,7 +3442,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="19" customFormat="1">
+    <row r="11" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
@@ -3417,7 +3451,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" s="19" customFormat="1">
+    <row r="12" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -3432,7 +3466,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="19" customFormat="1">
+    <row r="13" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="19" t="s">
         <v>10</v>
@@ -3445,7 +3479,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="19" customFormat="1">
+    <row r="14" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="19" t="s">
         <v>11</v>
@@ -3458,7 +3492,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="19" customFormat="1">
+    <row r="15" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="19" t="s">
         <v>12</v>
@@ -3471,7 +3505,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="19" customFormat="1">
+    <row r="16" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="19" t="s">
         <v>25</v>
@@ -3484,7 +3518,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="17" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -3499,7 +3533,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="18" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>10</v>
@@ -3512,7 +3546,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="19" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>11</v>
@@ -3525,7 +3559,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="20" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19" t="s">
         <v>12</v>
@@ -3538,7 +3572,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="19" t="s">
         <v>25</v>
@@ -3551,7 +3585,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="19" customFormat="1">
+    <row r="22" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
@@ -3568,7 +3602,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
         <v>197</v>
@@ -3580,7 +3614,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
+    <row r="24" spans="1:6" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>34</v>
       </c>
@@ -3598,7 +3632,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
+    <row r="25" spans="1:6" s="19" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
         <v>4</v>
@@ -3611,7 +3645,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="20" customFormat="1">
+    <row r="26" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
         <v>210</v>
@@ -3624,7 +3658,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="19" customFormat="1">
+    <row r="27" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
         <v>215</v>
@@ -3636,7 +3670,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="19" customFormat="1">
+    <row r="28" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
         <v>216</v>
@@ -3648,7 +3682,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="19" customFormat="1">
+    <row r="29" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
         <v>115</v>
@@ -3660,7 +3694,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="19" customFormat="1">
+    <row r="30" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
         <v>217</v>
@@ -3672,7 +3706,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="19" customFormat="1">
+    <row r="31" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
@@ -3685,7 +3719,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="19" customFormat="1">
+    <row r="32" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>169</v>
@@ -3698,7 +3732,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="19" customFormat="1">
+    <row r="33" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>116</v>
@@ -3710,7 +3744,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="19" customFormat="1">
+    <row r="34" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
         <v>117</v>
@@ -3722,7 +3756,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="19" customFormat="1">
+    <row r="35" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
         <v>21</v>
@@ -3735,7 +3769,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="19" customFormat="1">
+    <row r="36" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
         <v>22</v>
@@ -3748,7 +3782,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="19" customFormat="1">
+    <row r="37" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
         <v>23</v>
@@ -3761,7 +3795,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="19" customFormat="1">
+    <row r="38" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
         <v>24</v>
@@ -3774,7 +3808,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="19" customFormat="1">
+    <row r="39" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
         <v>118</v>
@@ -3786,7 +3820,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="19" customFormat="1">
+    <row r="40" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
         <v>218</v>
@@ -3798,7 +3832,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="19" customFormat="1">
+    <row r="41" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
         <v>6</v>
@@ -3811,7 +3845,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="45">
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>34</v>
       </c>
@@ -3829,7 +3863,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="19" customFormat="1">
+    <row r="43" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>34</v>
       </c>
@@ -3847,7 +3881,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>17</v>
       </c>
@@ -3862,7 +3896,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="s">
         <v>19</v>
@@ -3877,7 +3911,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="19" customFormat="1">
+    <row r="46" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
         <v>26</v>
       </c>
@@ -3886,7 +3920,7 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
     </row>
-    <row r="47" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C47" s="7" t="s">
         <v>27</v>
       </c>
@@ -3897,7 +3931,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="48" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C48" s="7" t="s">
         <v>64</v>
       </c>
@@ -3908,7 +3942,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="49" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="7" t="s">
         <v>213</v>
       </c>
@@ -3919,7 +3953,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="50" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="7" t="s">
         <v>246</v>
       </c>
@@ -3933,7 +3967,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="51" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="7" t="s">
         <v>244</v>
       </c>
@@ -3944,7 +3978,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C52" s="7" t="s">
         <v>113</v>
       </c>
@@ -3955,7 +3989,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C53" s="7" t="s">
         <v>114</v>
       </c>
@@ -3966,7 +4000,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C54" s="7" t="s">
         <v>28</v>
       </c>
@@ -3977,7 +4011,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C55" s="7" t="s">
         <v>220</v>
       </c>
@@ -3991,7 +4025,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C56" s="7" t="s">
         <v>221</v>
       </c>
@@ -4005,7 +4039,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="30">
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C57" s="7" t="s">
         <v>222</v>
       </c>
@@ -4019,7 +4053,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C58" s="7" t="s">
         <v>29</v>
       </c>
@@ -4030,7 +4064,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="19" customFormat="1" ht="30">
+    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
         <v>46</v>
       </c>
@@ -4039,7 +4073,7 @@
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
     </row>
-    <row r="60" spans="1:6" s="9" customFormat="1" ht="45">
+    <row r="60" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>34</v>
       </c>
@@ -4055,7 +4089,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="9" customFormat="1" ht="45">
+    <row r="61" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B61" s="16"/>
       <c r="C61" s="7" t="s">
         <v>252</v>
@@ -4068,7 +4102,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="62" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C62" s="7" t="s">
         <v>31</v>
       </c>
@@ -4079,7 +4113,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="63" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C63" s="7" t="s">
         <v>30</v>
       </c>
@@ -4090,7 +4124,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C64" s="19" t="s">
         <v>33</v>
       </c>
@@ -4101,7 +4135,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="19" customFormat="1">
+    <row r="65" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
         <v>35</v>
       </c>
@@ -4110,7 +4144,7 @@
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
     </row>
-    <row r="66" spans="1:6" s="22" customFormat="1" ht="45">
+    <row r="66" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C66" s="23" t="s">
         <v>36</v>
       </c>
@@ -4124,7 +4158,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
+    <row r="67" spans="1:6" s="19" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="7" t="s">
         <v>53</v>
       </c>
@@ -4135,7 +4169,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C68" s="7" t="s">
         <v>42</v>
       </c>
@@ -4146,7 +4180,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C69" s="7" t="s">
         <v>39</v>
       </c>
@@ -4157,7 +4191,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="22" customFormat="1" ht="45">
+    <row r="70" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C70" s="23" t="s">
         <v>54</v>
       </c>
@@ -4168,7 +4202,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
         <v>34</v>
       </c>
@@ -4185,7 +4219,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="60">
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
         <v>34</v>
       </c>
@@ -4202,7 +4236,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C73" s="6" t="s">
         <v>43</v>
       </c>
@@ -4216,7 +4250,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
         <v>34</v>
       </c>
@@ -4234,7 +4268,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C75" s="19" t="s">
         <v>66</v>
       </c>
@@ -4248,7 +4282,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>34</v>
       </c>
@@ -4266,7 +4300,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>34</v>
       </c>
@@ -4284,7 +4318,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>34</v>
       </c>
@@ -4301,7 +4335,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="45">
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C79" s="20" t="s">
         <v>170</v>
       </c>
@@ -4315,7 +4349,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="20" customFormat="1" ht="45">
+    <row r="80" spans="1:6" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
         <v>34</v>
       </c>
@@ -4333,7 +4367,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="22" customFormat="1" ht="45">
+    <row r="81" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
         <v>34</v>
       </c>
@@ -4350,25 +4384,25 @@
         <v>240</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="19" customFormat="1">
+    <row r="82" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="22"/>
     </row>
-    <row r="83" spans="1:6" s="19" customFormat="1"/>
-    <row r="84" spans="1:6" s="19" customFormat="1"/>
-    <row r="284" hidden="1"/>
-    <row r="285" hidden="1"/>
-    <row r="286" hidden="1"/>
-    <row r="287" hidden="1"/>
-    <row r="288" hidden="1"/>
-    <row r="289" hidden="1"/>
-    <row r="290" hidden="1"/>
-    <row r="291" hidden="1"/>
-    <row r="292" hidden="1"/>
-    <row r="293" hidden="1"/>
-    <row r="294" hidden="1"/>
-    <row r="295" hidden="1"/>
-    <row r="296" hidden="1"/>
-    <row r="297" hidden="1"/>
+    <row r="83" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="292" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="293" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="294" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="295" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="296" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="297" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4388,23 +4422,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B13" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23" customHeight="1">
+    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>49</v>
@@ -4415,7 +4449,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -4438,7 +4472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -4449,7 +4483,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4464,7 +4498,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="5" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="19" t="s">
         <v>10</v>
@@ -4477,7 +4511,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="6" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="19" t="s">
         <v>11</v>
@@ -4490,7 +4524,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="7" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
@@ -4503,7 +4537,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="8" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4517,7 +4551,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
         <v>216</v>
@@ -4531,7 +4565,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="10" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
         <v>217</v>
@@ -4545,7 +4579,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>35</v>
@@ -4556,7 +4590,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="19" customFormat="1" ht="45">
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>43</v>
       </c>
@@ -4570,7 +4604,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="30">
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>173</v>
       </c>
@@ -4584,7 +4618,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
         <v>66</v>
@@ -4599,7 +4633,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="19" customFormat="1">
+    <row r="16" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C16" s="20" t="s">
         <v>184</v>
       </c>
@@ -4607,7 +4641,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="20" customFormat="1" ht="34" customHeight="1">
+    <row r="17" spans="1:7" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>34</v>
       </c>
@@ -4626,234 +4660,234 @@
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" s="19" customFormat="1">
+    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="1:7" s="19" customFormat="1"/>
-    <row r="20" spans="1:7" s="19" customFormat="1"/>
-    <row r="21" spans="1:7" s="19" customFormat="1"/>
-    <row r="22" spans="1:7" s="19" customFormat="1"/>
-    <row r="23" spans="1:7">
+    <row r="19" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="19"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="19"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="19"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="19"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="19"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="19"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="19"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="19"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="19"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="19"/>
     </row>
   </sheetData>
@@ -4872,13 +4906,467 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="18">
+        <v>23235</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C13" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="C14" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="409.6" x14ac:dyDescent="0">
+      <c r="A36" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="409.6" x14ac:dyDescent="0">
+      <c r="A37" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="20"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="20"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="20"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="20"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="20"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="20"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="20"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="20"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="9"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="9"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="20"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="20"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="20"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="20"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="20"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="20"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="20"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="20"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="20"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="20"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="20"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="20"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="20"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="20"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="20"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="20"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="20"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="20"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="20"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="20"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="20"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Added Report Warrant Cancelled Action to the SSP.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="2940" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="8380" yWindow="1380" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -801,34 +801,34 @@
     <t>Warrant Cancelled Report</t>
   </si>
   <si>
-    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonNameSuffixText</t>
-  </si>
-  <si>
-    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
-  </si>
-  <si>
-    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonRaceText</t>
-  </si>
-  <si>
-    <t>wcr-doc:WarrantAcceptedReport/nc:Person[@structures:id=/wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonSexText</t>
-  </si>
-  <si>
-    <t>wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderEnforcementAgency/wir-ext:AgencyRecordIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>wcr-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderRequestEntity/nc:EntityPerson/wir-ext:PersonEmployeeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>wcr-doc:WarrantAcceptedReport/j:Warrant/wir-ext:WarrantAugmentation/wir-ext:StateWarrantRepositoryIdentification/nc:IdentificationID/#text</t>
+    <t>wcr-doc:WarrantCancelledReport/nc:Person[@structures:id=/wcr-doc:WarrantCancelledReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantCancelledReport/nc:Person[@structures:id=/wcr-doc:WarrantCancelledReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantCancelledReport/nc:Person[@structures:id=/wcr-doc:WarrantCancelledReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantCancelledReport/nc:Person[@structures:id=/wcr-doc:WarrantCancelledReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonNameSuffixText</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantCancelledReport/nc:Person[@structures:id=/wcr-doc:WarrantCancelledReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantCancelledReport/nc:Person[@structures:id=/wcr-doc:WarrantCancelledReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantCancelledReport/nc:Person[@structures:id=/wcr-doc:WarrantCancelledReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantCancelledReport/j:Warrant/j:CourtOrderEnforcementAgency/wir-ext:AgencyRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantCancelledReport/j:Warrant/j:CourtOrderRequestEntity/nc:EntityPerson/wir-ext:PersonEmployeeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wcr-doc:WarrantCancelledReport/j:Warrant/wir-ext:WarrantAugmentation/wir-ext:StateWarrantRepositoryIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -3281,18 +3281,18 @@
       <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="2"/>
+    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>50</v>
@@ -3302,7 +3302,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
         <v>62</v>
       </c>
@@ -3331,7 +3331,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="19" customFormat="1">
       <c r="C4" s="7" t="s">
         <v>38</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="19" customFormat="1">
       <c r="C5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.5">
       <c r="A6" s="19" t="s">
         <v>34</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="19" customFormat="1">
       <c r="A7" s="19" t="s">
         <v>34</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="19" customFormat="1">
       <c r="A8" s="19" t="s">
         <v>34</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.5">
       <c r="A9" s="22" t="s">
         <v>34</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="22" customFormat="1">
       <c r="A10" s="22" t="s">
         <v>34</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="19" customFormat="1">
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
@@ -3451,7 +3451,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="19" customFormat="1">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="19" customFormat="1">
       <c r="B13" s="6"/>
       <c r="C13" s="19" t="s">
         <v>10</v>
@@ -3479,7 +3479,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="19" customFormat="1">
       <c r="B14" s="6"/>
       <c r="C14" s="19" t="s">
         <v>11</v>
@@ -3492,7 +3492,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="19" customFormat="1">
       <c r="B15" s="6"/>
       <c r="C15" s="19" t="s">
         <v>12</v>
@@ -3505,7 +3505,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="19" customFormat="1">
       <c r="B16" s="6"/>
       <c r="C16" s="19" t="s">
         <v>25</v>
@@ -3518,7 +3518,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>10</v>
@@ -3546,7 +3546,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>11</v>
@@ -3559,7 +3559,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19" t="s">
         <v>12</v>
@@ -3572,7 +3572,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B21" s="6"/>
       <c r="C21" s="19" t="s">
         <v>25</v>
@@ -3585,7 +3585,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="19" customFormat="1">
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="20" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
         <v>197</v>
@@ -3614,7 +3614,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
       <c r="A24" s="20" t="s">
         <v>34</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="19" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
         <v>4</v>
@@ -3645,7 +3645,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="20" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
         <v>210</v>
@@ -3658,7 +3658,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="19" customFormat="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
         <v>215</v>
@@ -3670,7 +3670,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
         <v>216</v>
@@ -3682,7 +3682,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
         <v>115</v>
@@ -3694,7 +3694,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
         <v>217</v>
@@ -3706,7 +3706,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="19" customFormat="1">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
@@ -3719,7 +3719,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>169</v>
@@ -3732,7 +3732,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="19" customFormat="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>116</v>
@@ -3744,7 +3744,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="19" customFormat="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
         <v>117</v>
@@ -3756,7 +3756,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="19" customFormat="1">
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
         <v>21</v>
@@ -3769,7 +3769,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="19" customFormat="1">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
         <v>22</v>
@@ -3782,7 +3782,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="19" customFormat="1">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
         <v>23</v>
@@ -3795,7 +3795,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="19" customFormat="1">
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
         <v>24</v>
@@ -3808,7 +3808,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="19" customFormat="1">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
         <v>118</v>
@@ -3820,7 +3820,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="19" customFormat="1">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
         <v>218</v>
@@ -3832,7 +3832,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="19" customFormat="1">
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
         <v>6</v>
@@ -3845,7 +3845,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="47.25">
       <c r="A42" s="20" t="s">
         <v>34</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="19" customFormat="1">
       <c r="A43" s="19" t="s">
         <v>34</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B44" s="6" t="s">
         <v>17</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="s">
         <v>19</v>
@@ -3911,7 +3911,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="19" customFormat="1">
       <c r="B46" s="14" t="s">
         <v>26</v>
       </c>
@@ -3920,7 +3920,7 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
     </row>
-    <row r="47" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C47" s="7" t="s">
         <v>27</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C48" s="7" t="s">
         <v>64</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C49" s="7" t="s">
         <v>213</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C50" s="7" t="s">
         <v>246</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
       <c r="C51" s="7" t="s">
         <v>244</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C52" s="7" t="s">
         <v>113</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C53" s="7" t="s">
         <v>114</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C54" s="7" t="s">
         <v>28</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C55" s="7" t="s">
         <v>220</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C56" s="7" t="s">
         <v>221</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C57" s="7" t="s">
         <v>222</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C58" s="7" t="s">
         <v>29</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.5">
       <c r="B59" s="14" t="s">
         <v>46</v>
       </c>
@@ -4073,7 +4073,7 @@
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
     </row>
-    <row r="60" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" s="9" customFormat="1" ht="47.25">
       <c r="A60" s="9" t="s">
         <v>34</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" s="9" customFormat="1" ht="47.25">
       <c r="B61" s="16"/>
       <c r="C61" s="7" t="s">
         <v>252</v>
@@ -4102,7 +4102,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C62" s="7" t="s">
         <v>31</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C63" s="7" t="s">
         <v>30</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C64" s="19" t="s">
         <v>33</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" s="19" customFormat="1">
       <c r="B65" s="14" t="s">
         <v>35</v>
       </c>
@@ -4144,7 +4144,7 @@
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
     </row>
-    <row r="66" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="22" customFormat="1" ht="47.25">
       <c r="C66" s="23" t="s">
         <v>36</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="19" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
       <c r="C67" s="7" t="s">
         <v>53</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C68" s="7" t="s">
         <v>42</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C69" s="7" t="s">
         <v>39</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="22" customFormat="1" ht="47.25">
       <c r="C70" s="23" t="s">
         <v>54</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A71" s="19" t="s">
         <v>34</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="63">
       <c r="A72" s="19" t="s">
         <v>34</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C73" s="6" t="s">
         <v>43</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A74" s="20" t="s">
         <v>34</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C75" s="19" t="s">
         <v>66</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A76" s="19" t="s">
         <v>34</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A77" s="19" t="s">
         <v>34</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="A78" s="19" t="s">
         <v>34</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="47.25">
       <c r="C79" s="20" t="s">
         <v>170</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" s="20" customFormat="1" ht="47.25">
       <c r="A80" s="20" t="s">
         <v>34</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" s="22" customFormat="1" ht="47.25">
       <c r="A81" s="20" t="s">
         <v>34</v>
       </c>
@@ -4384,25 +4384,25 @@
         <v>240</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" s="19" customFormat="1">
       <c r="B82" s="22"/>
     </row>
-    <row r="83" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="292" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="293" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="294" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="295" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="296" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="297" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:6" s="19" customFormat="1"/>
+    <row r="84" spans="1:6" s="19" customFormat="1"/>
+    <row r="284" ht="15.75" hidden="1"/>
+    <row r="285" ht="15.75" hidden="1"/>
+    <row r="286" ht="15.75" hidden="1"/>
+    <row r="287" ht="15.75" hidden="1"/>
+    <row r="288" ht="15.75" hidden="1"/>
+    <row r="289" ht="15.75" hidden="1"/>
+    <row r="290" ht="15.75" hidden="1"/>
+    <row r="291" ht="15.75" hidden="1"/>
+    <row r="292" ht="15.75" hidden="1"/>
+    <row r="293" ht="15.75" hidden="1"/>
+    <row r="294" ht="15.75" hidden="1"/>
+    <row r="295" ht="15.75" hidden="1"/>
+    <row r="296" ht="15.75" hidden="1"/>
+    <row r="297" ht="15.75" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4422,23 +4422,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="2"/>
+    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>49</v>
@@ -4449,7 +4449,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -4483,7 +4483,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B5" s="6"/>
       <c r="C5" s="19" t="s">
         <v>10</v>
@@ -4511,7 +4511,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B6" s="6"/>
       <c r="C6" s="19" t="s">
         <v>11</v>
@@ -4524,7 +4524,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B7" s="6"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
@@ -4537,7 +4537,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4551,7 +4551,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
         <v>216</v>
@@ -4565,7 +4565,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
         <v>217</v>
@@ -4579,7 +4579,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>35</v>
@@ -4590,7 +4590,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="47.25">
       <c r="C13" s="6" t="s">
         <v>43</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.5">
       <c r="C14" s="6" t="s">
         <v>173</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.5">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
         <v>66</v>
@@ -4633,7 +4633,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="19" customFormat="1">
       <c r="C16" s="20" t="s">
         <v>184</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="20" customFormat="1" ht="34" customHeight="1">
       <c r="A17" s="20" t="s">
         <v>34</v>
       </c>
@@ -4660,234 +4660,234 @@
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="19" customFormat="1">
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="19" customFormat="1"/>
+    <row r="20" spans="1:7" s="19" customFormat="1"/>
+    <row r="21" spans="1:7" s="19" customFormat="1"/>
+    <row r="22" spans="1:7" s="19" customFormat="1"/>
+    <row r="23" spans="1:7">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="19"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="19"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="19"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="19"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="19"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="19"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="19"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="19"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="19"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="19"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="19"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="19"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="19"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="19"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="19"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="19"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="19"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="19"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="19"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="19"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="19"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" s="19"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" s="9"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" s="9"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1">
       <c r="A59" s="19"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1">
       <c r="A60" s="19"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1">
       <c r="A61" s="19"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1">
       <c r="A62" s="19"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1">
       <c r="A63" s="19"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1">
       <c r="A64" s="19"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1">
       <c r="A65" s="19"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1">
       <c r="A66" s="19"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1">
       <c r="A67" s="19"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1">
       <c r="A68" s="19"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1">
       <c r="A69" s="19"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1">
       <c r="A70" s="19"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1">
       <c r="A71" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1">
       <c r="A72" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1">
       <c r="A73" s="19"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1">
       <c r="A74" s="19"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1">
       <c r="A75" s="19"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1">
       <c r="A76" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1">
       <c r="A77" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1">
       <c r="A78" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1">
       <c r="A79" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1">
       <c r="A80" s="19"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1">
       <c r="A81" s="19"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1">
       <c r="A82" s="19"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1">
       <c r="A83" s="19"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1">
       <c r="A84" s="19"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1">
       <c r="A85" s="19"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1">
       <c r="A86" s="19"/>
     </row>
   </sheetData>
@@ -4908,23 +4908,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="2"/>
+    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>258</v>
@@ -4935,7 +4935,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="20"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -4969,7 +4969,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="20" customFormat="1" ht="45">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="20" customFormat="1" ht="47.25">
       <c r="B5" s="6"/>
       <c r="C5" s="20" t="s">
         <v>10</v>
@@ -4997,7 +4997,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="20" customFormat="1" ht="47.25">
       <c r="B6" s="6"/>
       <c r="C6" s="20" t="s">
         <v>11</v>
@@ -5010,7 +5010,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="20" customFormat="1" ht="47.25">
       <c r="B7" s="6"/>
       <c r="C7" s="20" t="s">
         <v>12</v>
@@ -5023,7 +5023,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="20" customFormat="1" ht="45">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="20" customFormat="1" ht="47.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
         <v>216</v>
@@ -5051,7 +5051,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="20" customFormat="1" ht="47.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
         <v>217</v>
@@ -5065,7 +5065,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
         <v>35</v>
@@ -5076,7 +5076,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="22" customFormat="1" ht="31.5">
       <c r="C13" s="6" t="s">
         <v>173</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="31.5">
       <c r="A14" s="20"/>
       <c r="C14" s="20" t="s">
         <v>66</v>
@@ -5105,7 +5105,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="20" customFormat="1" ht="34" customHeight="1">
       <c r="A15" s="20" t="s">
         <v>34</v>
       </c>
@@ -5124,229 +5124,229 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="20" customFormat="1"/>
+    <row r="17" spans="1:1" s="20" customFormat="1"/>
+    <row r="18" spans="1:1" s="20" customFormat="1"/>
+    <row r="19" spans="1:1" s="20" customFormat="1"/>
+    <row r="20" spans="1:1" s="20" customFormat="1"/>
+    <row r="21" spans="1:1">
       <c r="A21" s="20"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="20"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="20"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="20"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="20"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="20"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="20"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="20"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="20"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="20"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="20"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="20"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="20"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="409.6" x14ac:dyDescent="0">
+    <row r="36" spans="1:1" ht="409.5">
       <c r="A36" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="409.6" x14ac:dyDescent="0">
+    <row r="37" spans="1:1" ht="409.5">
       <c r="A37" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="20"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="20"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="20"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="20"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="20"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="20"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="20"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="20"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="20"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="20"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="20"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="20"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53" s="20"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" s="9"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" s="9"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" s="20"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" s="20"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1">
       <c r="A59" s="20"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1">
       <c r="A60" s="20"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1">
       <c r="A61" s="20"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1">
       <c r="A62" s="20"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1">
       <c r="A63" s="20"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1">
       <c r="A64" s="20"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1">
       <c r="A65" s="20"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1">
       <c r="A66" s="20"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1">
       <c r="A67" s="20"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1">
       <c r="A68" s="20"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1">
       <c r="A69" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1">
       <c r="A70" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1">
       <c r="A71" s="20"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1">
       <c r="A72" s="20"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1">
       <c r="A73" s="20"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1">
       <c r="A74" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1">
       <c r="A75" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1">
       <c r="A76" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1">
       <c r="A77" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1">
       <c r="A78" s="20"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1">
       <c r="A79" s="20"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1">
       <c r="A80" s="20"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1">
       <c r="A81" s="20"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1">
       <c r="A82" s="20"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1">
       <c r="A83" s="20"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1">
       <c r="A84" s="20"/>
     </row>
   </sheetData>
@@ -5355,6 +5355,11 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5366,7 +5371,7 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Added Warrant Modification Report to Mapping Spreadsheet.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,28 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="1380" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="8385" yWindow="1380" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
     <sheet name="Warrant Accepted Report" sheetId="2" r:id="rId2"/>
     <sheet name="Warrant Cancelled Report" sheetId="5" r:id="rId3"/>
-    <sheet name="Warrant Rejected Report" sheetId="3" r:id="rId4"/>
+    <sheet name="Warrant Modification Report" sheetId="6" r:id="rId4"/>
+    <sheet name="Warrant Rejected Report" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="350">
   <si>
     <t>CLASS</t>
   </si>
@@ -829,13 +825,256 @@
   </si>
   <si>
     <t>wcr-doc:WarrantCancelledReport/j:Warrant/wir-ext:WarrantAugmentation/wir-ext:StateWarrantRepositoryIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Warrant Modification Request</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Case/nc:CaseDocketID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Case/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Case/j:CaseAugmentation/j:CaseCharge/wm-req-ext:GeneralOffenseCharacterDescriptionText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Case/j:CaseAugmentation/j:CaseCharge/wm-req-ext:ChargeCodeText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Case/j:CaseAugmentation/j:CaseCharge/wm-req-ext:OriginalOffenseCodeText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Case/j:CaseAugmentation/j:CaseCharge/wm-req-ext:ProsecutionChargeCodeText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Case/wm-req-ext:CriminalTrackingNumber</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonName/nc:PersonNameSuffixText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonName/nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonCitizenshipText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonUSCitizenIndicator</t>
+  </si>
+  <si>
+    <t>True if a person query should include the DHS ICE Database; false otherwise.</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/wm-req-ext:PersonImmigrationAlienQueryIndicator</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonAgeDescriptionText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonEthnicityText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonEyeColorText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/j:PersonAugmentation/j:PersonFBIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonStateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonSkinToneText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonHairColorText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonHeightMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonHeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonWeightMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonWeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonBirthLocation/nc:LocationCategoryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureCategoryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonSSNIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Miscellaneous Person Record Number</t>
+  </si>
+  <si>
+    <t>A miscellaneous unique identification assigned to a person record.</t>
+  </si>
+  <si>
+    <t>MR456782</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/wm-req-ext:PersonMiscellaneousRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Caution Code Text</t>
+  </si>
+  <si>
+    <t>A cautionary code for a person</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/wm-req-ext:PersonCautionCodeText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationJurisdiction/j:JurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistration[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistration[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:ConveyanceRegistrationPlateCategoryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistration[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:RegistrationExpirationDate/nc:YearMonthDate</t>
+  </si>
+  <si>
+    <t>/wm-req-doc:WarrantIssuedReport/j:ConveyanceRegistration[not(j:RegistrationExpirationDate)]/wm-req-ext:ConveyanceRegistrationNonExpiringIndicator</t>
+  </si>
+  <si>
+    <t>Vehicle Registration State</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistration[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:JurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorPrimaryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorSecondaryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemMakeName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemModelName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemStyleText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemModelYearDate</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/wm-req-ext:AddressCategoryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStateName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/nc:ExpirationDate/nc:Date</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/j:WarrantAppearanceBail/j:BailSetAmount/nc:Amount</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/j:CourtOrderIssuingDate/nc:Date</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/j:CourtOrderIssuingCourt/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/j:CourtOrderDesignatedSubject/j:SubjectCorrectionsIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:ExtraditionIndicator</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:ExtraditionLimitCodeText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/j:CourtOrderEnforcementAgency/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/j:CourtOrderEnforcementAgency/wm-req-ext:AgencyRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/j:CourtOrderRequestEntity/nc:EntityPerson/wm-req-ext:PersonEmployeeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:SubjectPickupRadiusCodeText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:WarrantBroadcastCodeText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/scr:TransactionControlNumberIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>A comment note or remark regarding a warrant</t>
+  </si>
+  <si>
+    <t>Warrant Comment</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:WarrantCommentText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:WarrantEntryCategoryCodeText</t>
+  </si>
+  <si>
+    <t>State Warrant Repository ID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:StateWarrantRepositoryIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -922,6 +1161,25 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1909,7 +2167,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1987,6 +2245,46 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3281,18 +3579,18 @@
       <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23" customHeight="1">
+    <row r="1" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>50</v>
@@ -3302,7 +3600,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -3322,7 +3620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="19" customFormat="1">
+    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>62</v>
       </c>
@@ -3331,7 +3629,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" s="19" customFormat="1">
+    <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>38</v>
       </c>
@@ -3342,7 +3640,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="19" customFormat="1">
+    <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3356,7 +3654,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.5">
+    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>34</v>
       </c>
@@ -3373,7 +3671,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="19" customFormat="1">
+    <row r="7" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>34</v>
       </c>
@@ -3390,7 +3688,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="19" customFormat="1">
+    <row r="8" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>34</v>
       </c>
@@ -3407,7 +3705,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.5">
+    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>34</v>
       </c>
@@ -3424,7 +3722,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="22" customFormat="1">
+    <row r="10" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>34</v>
       </c>
@@ -3442,7 +3740,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="19" customFormat="1">
+    <row r="11" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
@@ -3451,7 +3749,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" s="19" customFormat="1">
+    <row r="12" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -3466,7 +3764,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="19" customFormat="1">
+    <row r="13" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="19" t="s">
         <v>10</v>
@@ -3479,7 +3777,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="19" customFormat="1">
+    <row r="14" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="19" t="s">
         <v>11</v>
@@ -3492,7 +3790,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="19" customFormat="1">
+    <row r="15" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="19" t="s">
         <v>12</v>
@@ -3505,7 +3803,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="19" customFormat="1">
+    <row r="16" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="19" t="s">
         <v>25</v>
@@ -3518,7 +3816,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="17" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -3533,7 +3831,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="18" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>10</v>
@@ -3546,7 +3844,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="19" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>11</v>
@@ -3559,7 +3857,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="20" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19" t="s">
         <v>12</v>
@@ -3572,7 +3870,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="19" t="s">
         <v>25</v>
@@ -3585,7 +3883,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="19" customFormat="1">
+    <row r="22" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
@@ -3602,7 +3900,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
         <v>197</v>
@@ -3614,7 +3912,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
+    <row r="24" spans="1:6" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>34</v>
       </c>
@@ -3632,7 +3930,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
+    <row r="25" spans="1:6" s="19" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
         <v>4</v>
@@ -3645,7 +3943,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="20" customFormat="1">
+    <row r="26" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
         <v>210</v>
@@ -3658,7 +3956,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="19" customFormat="1">
+    <row r="27" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
         <v>215</v>
@@ -3670,7 +3968,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="19" customFormat="1">
+    <row r="28" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
         <v>216</v>
@@ -3682,7 +3980,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="19" customFormat="1">
+    <row r="29" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
         <v>115</v>
@@ -3694,7 +3992,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="19" customFormat="1">
+    <row r="30" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
         <v>217</v>
@@ -3706,7 +4004,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="19" customFormat="1">
+    <row r="31" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
@@ -3719,7 +4017,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="19" customFormat="1">
+    <row r="32" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>169</v>
@@ -3732,7 +4030,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="19" customFormat="1">
+    <row r="33" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>116</v>
@@ -3744,7 +4042,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="19" customFormat="1">
+    <row r="34" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
         <v>117</v>
@@ -3756,7 +4054,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="19" customFormat="1">
+    <row r="35" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
         <v>21</v>
@@ -3769,7 +4067,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="19" customFormat="1">
+    <row r="36" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
         <v>22</v>
@@ -3782,7 +4080,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="19" customFormat="1">
+    <row r="37" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
         <v>23</v>
@@ -3795,7 +4093,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="19" customFormat="1">
+    <row r="38" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
         <v>24</v>
@@ -3808,7 +4106,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="19" customFormat="1">
+    <row r="39" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
         <v>118</v>
@@ -3820,7 +4118,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="19" customFormat="1">
+    <row r="40" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
         <v>218</v>
@@ -3832,7 +4130,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="19" customFormat="1">
+    <row r="41" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
         <v>6</v>
@@ -3845,7 +4143,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="47.25">
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>34</v>
       </c>
@@ -3863,7 +4161,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="19" customFormat="1">
+    <row r="43" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>34</v>
       </c>
@@ -3881,7 +4179,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>17</v>
       </c>
@@ -3896,7 +4194,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="s">
         <v>19</v>
@@ -3911,7 +4209,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="19" customFormat="1">
+    <row r="46" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
         <v>26</v>
       </c>
@@ -3920,7 +4218,7 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
     </row>
-    <row r="47" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C47" s="7" t="s">
         <v>27</v>
       </c>
@@ -3931,7 +4229,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="48" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C48" s="7" t="s">
         <v>64</v>
       </c>
@@ -3942,7 +4240,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="49" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="7" t="s">
         <v>213</v>
       </c>
@@ -3953,7 +4251,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="50" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="7" t="s">
         <v>246</v>
       </c>
@@ -3967,7 +4265,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="51" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="7" t="s">
         <v>244</v>
       </c>
@@ -3978,7 +4276,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C52" s="7" t="s">
         <v>113</v>
       </c>
@@ -3989,7 +4287,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C53" s="7" t="s">
         <v>114</v>
       </c>
@@ -4000,7 +4298,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C54" s="7" t="s">
         <v>28</v>
       </c>
@@ -4011,7 +4309,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C55" s="7" t="s">
         <v>220</v>
       </c>
@@ -4025,7 +4323,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C56" s="7" t="s">
         <v>221</v>
       </c>
@@ -4039,7 +4337,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C57" s="7" t="s">
         <v>222</v>
       </c>
@@ -4053,7 +4351,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C58" s="7" t="s">
         <v>29</v>
       </c>
@@ -4064,7 +4362,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.5">
+    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
         <v>46</v>
       </c>
@@ -4073,7 +4371,7 @@
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
     </row>
-    <row r="60" spans="1:6" s="9" customFormat="1" ht="47.25">
+    <row r="60" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>34</v>
       </c>
@@ -4089,7 +4387,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="9" customFormat="1" ht="47.25">
+    <row r="61" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B61" s="16"/>
       <c r="C61" s="7" t="s">
         <v>252</v>
@@ -4102,7 +4400,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="62" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C62" s="7" t="s">
         <v>31</v>
       </c>
@@ -4113,7 +4411,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="63" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C63" s="7" t="s">
         <v>30</v>
       </c>
@@ -4124,7 +4422,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C64" s="19" t="s">
         <v>33</v>
       </c>
@@ -4135,7 +4433,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="19" customFormat="1">
+    <row r="65" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
         <v>35</v>
       </c>
@@ -4144,7 +4442,7 @@
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
     </row>
-    <row r="66" spans="1:6" s="22" customFormat="1" ht="47.25">
+    <row r="66" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C66" s="23" t="s">
         <v>36</v>
       </c>
@@ -4158,7 +4456,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
+    <row r="67" spans="1:6" s="19" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="7" t="s">
         <v>53</v>
       </c>
@@ -4169,7 +4467,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C68" s="7" t="s">
         <v>42</v>
       </c>
@@ -4180,7 +4478,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C69" s="7" t="s">
         <v>39</v>
       </c>
@@ -4191,7 +4489,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="22" customFormat="1" ht="47.25">
+    <row r="70" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C70" s="23" t="s">
         <v>54</v>
       </c>
@@ -4202,7 +4500,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
         <v>34</v>
       </c>
@@ -4219,7 +4517,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="63">
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
         <v>34</v>
       </c>
@@ -4236,7 +4534,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C73" s="6" t="s">
         <v>43</v>
       </c>
@@ -4250,7 +4548,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
         <v>34</v>
       </c>
@@ -4268,7 +4566,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C75" s="19" t="s">
         <v>66</v>
       </c>
@@ -4282,7 +4580,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>34</v>
       </c>
@@ -4300,7 +4598,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>34</v>
       </c>
@@ -4318,7 +4616,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>34</v>
       </c>
@@ -4335,7 +4633,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C79" s="20" t="s">
         <v>170</v>
       </c>
@@ -4349,7 +4647,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="20" customFormat="1" ht="47.25">
+    <row r="80" spans="1:6" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
         <v>34</v>
       </c>
@@ -4367,7 +4665,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="22" customFormat="1" ht="47.25">
+    <row r="81" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
         <v>34</v>
       </c>
@@ -4384,25 +4682,25 @@
         <v>240</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="19" customFormat="1">
+    <row r="82" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="22"/>
     </row>
-    <row r="83" spans="1:6" s="19" customFormat="1"/>
-    <row r="84" spans="1:6" s="19" customFormat="1"/>
-    <row r="284" ht="15.75" hidden="1"/>
-    <row r="285" ht="15.75" hidden="1"/>
-    <row r="286" ht="15.75" hidden="1"/>
-    <row r="287" ht="15.75" hidden="1"/>
-    <row r="288" ht="15.75" hidden="1"/>
-    <row r="289" ht="15.75" hidden="1"/>
-    <row r="290" ht="15.75" hidden="1"/>
-    <row r="291" ht="15.75" hidden="1"/>
-    <row r="292" ht="15.75" hidden="1"/>
-    <row r="293" ht="15.75" hidden="1"/>
-    <row r="294" ht="15.75" hidden="1"/>
-    <row r="295" ht="15.75" hidden="1"/>
-    <row r="296" ht="15.75" hidden="1"/>
-    <row r="297" ht="15.75" hidden="1"/>
+    <row r="83" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="292" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="293" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="294" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="295" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="296" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="297" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4426,19 +4724,19 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23" customHeight="1">
+    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>49</v>
@@ -4449,7 +4747,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -4472,7 +4770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -4483,7 +4781,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4498,7 +4796,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="5" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="19" t="s">
         <v>10</v>
@@ -4511,7 +4809,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="6" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="19" t="s">
         <v>11</v>
@@ -4524,7 +4822,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="7" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
@@ -4537,7 +4835,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="8" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4551,7 +4849,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
         <v>216</v>
@@ -4565,7 +4863,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="10" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
         <v>217</v>
@@ -4579,7 +4877,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>35</v>
@@ -4590,7 +4888,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>43</v>
       </c>
@@ -4604,7 +4902,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.5">
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>173</v>
       </c>
@@ -4618,7 +4916,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.5">
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
         <v>66</v>
@@ -4633,7 +4931,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="19" customFormat="1">
+    <row r="16" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C16" s="20" t="s">
         <v>184</v>
       </c>
@@ -4641,7 +4939,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="20" customFormat="1" ht="34" customHeight="1">
+    <row r="17" spans="1:7" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>34</v>
       </c>
@@ -4660,234 +4958,234 @@
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" s="19" customFormat="1">
+    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="1:7" s="19" customFormat="1"/>
-    <row r="20" spans="1:7" s="19" customFormat="1"/>
-    <row r="21" spans="1:7" s="19" customFormat="1"/>
-    <row r="22" spans="1:7" s="19" customFormat="1"/>
-    <row r="23" spans="1:7">
+    <row r="19" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="19"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="19"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="19"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="19"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="19"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="19"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="19"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="19"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="19"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="19"/>
     </row>
   </sheetData>
@@ -4908,23 +5206,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+    <sheetView topLeftCell="D6" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23" customHeight="1">
+    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="26" t="s">
         <v>258</v>
@@ -4935,7 +5233,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -4958,7 +5256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -4969,7 +5267,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="20" customFormat="1" ht="45">
+    <row r="4" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4984,7 +5282,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="5" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="20" t="s">
         <v>10</v>
@@ -4997,7 +5295,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="6" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="20" t="s">
         <v>11</v>
@@ -5010,7 +5308,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="7" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="20" t="s">
         <v>12</v>
@@ -5023,7 +5321,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="20" customFormat="1" ht="45">
+    <row r="8" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -5037,7 +5335,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="9" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
         <v>216</v>
@@ -5051,7 +5349,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="10" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
         <v>217</v>
@@ -5065,7 +5363,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
         <v>35</v>
@@ -5076,7 +5374,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="22" customFormat="1" ht="31.5">
+    <row r="13" spans="1:7" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>173</v>
       </c>
@@ -5090,7 +5388,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="31.5">
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="C14" s="20" t="s">
         <v>66</v>
@@ -5105,7 +5403,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="20" customFormat="1" ht="34" customHeight="1">
+    <row r="15" spans="1:7" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>34</v>
       </c>
@@ -5124,229 +5422,229 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" s="20" customFormat="1"/>
-    <row r="17" spans="1:1" s="20" customFormat="1"/>
-    <row r="18" spans="1:1" s="20" customFormat="1"/>
-    <row r="19" spans="1:1" s="20" customFormat="1"/>
-    <row r="20" spans="1:1" s="20" customFormat="1"/>
-    <row r="21" spans="1:1">
+    <row r="16" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="409.5">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="409.5">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="20"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="20"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="20"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="20"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="20"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="20"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="20"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="20"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="20"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="20"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="20"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="20"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="20"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="20"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="20"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="20"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="20"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="20"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="20"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="20"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="20"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="20"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="20"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="20"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="20"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="20"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="20"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="20"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="20"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="20"/>
     </row>
   </sheetData>
@@ -5365,13 +5663,1179 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.75" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
+    <col min="6" max="6" width="55.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32"/>
+      <c r="B1" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+    </row>
+    <row r="4" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+    </row>
+    <row r="12" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>285</v>
+      </c>
+      <c r="E19" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38">
+        <v>23235</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="28"/>
+      <c r="E24" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30">
+        <v>354786908</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F27" s="30" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="E28" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="28"/>
+      <c r="E29" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30">
+        <v>71</v>
+      </c>
+      <c r="F30" s="30" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30">
+        <v>165</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="30" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="28"/>
+      <c r="E34" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="D35" s="28"/>
+      <c r="E35" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30">
+        <v>98213455</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30" t="s">
+        <v>304</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>305</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>306</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>309</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="28"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="28"/>
+      <c r="B41" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+    </row>
+    <row r="42" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="28"/>
+      <c r="E42" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="28"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="28"/>
+      <c r="E43" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="28"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="D44" s="28"/>
+      <c r="E44" s="39" t="s">
+        <v>234</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="E45" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="28"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="30" t="s">
+        <v>317</v>
+      </c>
+      <c r="D46" s="28"/>
+      <c r="E46" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="28"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D47" s="28"/>
+      <c r="E47" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="29" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="28"/>
+      <c r="E48" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="F48" s="29" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="28"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="28"/>
+      <c r="E49" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="F49" s="29" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="28"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="F50" s="29" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="D51" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="F51" s="29" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="28"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="28"/>
+      <c r="E53" s="39">
+        <v>2012</v>
+      </c>
+      <c r="F53" s="29" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="28"/>
+      <c r="B54" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+    </row>
+    <row r="55" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="36"/>
+      <c r="C55" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F55" s="29" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="31"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="F56" s="29" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="28"/>
+      <c r="E57" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="F57" s="29" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="28"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" s="28"/>
+      <c r="E58" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58" s="29" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="28"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="28"/>
+      <c r="E59" s="39">
+        <v>63412</v>
+      </c>
+      <c r="F59" s="39" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="28"/>
+      <c r="B60" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="35"/>
+    </row>
+    <row r="61" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" s="33">
+        <v>41133</v>
+      </c>
+      <c r="F61" s="29" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="28"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" s="28"/>
+      <c r="E62" s="39">
+        <v>5000</v>
+      </c>
+      <c r="F62" s="29" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="28"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="28"/>
+      <c r="E63" s="33">
+        <v>40767</v>
+      </c>
+      <c r="F63" s="29" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="28"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D64" s="28"/>
+      <c r="E64" s="39">
+        <v>659056746</v>
+      </c>
+      <c r="F64" s="29" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="28"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="28"/>
+      <c r="E65" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66" s="28"/>
+      <c r="C66" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B67" s="28"/>
+      <c r="C67" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="D67" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="E67" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="28"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D68" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E68" s="39">
+        <v>758075800</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="28"/>
+      <c r="C69" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="D69" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="E69" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="28"/>
+      <c r="B70" s="28"/>
+      <c r="C70" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E70" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="F70" s="39" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" s="31"/>
+      <c r="C71" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D71" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" s="31">
+        <v>500</v>
+      </c>
+      <c r="F71" s="39" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="28"/>
+      <c r="C72" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D72" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E72" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="F72" s="39" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="28"/>
+      <c r="C73" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="D73" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="E73" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F73" s="39" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="28"/>
+      <c r="C74" s="39" t="s">
+        <v>242</v>
+      </c>
+      <c r="D74" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="E74" s="39" t="s">
+        <v>345</v>
+      </c>
+      <c r="F74" s="39" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" s="28"/>
+      <c r="C75" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="D75" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E75" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="F75" s="39" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="28"/>
+      <c r="C76" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="D76" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="E76" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="F76" s="39" t="s">
+        <v>349</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Added Notify Document Complete Reporting SSP
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="1380" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="8385" yWindow="1380" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -3579,23 +3579,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F297"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="40.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23" customHeight="1">
+    <row r="1" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="39" t="s">
         <v>50</v>
@@ -3605,7 +3605,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="19" customFormat="1">
+    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>62</v>
       </c>
@@ -3634,7 +3634,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" s="19" customFormat="1">
+    <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>38</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="19" customFormat="1">
+    <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.5">
+    <row r="6" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>34</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="19" customFormat="1">
+    <row r="7" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>34</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="19" customFormat="1">
+    <row r="8" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>34</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.5">
+    <row r="9" spans="1:6" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>34</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="22" customFormat="1">
+    <row r="10" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>34</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="19" customFormat="1">
+    <row r="11" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
@@ -3754,7 +3754,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" s="19" customFormat="1">
+    <row r="12" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="19" customFormat="1">
+    <row r="13" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="19" t="s">
         <v>10</v>
@@ -3782,7 +3782,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="19" customFormat="1">
+    <row r="14" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="19" t="s">
         <v>11</v>
@@ -3795,7 +3795,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="19" customFormat="1">
+    <row r="15" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="19" t="s">
         <v>12</v>
@@ -3808,7 +3808,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="19" customFormat="1">
+    <row r="16" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="19" t="s">
         <v>25</v>
@@ -3821,7 +3821,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="17" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="18" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="19" t="s">
         <v>10</v>
@@ -3849,7 +3849,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="19" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="19" t="s">
         <v>11</v>
@@ -3862,7 +3862,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="20" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19" t="s">
         <v>12</v>
@@ -3875,7 +3875,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="19" t="s">
         <v>25</v>
@@ -3888,7 +3888,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="19" customFormat="1">
+    <row r="22" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="20" customFormat="1" ht="25" customHeight="1">
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
         <v>197</v>
@@ -3917,7 +3917,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="20" customFormat="1" ht="34" customHeight="1">
+    <row r="24" spans="1:6" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>34</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="19" customFormat="1" ht="34" customHeight="1">
+    <row r="25" spans="1:6" s="19" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
         <v>4</v>
@@ -3948,7 +3948,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="20" customFormat="1">
+    <row r="26" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
         <v>210</v>
@@ -3961,7 +3961,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="19" customFormat="1">
+    <row r="27" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
         <v>215</v>
@@ -3973,7 +3973,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="19" customFormat="1">
+    <row r="28" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
         <v>216</v>
@@ -3985,7 +3985,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="19" customFormat="1">
+    <row r="29" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
         <v>115</v>
@@ -3997,7 +3997,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="19" customFormat="1">
+    <row r="30" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
         <v>217</v>
@@ -4009,7 +4009,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="19" customFormat="1">
+    <row r="31" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
@@ -4022,7 +4022,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="19" customFormat="1">
+    <row r="32" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>169</v>
@@ -4035,7 +4035,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="19" customFormat="1">
+    <row r="33" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>116</v>
@@ -4047,7 +4047,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="19" customFormat="1">
+    <row r="34" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
         <v>117</v>
@@ -4059,7 +4059,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="19" customFormat="1">
+    <row r="35" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
         <v>21</v>
@@ -4072,7 +4072,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="19" customFormat="1">
+    <row r="36" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
         <v>22</v>
@@ -4085,7 +4085,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="19" customFormat="1">
+    <row r="37" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
         <v>23</v>
@@ -4098,7 +4098,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="19" customFormat="1">
+    <row r="38" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
         <v>24</v>
@@ -4111,7 +4111,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="19" customFormat="1">
+    <row r="39" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
         <v>118</v>
@@ -4123,7 +4123,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="19" customFormat="1">
+    <row r="40" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
         <v>218</v>
@@ -4135,7 +4135,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="19" customFormat="1">
+    <row r="41" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
         <v>6</v>
@@ -4148,7 +4148,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="47.25">
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>34</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="19" customFormat="1">
+    <row r="43" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>34</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>17</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="s">
         <v>19</v>
@@ -4214,7 +4214,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="19" customFormat="1">
+    <row r="46" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
         <v>26</v>
       </c>
@@ -4223,7 +4223,7 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
     </row>
-    <row r="47" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C47" s="7" t="s">
         <v>27</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="48" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C48" s="7" t="s">
         <v>64</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="49" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="7" t="s">
         <v>213</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="50" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="7" t="s">
         <v>246</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="20" customFormat="1" ht="56" customHeight="1">
+    <row r="51" spans="1:6" s="20" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="7" t="s">
         <v>244</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C52" s="7" t="s">
         <v>113</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C53" s="7" t="s">
         <v>114</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C54" s="7" t="s">
         <v>28</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="55" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C55" s="7" t="s">
         <v>220</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="56" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C56" s="7" t="s">
         <v>221</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C57" s="7" t="s">
         <v>222</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C58" s="7" t="s">
         <v>29</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.5">
+    <row r="59" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
         <v>46</v>
       </c>
@@ -4376,7 +4376,7 @@
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
     </row>
-    <row r="60" spans="1:6" s="9" customFormat="1" ht="47.25">
+    <row r="60" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>34</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="9" customFormat="1" ht="47.25">
+    <row r="61" spans="1:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B61" s="16"/>
       <c r="C61" s="7" t="s">
         <v>252</v>
@@ -4405,7 +4405,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="62" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C62" s="7" t="s">
         <v>31</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="63" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C63" s="7" t="s">
         <v>30</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C64" s="19" t="s">
         <v>33</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="19" customFormat="1">
+    <row r="65" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
         <v>35</v>
       </c>
@@ -4447,7 +4447,7 @@
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
     </row>
-    <row r="66" spans="1:6" s="22" customFormat="1" ht="47.25">
+    <row r="66" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C66" s="23" t="s">
         <v>36</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
+    <row r="67" spans="1:6" s="19" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="7" t="s">
         <v>53</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C68" s="7" t="s">
         <v>42</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C69" s="7" t="s">
         <v>39</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="22" customFormat="1" ht="47.25">
+    <row r="70" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C70" s="23" t="s">
         <v>54</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
         <v>34</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="19" customFormat="1" ht="63">
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
         <v>34</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C73" s="6" t="s">
         <v>43</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
         <v>34</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C75" s="19" t="s">
         <v>66</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>34</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="77" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>34</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="78" spans="1:6" s="19" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>34</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="19" customFormat="1" ht="47.25">
+    <row r="79" spans="1:6" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C79" s="20" t="s">
         <v>170</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="20" customFormat="1" ht="47.25">
+    <row r="80" spans="1:6" s="20" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
         <v>34</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="22" customFormat="1" ht="47.25">
+    <row r="81" spans="1:6" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
         <v>34</v>
       </c>
@@ -4687,25 +4687,25 @@
         <v>240</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="19" customFormat="1">
+    <row r="82" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="22"/>
     </row>
-    <row r="83" spans="1:6" s="19" customFormat="1"/>
-    <row r="84" spans="1:6" s="19" customFormat="1"/>
-    <row r="284" ht="15.75" hidden="1"/>
-    <row r="285" ht="15.75" hidden="1"/>
-    <row r="286" ht="15.75" hidden="1"/>
-    <row r="287" ht="15.75" hidden="1"/>
-    <row r="288" ht="15.75" hidden="1"/>
-    <row r="289" ht="15.75" hidden="1"/>
-    <row r="290" ht="15.75" hidden="1"/>
-    <row r="291" ht="15.75" hidden="1"/>
-    <row r="292" ht="15.75" hidden="1"/>
-    <row r="293" ht="15.75" hidden="1"/>
-    <row r="294" ht="15.75" hidden="1"/>
-    <row r="295" ht="15.75" hidden="1"/>
-    <row r="296" ht="15.75" hidden="1"/>
-    <row r="297" ht="15.75" hidden="1"/>
+    <row r="83" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="292" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="293" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="294" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="295" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="296" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="297" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -4729,19 +4729,19 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23" customHeight="1">
+    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="39" t="s">
         <v>49</v>
@@ -4752,7 +4752,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -4786,7 +4786,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="5" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="19" t="s">
         <v>10</v>
@@ -4814,7 +4814,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="6" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="19" t="s">
         <v>11</v>
@@ -4827,7 +4827,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="7" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
@@ -4840,7 +4840,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="8" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
         <v>216</v>
@@ -4868,7 +4868,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="10" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
         <v>217</v>
@@ -4882,7 +4882,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>35</v>
@@ -4893,7 +4893,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="19" customFormat="1" ht="47.25">
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>43</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.5">
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>173</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.5">
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="C15" s="19" t="s">
         <v>66</v>
@@ -4936,7 +4936,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="19" customFormat="1">
+    <row r="16" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C16" s="20" t="s">
         <v>184</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="20" customFormat="1" ht="34" customHeight="1">
+    <row r="17" spans="1:7" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>34</v>
       </c>
@@ -4963,234 +4963,234 @@
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" s="19" customFormat="1">
+    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="1:7" s="19" customFormat="1"/>
-    <row r="20" spans="1:7" s="19" customFormat="1"/>
-    <row r="21" spans="1:7" s="19" customFormat="1"/>
-    <row r="22" spans="1:7" s="19" customFormat="1"/>
-    <row r="23" spans="1:7">
+    <row r="19" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="19"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="19"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="19"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="19"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="19"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="19"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="19"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="19"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="19"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="19"/>
     </row>
   </sheetData>
@@ -5215,19 +5215,19 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23" customHeight="1">
+    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="39" t="s">
         <v>258</v>
@@ -5238,7 +5238,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -5272,7 +5272,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="4" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="5" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="20" t="s">
         <v>10</v>
@@ -5300,7 +5300,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="6" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="20" t="s">
         <v>11</v>
@@ -5313,7 +5313,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="7" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="20" t="s">
         <v>12</v>
@@ -5326,7 +5326,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="8" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -5340,7 +5340,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="9" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
         <v>216</v>
@@ -5354,7 +5354,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="20" customFormat="1" ht="47.25">
+    <row r="10" spans="1:7" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
         <v>217</v>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
         <v>35</v>
@@ -5379,7 +5379,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="22" customFormat="1" ht="31.5">
+    <row r="13" spans="1:7" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>173</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="31.5">
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="C14" s="20" t="s">
         <v>66</v>
@@ -5408,7 +5408,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="20" customFormat="1" ht="34" customHeight="1">
+    <row r="15" spans="1:7" s="20" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>34</v>
       </c>
@@ -5427,229 +5427,229 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" s="20" customFormat="1"/>
-    <row r="17" spans="1:1" s="20" customFormat="1"/>
-    <row r="18" spans="1:1" s="20" customFormat="1"/>
-    <row r="19" spans="1:1" s="20" customFormat="1"/>
-    <row r="20" spans="1:1" s="20" customFormat="1"/>
-    <row r="21" spans="1:1">
+    <row r="16" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="20"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="20"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="20"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="20"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="20"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="20"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="20"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="20"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="20"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="20"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="20"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="20"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="20"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="20"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="20"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="20"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="20"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="20"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="20"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="20"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="20"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="20"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="20"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="20"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="20"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="20"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="20"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="20"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="20"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="20"/>
     </row>
   </sheetData>
@@ -5670,21 +5670,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="55.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
+    <col min="6" max="6" width="55.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="37.5" customHeight="1">
+    <row r="1" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30"/>
       <c r="B1" s="40" t="s">
         <v>269</v>
@@ -5694,7 +5694,7 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
     </row>
-    <row r="2" spans="1:6" ht="37.5" customHeight="1">
+    <row r="2" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>111</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="37.5" customHeight="1">
+    <row r="3" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="B3" s="32" t="s">
         <v>62</v>
@@ -5724,7 +5724,7 @@
       <c r="E3" s="33"/>
       <c r="F3" s="33"/>
     </row>
-    <row r="4" spans="1:6" ht="37.5" customHeight="1">
+    <row r="4" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
       <c r="B4" s="26"/>
       <c r="C4" s="28" t="s">
@@ -5738,7 +5738,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="37.5" customHeight="1">
+    <row r="5" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
       <c r="B5" s="26"/>
       <c r="C5" s="28" t="s">
@@ -5754,7 +5754,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="37.5" customHeight="1">
+    <row r="6" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
         <v>34</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="37.5" customHeight="1">
+    <row r="7" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>34</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="37.5" customHeight="1">
+    <row r="8" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
         <v>34</v>
       </c>
@@ -5808,7 +5808,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="37.5" customHeight="1">
+    <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>34</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="37.5" customHeight="1">
+    <row r="10" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
         <v>34</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="37.5" customHeight="1">
+    <row r="11" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="32" t="s">
         <v>15</v>
@@ -5854,7 +5854,7 @@
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
     </row>
-    <row r="12" spans="1:6" ht="37.5" customHeight="1">
+    <row r="12" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="27" t="s">
         <v>13</v>
@@ -5870,7 +5870,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="37.5" customHeight="1">
+    <row r="13" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="27"/>
       <c r="C13" s="37" t="s">
@@ -5884,7 +5884,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="37.5" customHeight="1">
+    <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="27"/>
       <c r="C14" s="37" t="s">
@@ -5898,7 +5898,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="37.5" customHeight="1">
+    <row r="15" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="27"/>
       <c r="C15" s="37" t="s">
@@ -5912,7 +5912,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="37.5" customHeight="1">
+    <row r="16" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="27"/>
       <c r="C16" s="37" t="s">
@@ -5926,7 +5926,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="37.5" customHeight="1">
+    <row r="17" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="27" t="s">
         <v>5</v>
@@ -5942,7 +5942,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="37.5" customHeight="1">
+    <row r="18" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="27"/>
       <c r="C18" s="37" t="s">
@@ -5956,7 +5956,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="37.5" customHeight="1">
+    <row r="19" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>34</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="37.5" customHeight="1">
+    <row r="20" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="28"/>
       <c r="C20" s="28" t="s">
@@ -5988,7 +5988,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="37.5" customHeight="1">
+    <row r="21" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="28"/>
       <c r="C21" s="28" t="s">
@@ -6002,7 +6002,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="37.5" customHeight="1">
+    <row r="22" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="28"/>
       <c r="C22" s="28" t="s">
@@ -6016,7 +6016,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="37.5" customHeight="1">
+    <row r="23" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="28"/>
       <c r="C23" s="28" t="s">
@@ -6030,7 +6030,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="37.5" customHeight="1">
+    <row r="24" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="28"/>
       <c r="C24" s="28" t="s">
@@ -6044,7 +6044,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="37.5" customHeight="1">
+    <row r="25" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="28"/>
       <c r="C25" s="28" t="s">
@@ -6058,7 +6058,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="37.5" customHeight="1">
+    <row r="26" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="28"/>
       <c r="C26" s="28" t="s">
@@ -6072,7 +6072,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="37.5" customHeight="1">
+    <row r="27" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="28"/>
       <c r="C27" s="28" t="s">
@@ -6086,7 +6086,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="37.5" customHeight="1">
+    <row r="28" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="28"/>
       <c r="C28" s="28" t="s">
@@ -6100,7 +6100,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="37.5" customHeight="1">
+    <row r="29" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="28"/>
       <c r="C29" s="28" t="s">
@@ -6114,7 +6114,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="37.5" customHeight="1">
+    <row r="30" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="28"/>
       <c r="C30" s="28" t="s">
@@ -6128,7 +6128,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="37.5" customHeight="1">
+    <row r="31" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
       <c r="B31" s="28"/>
       <c r="C31" s="28" t="s">
@@ -6142,7 +6142,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="37.5" customHeight="1">
+    <row r="32" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="28"/>
       <c r="C32" s="28" t="s">
@@ -6156,7 +6156,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="37.5" customHeight="1">
+    <row r="33" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26"/>
       <c r="B33" s="28"/>
       <c r="C33" s="28" t="s">
@@ -6170,7 +6170,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="37.5" customHeight="1">
+    <row r="34" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
       <c r="B34" s="28"/>
       <c r="C34" s="28" t="s">
@@ -6184,7 +6184,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="37.5" customHeight="1">
+    <row r="35" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="26"/>
       <c r="B35" s="28"/>
       <c r="C35" s="28" t="s">
@@ -6198,7 +6198,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="37.5" customHeight="1">
+    <row r="36" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
       <c r="B36" s="28"/>
       <c r="C36" s="28" t="s">
@@ -6212,7 +6212,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="37.5" customHeight="1">
+    <row r="37" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="s">
         <v>34</v>
       </c>
@@ -6230,7 +6230,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="37.5" customHeight="1">
+    <row r="38" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="37" t="s">
         <v>34</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="37.5" customHeight="1">
+    <row r="39" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26"/>
       <c r="B39" s="27" t="s">
         <v>17</v>
@@ -6264,7 +6264,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="37.5" customHeight="1">
+    <row r="40" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26"/>
       <c r="B40" s="27"/>
       <c r="C40" s="27" t="s">
@@ -6280,7 +6280,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="37.5" customHeight="1">
+    <row r="41" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
       <c r="B41" s="32" t="s">
         <v>26</v>
@@ -6290,7 +6290,7 @@
       <c r="E41" s="33"/>
       <c r="F41" s="33"/>
     </row>
-    <row r="42" spans="1:6" ht="37.5" customHeight="1">
+    <row r="42" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
       <c r="B42" s="26"/>
       <c r="C42" s="28" t="s">
@@ -6304,7 +6304,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="37.5" customHeight="1">
+    <row r="43" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="26"/>
       <c r="B43" s="26"/>
       <c r="C43" s="28" t="s">
@@ -6318,7 +6318,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="37.5" customHeight="1">
+    <row r="44" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="26"/>
       <c r="B44" s="26"/>
       <c r="C44" s="28" t="s">
@@ -6332,7 +6332,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="37.5" customHeight="1">
+    <row r="45" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="26"/>
       <c r="B45" s="26"/>
       <c r="C45" s="28" t="s">
@@ -6348,7 +6348,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="37.5" customHeight="1">
+    <row r="46" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="26"/>
       <c r="B46" s="26"/>
       <c r="C46" s="28" t="s">
@@ -6362,7 +6362,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="37.5" customHeight="1">
+    <row r="47" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="26"/>
       <c r="B47" s="26"/>
       <c r="C47" s="28" t="s">
@@ -6376,7 +6376,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="37.5" customHeight="1">
+    <row r="48" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="26"/>
       <c r="B48" s="26"/>
       <c r="C48" s="28" t="s">
@@ -6390,7 +6390,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="37.5" customHeight="1">
+    <row r="49" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="26"/>
       <c r="B49" s="26"/>
       <c r="C49" s="28" t="s">
@@ -6404,7 +6404,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="37.5" customHeight="1">
+    <row r="50" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="26"/>
       <c r="B50" s="26"/>
       <c r="C50" s="28" t="s">
@@ -6420,7 +6420,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="37.5" customHeight="1">
+    <row r="51" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="26"/>
       <c r="B51" s="26"/>
       <c r="C51" s="28" t="s">
@@ -6436,7 +6436,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="37.5" customHeight="1">
+    <row r="52" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="26"/>
       <c r="B52" s="26"/>
       <c r="C52" s="28" t="s">
@@ -6452,7 +6452,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="37.5" customHeight="1">
+    <row r="53" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="26"/>
       <c r="B53" s="26"/>
       <c r="C53" s="28" t="s">
@@ -6466,7 +6466,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="50.25" customHeight="1">
+    <row r="54" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26"/>
       <c r="B54" s="32" t="s">
         <v>46</v>
@@ -6476,7 +6476,7 @@
       <c r="E54" s="33"/>
       <c r="F54" s="33"/>
     </row>
-    <row r="55" spans="1:6" ht="37.5" customHeight="1">
+    <row r="55" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
         <v>34</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="37.5" customHeight="1">
+    <row r="56" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="29"/>
       <c r="B56" s="34"/>
       <c r="C56" s="28" t="s">
@@ -6506,7 +6506,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="37.5" customHeight="1">
+    <row r="57" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="26"/>
       <c r="B57" s="26"/>
       <c r="C57" s="28" t="s">
@@ -6520,7 +6520,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="37.5" customHeight="1">
+    <row r="58" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="26"/>
       <c r="B58" s="26"/>
       <c r="C58" s="28" t="s">
@@ -6534,7 +6534,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="37.5" customHeight="1">
+    <row r="59" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="26"/>
       <c r="B59" s="26"/>
       <c r="C59" s="37" t="s">
@@ -6548,7 +6548,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="37.5" customHeight="1">
+    <row r="60" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="26"/>
       <c r="B60" s="32" t="s">
         <v>35</v>
@@ -6558,7 +6558,7 @@
       <c r="E60" s="33"/>
       <c r="F60" s="33"/>
     </row>
-    <row r="61" spans="1:6" ht="37.5" customHeight="1">
+    <row r="61" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="26"/>
       <c r="B61" s="26"/>
       <c r="C61" s="28" t="s">
@@ -6574,7 +6574,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="37.5" customHeight="1">
+    <row r="62" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="26"/>
       <c r="B62" s="26"/>
       <c r="C62" s="28" t="s">
@@ -6588,7 +6588,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="37.5" customHeight="1">
+    <row r="63" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="26"/>
       <c r="B63" s="26"/>
       <c r="C63" s="28" t="s">
@@ -6602,7 +6602,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="37.5" customHeight="1">
+    <row r="64" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="26"/>
       <c r="B64" s="26"/>
       <c r="C64" s="28" t="s">
@@ -6616,7 +6616,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="37.5" customHeight="1">
+    <row r="65" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="26"/>
       <c r="B65" s="26"/>
       <c r="C65" s="28" t="s">
@@ -6630,7 +6630,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="37.5" customHeight="1">
+    <row r="66" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="37" t="s">
         <v>34</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="37.5" customHeight="1">
+    <row r="67" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37" t="s">
         <v>34</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="37.5" customHeight="1">
+    <row r="68" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="26"/>
       <c r="B68" s="26"/>
       <c r="C68" s="27" t="s">
@@ -6682,7 +6682,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="37.5" customHeight="1">
+    <row r="69" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="37" t="s">
         <v>34</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="37.5" customHeight="1">
+    <row r="70" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="26"/>
       <c r="B70" s="26"/>
       <c r="C70" s="37" t="s">
@@ -6716,7 +6716,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="37.5" customHeight="1">
+    <row r="71" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="37" t="s">
         <v>34</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="37.5" customHeight="1">
+    <row r="72" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="37" t="s">
         <v>34</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="37.5" customHeight="1">
+    <row r="73" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="37" t="s">
         <v>34</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="37.5" customHeight="1">
+    <row r="74" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="37" t="s">
         <v>34</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="37.5" customHeight="1">
+    <row r="75" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="37" t="s">
         <v>34</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="37.5" customHeight="1">
+    <row r="76" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="37" t="s">
         <v>34</v>
       </c>
@@ -6845,7 +6845,7 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>